<commit_message>
use more or less same test data as other 1508 fixtures
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
+++ b/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDCCF5F-4FB7-9648-A0CF-B6414BC50A6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B77A01-7DA5-7545-8B81-CEA16084D8D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2900" yWindow="2760" windowWidth="46600" windowHeight="25180" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="511">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1774,15 +1774,6 @@
   </si>
   <si>
     <t>Sampling time-point</t>
-  </si>
-  <si>
-    <t>child</t>
-  </si>
-  <si>
-    <t>father</t>
-  </si>
-  <si>
-    <t>mother</t>
   </si>
   <si>
     <t>MIP RNA</t>
@@ -4688,7 +4679,7 @@
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="15" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" spans="1:1">
@@ -4821,18 +4812,18 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1">
       <c r="A45" s="19" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13" customHeight="1"/>
     <row r="47" spans="1:5" ht="42" customHeight="1">
       <c r="A47" s="34" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="42" customHeight="1">
       <c r="A48" s="34" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="18" customHeight="1">
@@ -4972,7 +4963,7 @@
   <dimension ref="A1:AH428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18:V52"/>
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5639,19 +5630,19 @@
     </row>
     <row r="15" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="198" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B15" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D15" s="201" t="s">
         <v>283</v>
       </c>
       <c r="E15" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F15" s="200" t="s">
         <v>15</v>
@@ -5673,7 +5664,7 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
@@ -5686,25 +5677,25 @@
         <v>298</v>
       </c>
       <c r="R15" s="198" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="S15" s="206" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="T15" s="150"/>
-      <c r="U15" s="61" t="s">
-        <v>429</v>
+      <c r="U15" s="198" t="s">
+        <v>437</v>
       </c>
       <c r="V15" s="61">
         <v>1</v>
       </c>
       <c r="W15" s="150"/>
       <c r="X15" s="31" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="Y15" s="180"/>
       <c r="Z15" s="210" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="AA15" s="211">
         <v>5</v>
@@ -5721,27 +5712,27 @@
       </c>
       <c r="AF15" s="152"/>
       <c r="AG15" s="58" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="AH15" s="58" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="16" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="198" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B16" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D16" s="201" t="s">
         <v>288</v>
       </c>
       <c r="E16" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F16" s="200" t="s">
         <v>16</v>
@@ -5774,15 +5765,15 @@
       <c r="R16" s="207"/>
       <c r="S16" s="208"/>
       <c r="T16" s="150"/>
-      <c r="U16" s="61" t="s">
-        <v>430</v>
+      <c r="U16" s="198" t="s">
+        <v>439</v>
       </c>
       <c r="V16" s="61">
         <v>1</v>
       </c>
       <c r="W16" s="150"/>
       <c r="X16" s="209" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="Y16" s="180"/>
       <c r="Z16" s="212"/>
@@ -5801,19 +5792,19 @@
     </row>
     <row r="17" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="198" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B17" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D17" s="201" t="s">
         <v>284</v>
       </c>
       <c r="E17" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F17" s="200" t="s">
         <v>15</v>
@@ -5846,15 +5837,15 @@
       <c r="R17" s="207"/>
       <c r="S17" s="208"/>
       <c r="T17" s="150"/>
-      <c r="U17" s="61" t="s">
-        <v>431</v>
+      <c r="U17" s="206" t="s">
+        <v>440</v>
       </c>
       <c r="V17" s="61">
         <v>1</v>
       </c>
       <c r="W17" s="150"/>
       <c r="X17" s="31" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="Y17" s="180"/>
       <c r="Z17" s="212"/>
@@ -5871,19 +5862,19 @@
     </row>
     <row r="18" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="198" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B18" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D18" s="201" t="s">
         <v>285</v>
       </c>
       <c r="E18" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F18" s="200" t="s">
         <v>77</v>
@@ -5925,7 +5916,7 @@
       </c>
       <c r="W18" s="150"/>
       <c r="X18" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y18" s="180"/>
       <c r="Z18" s="212"/>
@@ -5942,19 +5933,19 @@
     </row>
     <row r="19" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="198" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B19" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D19" s="201" t="s">
         <v>286</v>
       </c>
       <c r="E19" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F19" s="200" t="s">
         <v>77</v>
@@ -5996,7 +5987,7 @@
       </c>
       <c r="W19" s="150"/>
       <c r="X19" s="31" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="Y19" s="180"/>
       <c r="Z19" s="212"/>
@@ -6010,24 +6001,24 @@
       <c r="AF19" s="152"/>
       <c r="AG19" s="58"/>
       <c r="AH19" s="58" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="198" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B20" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D20" s="201" t="s">
         <v>287</v>
       </c>
       <c r="E20" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F20" s="200" t="s">
         <v>77</v>
@@ -6069,7 +6060,7 @@
       </c>
       <c r="W20" s="150"/>
       <c r="X20" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y20" s="180"/>
       <c r="Z20" s="212"/>
@@ -6086,19 +6077,19 @@
     </row>
     <row r="21" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="198" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B21" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D21" s="201" t="s">
         <v>376</v>
       </c>
       <c r="E21" s="198" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="F21" s="200" t="s">
         <v>77</v>
@@ -6140,7 +6131,7 @@
       </c>
       <c r="W21" s="150"/>
       <c r="X21" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y21" s="180"/>
       <c r="Z21" s="212"/>
@@ -6157,19 +6148,19 @@
     </row>
     <row r="22" spans="1:34" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="198" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B22" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D22" s="201" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="E22" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F22" s="200" t="s">
         <v>77</v>
@@ -6211,7 +6202,7 @@
       </c>
       <c r="W22" s="150"/>
       <c r="X22" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y22" s="180"/>
       <c r="Z22" s="173" t="s">
@@ -6229,19 +6220,19 @@
     </row>
     <row r="23" spans="1:34" ht="25" customHeight="1">
       <c r="A23" s="198" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B23" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D23" s="201" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E23" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F23" s="200" t="s">
         <v>77</v>
@@ -6283,7 +6274,7 @@
       </c>
       <c r="W23" s="150"/>
       <c r="X23" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y23" s="180"/>
       <c r="Z23" s="173" t="s">
@@ -6302,19 +6293,19 @@
     </row>
     <row r="24" spans="1:34" ht="25" customHeight="1">
       <c r="A24" s="198" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B24" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D24" s="201" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E24" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F24" s="200" t="s">
         <v>77</v>
@@ -6356,7 +6347,7 @@
       </c>
       <c r="W24" s="150"/>
       <c r="X24" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y24" s="180"/>
       <c r="Z24" s="196" t="s">
@@ -6375,19 +6366,19 @@
     </row>
     <row r="25" spans="1:34" ht="25" customHeight="1">
       <c r="A25" s="198" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B25" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D25" s="201" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E25" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F25" s="200" t="s">
         <v>77</v>
@@ -6429,7 +6420,7 @@
       </c>
       <c r="W25" s="150"/>
       <c r="X25" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y25" s="180"/>
       <c r="Z25" s="173" t="s">
@@ -6445,24 +6436,24 @@
       <c r="AF25" s="152"/>
       <c r="AG25" s="58"/>
       <c r="AH25" s="58" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="25" customHeight="1">
       <c r="A26" s="198" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B26" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D26" s="201" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="E26" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F26" s="200" t="s">
         <v>77</v>
@@ -6504,7 +6495,7 @@
       </c>
       <c r="W26" s="150"/>
       <c r="X26" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y26" s="180"/>
       <c r="Z26" s="173" t="s">
@@ -6523,19 +6514,19 @@
     </row>
     <row r="27" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="198" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B27" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D27" s="201" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E27" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F27" s="200" t="s">
         <v>77</v>
@@ -6577,7 +6568,7 @@
       </c>
       <c r="W27" s="150"/>
       <c r="X27" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y27" s="180"/>
       <c r="Z27" s="173" t="s">
@@ -6596,19 +6587,19 @@
     </row>
     <row r="28" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="198" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B28" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D28" s="201" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="E28" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F28" s="200" t="s">
         <v>77</v>
@@ -6650,7 +6641,7 @@
       </c>
       <c r="W28" s="150"/>
       <c r="X28" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y28" s="180"/>
       <c r="Z28" s="173" t="s">
@@ -6669,19 +6660,19 @@
     </row>
     <row r="29" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="198" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B29" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D29" s="201" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E29" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F29" s="200" t="s">
         <v>77</v>
@@ -6723,7 +6714,7 @@
       </c>
       <c r="W29" s="150"/>
       <c r="X29" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y29" s="180"/>
       <c r="Z29" s="173" t="s">
@@ -6742,19 +6733,19 @@
     </row>
     <row r="30" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="198" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B30" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D30" s="201" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="E30" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F30" s="200" t="s">
         <v>77</v>
@@ -6796,7 +6787,7 @@
       </c>
       <c r="W30" s="150"/>
       <c r="X30" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y30" s="180"/>
       <c r="Z30" s="173" t="s">
@@ -6815,19 +6806,19 @@
     </row>
     <row r="31" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="198" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B31" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D31" s="201" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E31" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F31" s="200" t="s">
         <v>77</v>
@@ -6869,7 +6860,7 @@
       </c>
       <c r="W31" s="150"/>
       <c r="X31" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y31" s="180"/>
       <c r="Z31" s="173" t="s">
@@ -6888,19 +6879,19 @@
     </row>
     <row r="32" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="198" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="B32" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D32" s="201" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="E32" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F32" s="200" t="s">
         <v>77</v>
@@ -6942,7 +6933,7 @@
       </c>
       <c r="W32" s="150"/>
       <c r="X32" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y32" s="180"/>
       <c r="Z32" s="173" t="s">
@@ -6961,19 +6952,19 @@
     </row>
     <row r="33" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="198" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="B33" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D33" s="201" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="E33" s="198" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="F33" s="200" t="s">
         <v>77</v>
@@ -7015,7 +7006,7 @@
       </c>
       <c r="W33" s="150"/>
       <c r="X33" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y33" s="180"/>
       <c r="Z33" s="173" t="s">
@@ -7034,19 +7025,19 @@
     </row>
     <row r="34" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="198" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B34" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D34" s="201" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E34" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F34" s="200" t="s">
         <v>77</v>
@@ -7088,7 +7079,7 @@
       </c>
       <c r="W34" s="150"/>
       <c r="X34" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y34" s="180"/>
       <c r="Z34" s="173" t="s">
@@ -7107,19 +7098,19 @@
     </row>
     <row r="35" spans="1:34" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="198" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B35" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D35" s="201" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E35" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F35" s="200" t="s">
         <v>77</v>
@@ -7161,7 +7152,7 @@
       </c>
       <c r="W35" s="150"/>
       <c r="X35" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y35" s="180"/>
       <c r="Z35" s="173" t="s">
@@ -7180,19 +7171,19 @@
     </row>
     <row r="36" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="198" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B36" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D36" s="201" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E36" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F36" s="200" t="s">
         <v>77</v>
@@ -7234,7 +7225,7 @@
       </c>
       <c r="W36" s="150"/>
       <c r="X36" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y36" s="180"/>
       <c r="Z36" s="173" t="s">
@@ -7253,19 +7244,19 @@
     </row>
     <row r="37" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="198" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B37" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D37" s="201" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E37" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F37" s="200" t="s">
         <v>77</v>
@@ -7307,7 +7298,7 @@
       </c>
       <c r="W37" s="150"/>
       <c r="X37" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y37" s="180"/>
       <c r="Z37" s="173" t="s">
@@ -7326,19 +7317,19 @@
     </row>
     <row r="38" spans="1:34" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="198" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B38" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D38" s="201" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E38" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F38" s="200" t="s">
         <v>77</v>
@@ -7380,7 +7371,7 @@
       </c>
       <c r="W38" s="150"/>
       <c r="X38" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y38" s="180"/>
       <c r="Z38" s="173" t="s">
@@ -7399,19 +7390,19 @@
     </row>
     <row r="39" spans="1:34" ht="25" customHeight="1">
       <c r="A39" s="198" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B39" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D39" s="201" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E39" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F39" s="200" t="s">
         <v>77</v>
@@ -7453,7 +7444,7 @@
       </c>
       <c r="W39" s="150"/>
       <c r="X39" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y39" s="180"/>
       <c r="Z39" s="173" t="s">
@@ -7472,19 +7463,19 @@
     </row>
     <row r="40" spans="1:34" ht="25" customHeight="1">
       <c r="A40" s="198" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B40" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D40" s="201" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E40" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F40" s="200" t="s">
         <v>77</v>
@@ -7526,7 +7517,7 @@
       </c>
       <c r="W40" s="150"/>
       <c r="X40" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y40" s="180"/>
       <c r="Z40" s="173" t="s">
@@ -7545,19 +7536,19 @@
     </row>
     <row r="41" spans="1:34" ht="25" customHeight="1">
       <c r="A41" s="198" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B41" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D41" s="201" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E41" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F41" s="200" t="s">
         <v>77</v>
@@ -7599,7 +7590,7 @@
       </c>
       <c r="W41" s="150"/>
       <c r="X41" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y41" s="180"/>
       <c r="Z41" s="173" t="s">
@@ -7618,19 +7609,19 @@
     </row>
     <row r="42" spans="1:34" ht="25" customHeight="1">
       <c r="A42" s="198" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B42" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D42" s="201" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E42" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F42" s="200" t="s">
         <v>77</v>
@@ -7672,7 +7663,7 @@
       </c>
       <c r="W42" s="150"/>
       <c r="X42" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y42" s="180"/>
       <c r="Z42" s="173" t="s">
@@ -7691,19 +7682,19 @@
     </row>
     <row r="43" spans="1:34" ht="25" customHeight="1">
       <c r="A43" s="198" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B43" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D43" s="201" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="E43" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F43" s="200" t="s">
         <v>77</v>
@@ -7745,7 +7736,7 @@
       </c>
       <c r="W43" s="150"/>
       <c r="X43" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y43" s="180"/>
       <c r="Z43" s="173" t="s">
@@ -7764,19 +7755,19 @@
     </row>
     <row r="44" spans="1:34" ht="25" customHeight="1">
       <c r="A44" s="198" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B44" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D44" s="201" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E44" s="198" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F44" s="200" t="s">
         <v>77</v>
@@ -7818,7 +7809,7 @@
       </c>
       <c r="W44" s="150"/>
       <c r="X44" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y44" s="180"/>
       <c r="Z44" s="173" t="s">
@@ -7837,19 +7828,19 @@
     </row>
     <row r="45" spans="1:34" ht="25" customHeight="1">
       <c r="A45" s="198" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B45" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D45" s="201" t="s">
         <v>381</v>
       </c>
       <c r="E45" s="198" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F45" s="200" t="s">
         <v>77</v>
@@ -7891,7 +7882,7 @@
       </c>
       <c r="W45" s="150"/>
       <c r="X45" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y45" s="180"/>
       <c r="Z45" s="212"/>
@@ -7908,19 +7899,19 @@
     </row>
     <row r="46" spans="1:34" ht="25" customHeight="1">
       <c r="A46" s="198" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B46" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C46" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D46" s="201" t="s">
         <v>382</v>
       </c>
       <c r="E46" s="198" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F46" s="200" t="s">
         <v>77</v>
@@ -7962,7 +7953,7 @@
       </c>
       <c r="W46" s="150"/>
       <c r="X46" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y46" s="180"/>
       <c r="Z46" s="212"/>
@@ -7979,19 +7970,19 @@
     </row>
     <row r="47" spans="1:34" ht="25" customHeight="1">
       <c r="A47" s="198" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B47" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C47" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D47" s="201" t="s">
         <v>383</v>
       </c>
       <c r="E47" s="198" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F47" s="200" t="s">
         <v>77</v>
@@ -8033,7 +8024,7 @@
       </c>
       <c r="W47" s="150"/>
       <c r="X47" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y47" s="180"/>
       <c r="Z47" s="212"/>
@@ -8050,19 +8041,19 @@
     </row>
     <row r="48" spans="1:34" ht="25" customHeight="1">
       <c r="A48" s="198" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B48" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C48" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D48" s="201" t="s">
         <v>384</v>
       </c>
       <c r="E48" s="198" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F48" s="200" t="s">
         <v>77</v>
@@ -8104,7 +8095,7 @@
       </c>
       <c r="W48" s="150"/>
       <c r="X48" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y48" s="180"/>
       <c r="Z48" s="212"/>
@@ -8121,19 +8112,19 @@
     </row>
     <row r="49" spans="1:34" ht="25" customHeight="1">
       <c r="A49" s="198" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B49" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C49" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D49" s="201" t="s">
         <v>385</v>
       </c>
       <c r="E49" s="198" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F49" s="200" t="s">
         <v>77</v>
@@ -8175,7 +8166,7 @@
       </c>
       <c r="W49" s="150"/>
       <c r="X49" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y49" s="180"/>
       <c r="Z49" s="212"/>
@@ -8192,19 +8183,19 @@
     </row>
     <row r="50" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="205" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B50" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C50" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D50" s="201" t="s">
         <v>283</v>
       </c>
       <c r="E50" s="198" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F50" s="200" t="s">
         <v>77</v>
@@ -8246,7 +8237,7 @@
       </c>
       <c r="W50" s="150"/>
       <c r="X50" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y50" s="180"/>
       <c r="Z50" s="212"/>
@@ -8263,19 +8254,19 @@
     </row>
     <row r="51" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="205" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B51" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C51" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D51" s="201" t="s">
         <v>283</v>
       </c>
       <c r="E51" s="198" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F51" s="200" t="s">
         <v>77</v>
@@ -8317,7 +8308,7 @@
       </c>
       <c r="W51" s="150"/>
       <c r="X51" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y51" s="180"/>
       <c r="Z51" s="212"/>
@@ -8334,19 +8325,19 @@
     </row>
     <row r="52" spans="1:34" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="205" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B52" s="199" t="s">
         <v>37</v>
       </c>
       <c r="C52" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D52" s="201" t="s">
         <v>283</v>
       </c>
       <c r="E52" s="198" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F52" s="200" t="s">
         <v>77</v>
@@ -8388,7 +8379,7 @@
       </c>
       <c r="W52" s="150"/>
       <c r="X52" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="Y52" s="180"/>
       <c r="Z52" s="212"/>
@@ -21378,7 +21369,7 @@
     <row r="7" spans="1:38">
       <c r="A7" s="31"/>
       <c r="B7" s="37" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>285</v>

</xml_diff>

<commit_message>
use only wts applications in rna test
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
+++ b/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AA3D19-29D8-D249-A98C-0B0B8D983E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53F77D1-DC95-644E-A119-519075B3DD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="23860" windowHeight="25900" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13000" yWindow="460" windowWidth="35700" windowHeight="25000" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="488">
   <si>
     <t>Document name</t>
   </si>
@@ -1920,19 +1920,7 @@
     <t>Emilia Ottosson Laakso</t>
   </si>
   <si>
-    <t>whole-genome-1</t>
-  </si>
-  <si>
-    <t>whole-genome</t>
-  </si>
-  <si>
     <t>plate</t>
-  </si>
-  <si>
-    <t>whole-genome-2</t>
-  </si>
-  <si>
-    <t>whole-genome-3</t>
   </si>
   <si>
     <t>LymphoMATIC</t>
@@ -1953,13 +1941,7 @@
     <t>GMCKsolid</t>
   </si>
   <si>
-    <t>whole-genome-4</t>
-  </si>
-  <si>
     <t>GMSmyeloid</t>
-  </si>
-  <si>
-    <t>whole-genome-5</t>
   </si>
   <si>
     <t>other (specify in comment field)</t>
@@ -1968,157 +1950,7 @@
     <t>Other bait set</t>
   </si>
   <si>
-    <t>whole-genome-6</t>
-  </si>
-  <si>
-    <t>whole-genome-7</t>
-  </si>
-  <si>
-    <t>whole-exome-1</t>
-  </si>
-  <si>
-    <t>EXOTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome</t>
-  </si>
-  <si>
-    <t>whole-exome-2</t>
-  </si>
-  <si>
-    <t>EXOTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-3</t>
-  </si>
-  <si>
-    <t>EXOTTTR060</t>
-  </si>
-  <si>
-    <t>whole-exome-4</t>
-  </si>
-  <si>
-    <t>EXOTTTR080</t>
-  </si>
-  <si>
     <t>Other Elution buffer</t>
-  </si>
-  <si>
-    <t>whole-exome-5</t>
-  </si>
-  <si>
-    <t>EXOTTTR100</t>
-  </si>
-  <si>
-    <t>whole-exome-6</t>
-  </si>
-  <si>
-    <t>EXOTTTR120</t>
-  </si>
-  <si>
-    <t>whole-exome-7</t>
-  </si>
-  <si>
-    <t>EXOTTTR140</t>
-  </si>
-  <si>
-    <t>whole-exome-8</t>
-  </si>
-  <si>
-    <t>EXTTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome-9</t>
-  </si>
-  <si>
-    <t>EXTTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-10</t>
-  </si>
-  <si>
-    <t>EXLTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome-11</t>
-  </si>
-  <si>
-    <t>EXLTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-12</t>
-  </si>
-  <si>
-    <t>EXLTTTR060</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-1</t>
-  </si>
-  <si>
-    <t>EXLTTTR080</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-2</t>
-  </si>
-  <si>
-    <t>PANTTTR010</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-3</t>
-  </si>
-  <si>
-    <t>PANTTTR020</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-4</t>
-  </si>
-  <si>
-    <t>PANTTTR030</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-5</t>
-  </si>
-  <si>
-    <t>PANTTTR040</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-6</t>
-  </si>
-  <si>
-    <t>PANTTTR050</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-7</t>
-  </si>
-  <si>
-    <t>PALTTTR010</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-8</t>
-  </si>
-  <si>
-    <t>PALTTTR020</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-9</t>
-  </si>
-  <si>
-    <t>PALTTTR030</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-10</t>
-  </si>
-  <si>
-    <t>PALTTTR040</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-11</t>
-  </si>
-  <si>
-    <t>PALTTTR050</t>
   </si>
   <si>
     <t>rna-1</t>
@@ -2139,16 +1971,103 @@
     <t>rna-5</t>
   </si>
   <si>
-    <t>gene-list-test-1</t>
+    <t>rna-6</t>
   </si>
   <si>
-    <t>gene-list-test</t>
+    <t>rna-7</t>
   </si>
   <si>
-    <t>gene-list-test-2</t>
+    <t>rna-8</t>
   </si>
   <si>
-    <t>gene-list-test-3</t>
+    <t>rna-9</t>
+  </si>
+  <si>
+    <t>rna-10</t>
+  </si>
+  <si>
+    <t>rna-11</t>
+  </si>
+  <si>
+    <t>rna-12</t>
+  </si>
+  <si>
+    <t>rna-13</t>
+  </si>
+  <si>
+    <t>rna-14</t>
+  </si>
+  <si>
+    <t>rna-15</t>
+  </si>
+  <si>
+    <t>rna-16</t>
+  </si>
+  <si>
+    <t>rna-17</t>
+  </si>
+  <si>
+    <t>rna-18</t>
+  </si>
+  <si>
+    <t>rna-19</t>
+  </si>
+  <si>
+    <t>rna-20</t>
+  </si>
+  <si>
+    <t>rna-21</t>
+  </si>
+  <si>
+    <t>rna-22</t>
+  </si>
+  <si>
+    <t>rna-23</t>
+  </si>
+  <si>
+    <t>rna-24</t>
+  </si>
+  <si>
+    <t>rna-25</t>
+  </si>
+  <si>
+    <t>rna-26</t>
+  </si>
+  <si>
+    <t>rna-27</t>
+  </si>
+  <si>
+    <t>rna-28</t>
+  </si>
+  <si>
+    <t>rna-29</t>
+  </si>
+  <si>
+    <t>rna-30</t>
+  </si>
+  <si>
+    <t>rna-31</t>
+  </si>
+  <si>
+    <t>rna-32</t>
+  </si>
+  <si>
+    <t>rna-33</t>
+  </si>
+  <si>
+    <t>rna-34</t>
+  </si>
+  <si>
+    <t>rna-35</t>
+  </si>
+  <si>
+    <t>rna-36</t>
+  </si>
+  <si>
+    <t>rna-37</t>
+  </si>
+  <si>
+    <t>rna-38</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2078,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2478,6 +2397,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -2794,7 +2719,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3252,27 +3177,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3326,10 +3230,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="36" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3341,6 +3241,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -4226,8 +4147,8 @@
   </sheetPr>
   <dimension ref="A1:AMK395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:AH52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15:U52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -10499,56 +10420,56 @@
       <c r="AH8" s="42"/>
     </row>
     <row r="9" spans="1:1024" s="48" customFormat="1" ht="22" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="167" t="s">
+      <c r="A9" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="167"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="167"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="167"/>
-      <c r="G9" s="167"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="167"/>
-      <c r="K9" s="167"/>
+      <c r="B9" s="186"/>
+      <c r="C9" s="186"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="186"/>
+      <c r="F9" s="186"/>
+      <c r="G9" s="186"/>
+      <c r="H9" s="186"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="186"/>
       <c r="L9" s="44"/>
-      <c r="M9" s="168" t="s">
+      <c r="M9" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="168"/>
+      <c r="N9" s="187"/>
       <c r="O9" s="159"/>
-      <c r="P9" s="169" t="s">
+      <c r="P9" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="169"/>
-      <c r="R9" s="169"/>
-      <c r="S9" s="169"/>
+      <c r="Q9" s="188"/>
+      <c r="R9" s="188"/>
+      <c r="S9" s="188"/>
       <c r="T9" s="45"/>
-      <c r="U9" s="170" t="s">
+      <c r="U9" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="170"/>
+      <c r="V9" s="189"/>
       <c r="W9" s="45"/>
       <c r="X9" s="46" t="s">
         <v>28</v>
       </c>
       <c r="Y9" s="47"/>
-      <c r="Z9" s="171" t="s">
+      <c r="Z9" s="190" t="s">
         <v>29</v>
       </c>
-      <c r="AA9" s="171"/>
+      <c r="AA9" s="190"/>
       <c r="AB9" s="47"/>
-      <c r="AC9" s="165" t="s">
+      <c r="AC9" s="184" t="s">
         <v>30</v>
       </c>
-      <c r="AD9" s="165"/>
-      <c r="AE9" s="165"/>
+      <c r="AD9" s="184"/>
+      <c r="AE9" s="184"/>
       <c r="AF9" s="45"/>
-      <c r="AG9" s="166" t="s">
+      <c r="AG9" s="185" t="s">
         <v>18</v>
       </c>
-      <c r="AH9" s="166"/>
+      <c r="AH9" s="185"/>
     </row>
     <row r="10" spans="1:1024" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="49" t="s">
@@ -11836,19 +11757,19 @@
     </row>
     <row r="15" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="85" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="172" t="s">
+      <c r="C15" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F15" s="88" t="s">
         <v>95</v>
@@ -11856,72 +11777,72 @@
       <c r="G15" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="173" t="s">
+      <c r="H15" s="166" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="173" t="s">
+      <c r="I15" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J15" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="K15" s="174" t="s">
+      <c r="K15" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="L15" s="175"/>
-      <c r="M15" s="176" t="s">
-        <v>440</v>
-      </c>
-      <c r="N15" s="177" t="s">
+      <c r="L15" s="168"/>
+      <c r="M15" s="169" t="s">
+        <v>438</v>
+      </c>
+      <c r="N15" s="170" t="s">
         <v>102</v>
       </c>
-      <c r="O15" s="175"/>
-      <c r="P15" s="173" t="s">
+      <c r="O15" s="168"/>
+      <c r="P15" s="166" t="s">
         <v>103</v>
       </c>
       <c r="Q15" s="89" t="s">
         <v>100</v>
       </c>
       <c r="R15" s="85" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="S15" s="94" t="s">
-        <v>442</v>
-      </c>
-      <c r="T15" s="178"/>
+        <v>452</v>
+      </c>
+      <c r="T15" s="171"/>
       <c r="U15" s="85" t="s">
-        <v>438</v>
-      </c>
-      <c r="V15" s="179">
+        <v>449</v>
+      </c>
+      <c r="V15" s="172">
         <v>1</v>
       </c>
-      <c r="W15" s="178"/>
+      <c r="W15" s="171"/>
       <c r="X15" s="112" t="s">
-        <v>443</v>
-      </c>
-      <c r="Y15" s="180"/>
+        <v>439</v>
+      </c>
+      <c r="Y15" s="173"/>
       <c r="Z15" s="96" t="s">
-        <v>444</v>
-      </c>
-      <c r="AA15" s="181">
+        <v>440</v>
+      </c>
+      <c r="AA15" s="174">
         <v>5</v>
       </c>
-      <c r="AB15" s="182"/>
-      <c r="AC15" s="183">
+      <c r="AB15" s="175"/>
+      <c r="AC15" s="176">
         <v>1</v>
       </c>
-      <c r="AD15" s="183">
+      <c r="AD15" s="176">
         <v>2</v>
       </c>
       <c r="AE15" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="AF15" s="175"/>
-      <c r="AG15" s="176" t="s">
-        <v>445</v>
-      </c>
-      <c r="AH15" s="176" t="s">
-        <v>446</v>
+      <c r="AF15" s="168"/>
+      <c r="AG15" s="169" t="s">
+        <v>441</v>
+      </c>
+      <c r="AH15" s="169" t="s">
+        <v>442</v>
       </c>
       <c r="AI15"/>
       <c r="AJ15"/>
@@ -12916,19 +12837,19 @@
     </row>
     <row r="16" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="85" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="172" t="s">
+      <c r="C16" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>119</v>
+        <v>406</v>
       </c>
       <c r="E16" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F16" s="88" t="s">
         <v>108</v>
@@ -12936,23 +12857,23 @@
       <c r="G16" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="173" t="s">
+      <c r="H16" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="I16" s="173" t="s">
+      <c r="I16" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J16" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="174" t="s">
+      <c r="K16" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L16" s="175"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="175"/>
-      <c r="P16" s="173" t="s">
+      <c r="L16" s="168"/>
+      <c r="M16" s="169"/>
+      <c r="N16" s="170"/>
+      <c r="O16" s="168"/>
+      <c r="P16" s="166" t="s">
         <v>116</v>
       </c>
       <c r="Q16" s="89" t="s">
@@ -12960,31 +12881,31 @@
       </c>
       <c r="R16" s="99"/>
       <c r="S16" s="100"/>
-      <c r="T16" s="178"/>
+      <c r="T16" s="171"/>
       <c r="U16" s="85" t="s">
-        <v>441</v>
-      </c>
-      <c r="V16" s="179">
+        <v>451</v>
+      </c>
+      <c r="V16" s="172">
         <v>1</v>
       </c>
-      <c r="W16" s="178"/>
+      <c r="W16" s="171"/>
       <c r="X16" s="101" t="s">
-        <v>447</v>
-      </c>
-      <c r="Y16" s="180"/>
-      <c r="Z16" s="184"/>
-      <c r="AA16" s="181">
+        <v>443</v>
+      </c>
+      <c r="Y16" s="173"/>
+      <c r="Z16" s="177"/>
+      <c r="AA16" s="174">
         <v>10</v>
       </c>
-      <c r="AB16" s="182"/>
-      <c r="AC16" s="183"/>
-      <c r="AD16" s="183"/>
+      <c r="AB16" s="175"/>
+      <c r="AC16" s="176"/>
+      <c r="AD16" s="176"/>
       <c r="AE16" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="AF16" s="175"/>
-      <c r="AG16" s="176"/>
-      <c r="AH16" s="176"/>
+      <c r="AF16" s="168"/>
+      <c r="AG16" s="169"/>
+      <c r="AH16" s="169"/>
       <c r="AI16"/>
       <c r="AJ16"/>
       <c r="AK16"/>
@@ -13978,19 +13899,19 @@
     </row>
     <row r="17" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="85" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="172" t="s">
+      <c r="C17" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>128</v>
+        <v>271</v>
       </c>
       <c r="E17" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F17" s="88" t="s">
         <v>95</v>
@@ -13998,23 +13919,23 @@
       <c r="G17" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="173" t="s">
+      <c r="H17" s="166" t="s">
         <v>179</v>
       </c>
-      <c r="I17" s="173" t="s">
+      <c r="I17" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J17" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="174" t="s">
+      <c r="K17" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L17" s="175"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="177"/>
-      <c r="O17" s="175"/>
-      <c r="P17" s="173" t="s">
+      <c r="L17" s="168"/>
+      <c r="M17" s="169"/>
+      <c r="N17" s="170"/>
+      <c r="O17" s="168"/>
+      <c r="P17" s="166" t="s">
         <v>126</v>
       </c>
       <c r="Q17" s="89" t="s">
@@ -14022,29 +13943,29 @@
       </c>
       <c r="R17" s="99"/>
       <c r="S17" s="100"/>
-      <c r="T17" s="178"/>
-      <c r="U17" s="94" t="s">
-        <v>442</v>
-      </c>
-      <c r="V17" s="179">
+      <c r="T17" s="171"/>
+      <c r="U17" s="85" t="s">
+        <v>452</v>
+      </c>
+      <c r="V17" s="172">
         <v>1</v>
       </c>
-      <c r="W17" s="178"/>
+      <c r="W17" s="171"/>
       <c r="X17" s="112" t="s">
-        <v>448</v>
-      </c>
-      <c r="Y17" s="180"/>
-      <c r="Z17" s="184"/>
-      <c r="AA17" s="181">
+        <v>444</v>
+      </c>
+      <c r="Y17" s="173"/>
+      <c r="Z17" s="177"/>
+      <c r="AA17" s="174">
         <v>15</v>
       </c>
-      <c r="AB17" s="182"/>
-      <c r="AC17" s="185"/>
-      <c r="AD17" s="185"/>
-      <c r="AE17" s="186"/>
-      <c r="AF17" s="175"/>
-      <c r="AG17" s="176"/>
-      <c r="AH17" s="176"/>
+      <c r="AB17" s="175"/>
+      <c r="AC17" s="178"/>
+      <c r="AD17" s="178"/>
+      <c r="AE17" s="179"/>
+      <c r="AF17" s="168"/>
+      <c r="AG17" s="169"/>
+      <c r="AH17" s="169"/>
       <c r="AI17"/>
       <c r="AJ17"/>
       <c r="AK17"/>
@@ -15038,19 +14959,19 @@
     </row>
     <row r="18" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="85" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D18" s="87" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="E18" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F18" s="88" t="s">
         <v>120</v>
@@ -15058,23 +14979,23 @@
       <c r="G18" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="173" t="s">
+      <c r="H18" s="166" t="s">
         <v>174</v>
       </c>
-      <c r="I18" s="173" t="s">
+      <c r="I18" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J18" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="174" t="s">
+      <c r="K18" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L18" s="175"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="177"/>
-      <c r="O18" s="175"/>
-      <c r="P18" s="173" t="s">
+      <c r="L18" s="168"/>
+      <c r="M18" s="169"/>
+      <c r="N18" s="170"/>
+      <c r="O18" s="168"/>
+      <c r="P18" s="166" t="s">
         <v>134</v>
       </c>
       <c r="Q18" s="89" t="s">
@@ -15082,30 +15003,29 @@
       </c>
       <c r="R18" s="99"/>
       <c r="S18" s="100"/>
-      <c r="T18" s="178"/>
-      <c r="U18" s="187" t="str">
-        <f>A18</f>
-        <v>whole-genome-4</v>
-      </c>
-      <c r="V18" s="179">
+      <c r="T18" s="171"/>
+      <c r="U18" s="85" t="s">
+        <v>453</v>
+      </c>
+      <c r="V18" s="172">
         <v>1</v>
       </c>
-      <c r="W18" s="178"/>
+      <c r="W18" s="171"/>
       <c r="X18" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y18" s="180"/>
-      <c r="Z18" s="184"/>
-      <c r="AA18" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y18" s="173"/>
+      <c r="Z18" s="177"/>
+      <c r="AA18" s="174">
         <v>20</v>
       </c>
-      <c r="AB18" s="182"/>
-      <c r="AC18" s="185"/>
-      <c r="AD18" s="185"/>
-      <c r="AE18" s="186"/>
-      <c r="AF18" s="175"/>
-      <c r="AG18" s="176"/>
-      <c r="AH18" s="176"/>
+      <c r="AB18" s="175"/>
+      <c r="AC18" s="178"/>
+      <c r="AD18" s="178"/>
+      <c r="AE18" s="179"/>
+      <c r="AF18" s="168"/>
+      <c r="AG18" s="169"/>
+      <c r="AH18" s="169"/>
       <c r="AI18"/>
       <c r="AJ18"/>
       <c r="AK18"/>
@@ -16099,19 +16019,19 @@
     </row>
     <row r="19" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="85" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="E19" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F19" s="88" t="s">
         <v>120</v>
@@ -16119,23 +16039,23 @@
       <c r="G19" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="188" t="s">
+      <c r="H19" s="180" t="s">
         <v>138</v>
       </c>
-      <c r="I19" s="173" t="s">
+      <c r="I19" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J19" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="174" t="s">
+      <c r="K19" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="175"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="177"/>
-      <c r="O19" s="175"/>
-      <c r="P19" s="173" t="s">
+      <c r="L19" s="168"/>
+      <c r="M19" s="169"/>
+      <c r="N19" s="170"/>
+      <c r="O19" s="168"/>
+      <c r="P19" s="166" t="s">
         <v>141</v>
       </c>
       <c r="Q19" s="89" t="s">
@@ -16143,31 +16063,30 @@
       </c>
       <c r="R19" s="99"/>
       <c r="S19" s="100"/>
-      <c r="T19" s="178"/>
-      <c r="U19" s="187" t="str">
-        <f t="shared" ref="U19:U52" si="0">A19</f>
-        <v>whole-genome-5</v>
-      </c>
-      <c r="V19" s="179">
+      <c r="T19" s="171"/>
+      <c r="U19" s="85" t="s">
+        <v>454</v>
+      </c>
+      <c r="V19" s="172">
         <v>1</v>
       </c>
-      <c r="W19" s="178"/>
+      <c r="W19" s="171"/>
       <c r="X19" s="112" t="s">
-        <v>452</v>
-      </c>
-      <c r="Y19" s="180"/>
-      <c r="Z19" s="184"/>
-      <c r="AA19" s="181">
+        <v>446</v>
+      </c>
+      <c r="Y19" s="173"/>
+      <c r="Z19" s="177"/>
+      <c r="AA19" s="174">
         <v>25</v>
       </c>
-      <c r="AB19" s="182"/>
-      <c r="AC19" s="185"/>
-      <c r="AD19" s="185"/>
-      <c r="AE19" s="186"/>
-      <c r="AF19" s="175"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="176" t="s">
-        <v>453</v>
+      <c r="AB19" s="175"/>
+      <c r="AC19" s="178"/>
+      <c r="AD19" s="178"/>
+      <c r="AE19" s="179"/>
+      <c r="AF19" s="168"/>
+      <c r="AG19" s="169"/>
+      <c r="AH19" s="169" t="s">
+        <v>447</v>
       </c>
       <c r="AI19"/>
       <c r="AJ19"/>
@@ -17162,19 +17081,19 @@
     </row>
     <row r="20" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="85" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D20" s="87" t="s">
-        <v>147</v>
+        <v>405</v>
       </c>
       <c r="E20" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F20" s="88" t="s">
         <v>120</v>
@@ -17182,23 +17101,23 @@
       <c r="G20" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="173" t="s">
+      <c r="H20" s="166" t="s">
         <v>154</v>
       </c>
-      <c r="I20" s="173" t="s">
+      <c r="I20" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J20" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K20" s="174" t="s">
+      <c r="K20" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L20" s="175"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="177"/>
-      <c r="O20" s="175"/>
-      <c r="P20" s="173" t="s">
+      <c r="L20" s="168"/>
+      <c r="M20" s="169"/>
+      <c r="N20" s="170"/>
+      <c r="O20" s="168"/>
+      <c r="P20" s="166" t="s">
         <v>146</v>
       </c>
       <c r="Q20" s="89" t="s">
@@ -17206,30 +17125,29 @@
       </c>
       <c r="R20" s="99"/>
       <c r="S20" s="100"/>
-      <c r="T20" s="178"/>
-      <c r="U20" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-genome-6</v>
-      </c>
-      <c r="V20" s="179">
+      <c r="T20" s="171"/>
+      <c r="U20" s="85" t="s">
+        <v>455</v>
+      </c>
+      <c r="V20" s="172">
         <v>1</v>
       </c>
-      <c r="W20" s="178"/>
+      <c r="W20" s="171"/>
       <c r="X20" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y20" s="180"/>
-      <c r="Z20" s="184"/>
-      <c r="AA20" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y20" s="173"/>
+      <c r="Z20" s="177"/>
+      <c r="AA20" s="174">
         <v>30</v>
       </c>
-      <c r="AB20" s="182"/>
-      <c r="AC20" s="185"/>
-      <c r="AD20" s="185"/>
-      <c r="AE20" s="186"/>
-      <c r="AF20" s="175"/>
-      <c r="AG20" s="176"/>
-      <c r="AH20" s="176"/>
+      <c r="AB20" s="175"/>
+      <c r="AC20" s="178"/>
+      <c r="AD20" s="178"/>
+      <c r="AE20" s="179"/>
+      <c r="AF20" s="168"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="169"/>
       <c r="AI20"/>
       <c r="AJ20"/>
       <c r="AK20"/>
@@ -18223,19 +18141,19 @@
     </row>
     <row r="21" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="85" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D21" s="87" t="s">
-        <v>152</v>
+        <v>283</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F21" s="88" t="s">
         <v>120</v>
@@ -18243,23 +18161,23 @@
       <c r="G21" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="173" t="s">
+      <c r="H21" s="166" t="s">
         <v>169</v>
       </c>
-      <c r="I21" s="173" t="s">
+      <c r="I21" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J21" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="174" t="s">
+      <c r="K21" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L21" s="175"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="177"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="173" t="s">
+      <c r="L21" s="168"/>
+      <c r="M21" s="169"/>
+      <c r="N21" s="170"/>
+      <c r="O21" s="168"/>
+      <c r="P21" s="166" t="s">
         <v>151</v>
       </c>
       <c r="Q21" s="89" t="s">
@@ -18267,30 +18185,29 @@
       </c>
       <c r="R21" s="99"/>
       <c r="S21" s="100"/>
-      <c r="T21" s="178"/>
-      <c r="U21" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-genome-7</v>
-      </c>
-      <c r="V21" s="179">
+      <c r="T21" s="171"/>
+      <c r="U21" s="85" t="s">
+        <v>456</v>
+      </c>
+      <c r="V21" s="172">
         <v>1</v>
       </c>
-      <c r="W21" s="178"/>
+      <c r="W21" s="171"/>
       <c r="X21" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y21" s="180"/>
-      <c r="Z21" s="184"/>
-      <c r="AA21" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y21" s="173"/>
+      <c r="Z21" s="177"/>
+      <c r="AA21" s="174">
         <v>35</v>
       </c>
-      <c r="AB21" s="182"/>
-      <c r="AC21" s="185"/>
-      <c r="AD21" s="185"/>
-      <c r="AE21" s="186"/>
-      <c r="AF21" s="175"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="176"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="178"/>
+      <c r="AD21" s="178"/>
+      <c r="AE21" s="179"/>
+      <c r="AF21" s="168"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="169"/>
       <c r="AI21"/>
       <c r="AJ21"/>
       <c r="AK21"/>
@@ -19284,19 +19201,19 @@
     </row>
     <row r="22" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="85" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="87" t="s">
-        <v>457</v>
+      <c r="D22" s="112" t="s">
+        <v>407</v>
       </c>
       <c r="E22" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F22" s="88" t="s">
         <v>120</v>
@@ -19304,23 +19221,23 @@
       <c r="G22" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="173" t="s">
+      <c r="H22" s="166" t="s">
         <v>130</v>
       </c>
-      <c r="I22" s="173" t="s">
+      <c r="I22" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J22" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K22" s="174" t="s">
+      <c r="K22" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L22" s="175"/>
-      <c r="M22" s="176"/>
-      <c r="N22" s="177"/>
-      <c r="O22" s="175"/>
-      <c r="P22" s="173" t="s">
+      <c r="L22" s="168"/>
+      <c r="M22" s="169"/>
+      <c r="N22" s="170"/>
+      <c r="O22" s="168"/>
+      <c r="P22" s="166" t="s">
         <v>156</v>
       </c>
       <c r="Q22" s="89" t="s">
@@ -19328,32 +19245,31 @@
       </c>
       <c r="R22" s="99"/>
       <c r="S22" s="100"/>
-      <c r="T22" s="178"/>
-      <c r="U22" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-1</v>
-      </c>
-      <c r="V22" s="179">
+      <c r="T22" s="171"/>
+      <c r="U22" s="85" t="s">
+        <v>457</v>
+      </c>
+      <c r="V22" s="172">
         <v>1</v>
       </c>
-      <c r="W22" s="178"/>
+      <c r="W22" s="171"/>
       <c r="X22" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y22" s="180"/>
-      <c r="Z22" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y22" s="173"/>
+      <c r="Z22" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA22" s="181">
+      <c r="AA22" s="174">
         <v>40</v>
       </c>
-      <c r="AB22" s="182"/>
-      <c r="AC22" s="185"/>
-      <c r="AD22" s="185"/>
-      <c r="AE22" s="186"/>
-      <c r="AF22" s="175"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="189"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="178"/>
+      <c r="AD22" s="178"/>
+      <c r="AE22" s="179"/>
+      <c r="AF22" s="168"/>
+      <c r="AG22" s="169"/>
+      <c r="AH22" s="181"/>
       <c r="AI22"/>
       <c r="AJ22"/>
       <c r="AK22"/>
@@ -20347,19 +20263,19 @@
     </row>
     <row r="23" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="85" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="87" t="s">
-        <v>460</v>
+      <c r="D23" s="112" t="s">
+        <v>409</v>
       </c>
       <c r="E23" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F23" s="88" t="s">
         <v>120</v>
@@ -20367,23 +20283,23 @@
       <c r="G23" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="173" t="s">
+      <c r="H23" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="I23" s="173" t="s">
+      <c r="I23" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J23" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="174" t="s">
+      <c r="K23" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L23" s="175"/>
-      <c r="M23" s="176"/>
-      <c r="N23" s="177"/>
-      <c r="O23" s="175"/>
-      <c r="P23" s="173" t="s">
+      <c r="L23" s="168"/>
+      <c r="M23" s="169"/>
+      <c r="N23" s="170"/>
+      <c r="O23" s="168"/>
+      <c r="P23" s="166" t="s">
         <v>161</v>
       </c>
       <c r="Q23" s="89" t="s">
@@ -20391,32 +20307,31 @@
       </c>
       <c r="R23" s="99"/>
       <c r="S23" s="100"/>
-      <c r="T23" s="178"/>
-      <c r="U23" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-2</v>
-      </c>
-      <c r="V23" s="179">
+      <c r="T23" s="171"/>
+      <c r="U23" s="85" t="s">
+        <v>458</v>
+      </c>
+      <c r="V23" s="172">
         <v>1</v>
       </c>
-      <c r="W23" s="178"/>
+      <c r="W23" s="171"/>
       <c r="X23" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y23" s="180"/>
-      <c r="Z23" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y23" s="173"/>
+      <c r="Z23" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="AA23" s="181">
+      <c r="AA23" s="174">
         <v>45</v>
       </c>
-      <c r="AB23" s="182"/>
-      <c r="AC23" s="185"/>
-      <c r="AD23" s="185"/>
-      <c r="AE23" s="186"/>
-      <c r="AF23" s="175"/>
-      <c r="AG23" s="176"/>
-      <c r="AH23" s="176"/>
+      <c r="AB23" s="175"/>
+      <c r="AC23" s="178"/>
+      <c r="AD23" s="178"/>
+      <c r="AE23" s="179"/>
+      <c r="AF23" s="168"/>
+      <c r="AG23" s="169"/>
+      <c r="AH23" s="169"/>
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
@@ -21410,19 +21325,19 @@
     </row>
     <row r="24" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="85" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="87" t="s">
-        <v>462</v>
+      <c r="D24" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E24" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F24" s="88" t="s">
         <v>120</v>
@@ -21430,23 +21345,23 @@
       <c r="G24" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="173" t="s">
+      <c r="H24" s="166" t="s">
         <v>122</v>
       </c>
-      <c r="I24" s="173" t="s">
+      <c r="I24" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J24" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K24" s="174" t="s">
+      <c r="K24" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L24" s="175"/>
-      <c r="M24" s="176"/>
-      <c r="N24" s="177"/>
-      <c r="O24" s="175"/>
-      <c r="P24" s="173" t="s">
+      <c r="L24" s="168"/>
+      <c r="M24" s="169"/>
+      <c r="N24" s="170"/>
+      <c r="O24" s="168"/>
+      <c r="P24" s="166" t="s">
         <v>166</v>
       </c>
       <c r="Q24" s="89" t="s">
@@ -21454,32 +21369,31 @@
       </c>
       <c r="R24" s="99"/>
       <c r="S24" s="100"/>
-      <c r="T24" s="178"/>
-      <c r="U24" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-3</v>
-      </c>
-      <c r="V24" s="179">
+      <c r="T24" s="171"/>
+      <c r="U24" s="85" t="s">
+        <v>459</v>
+      </c>
+      <c r="V24" s="172">
         <v>1</v>
       </c>
-      <c r="W24" s="178"/>
+      <c r="W24" s="171"/>
       <c r="X24" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y24" s="180"/>
+        <v>445</v>
+      </c>
+      <c r="Y24" s="173"/>
       <c r="Z24" s="112" t="s">
         <v>124</v>
       </c>
-      <c r="AA24" s="181">
+      <c r="AA24" s="174">
         <v>50</v>
       </c>
-      <c r="AB24" s="182"/>
-      <c r="AC24" s="185"/>
-      <c r="AD24" s="185"/>
-      <c r="AE24" s="186"/>
-      <c r="AF24" s="175"/>
-      <c r="AG24" s="176"/>
-      <c r="AH24" s="176"/>
+      <c r="AB24" s="175"/>
+      <c r="AC24" s="178"/>
+      <c r="AD24" s="178"/>
+      <c r="AE24" s="179"/>
+      <c r="AF24" s="168"/>
+      <c r="AG24" s="169"/>
+      <c r="AH24" s="169"/>
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -22473,19 +22387,19 @@
     </row>
     <row r="25" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="85" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="172" t="s">
+      <c r="C25" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="87" t="s">
-        <v>464</v>
+      <c r="D25" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E25" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F25" s="88" t="s">
         <v>120</v>
@@ -22493,23 +22407,23 @@
       <c r="G25" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H25" s="190" t="s">
+      <c r="H25" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="I25" s="173" t="s">
+      <c r="I25" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J25" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="174" t="s">
+      <c r="K25" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="175"/>
-      <c r="M25" s="176"/>
-      <c r="N25" s="177"/>
-      <c r="O25" s="175"/>
-      <c r="P25" s="173" t="s">
+      <c r="L25" s="168"/>
+      <c r="M25" s="169"/>
+      <c r="N25" s="170"/>
+      <c r="O25" s="168"/>
+      <c r="P25" s="166" t="s">
         <v>171</v>
       </c>
       <c r="Q25" s="89" t="s">
@@ -22517,33 +22431,32 @@
       </c>
       <c r="R25" s="99"/>
       <c r="S25" s="100"/>
-      <c r="T25" s="178"/>
-      <c r="U25" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-4</v>
-      </c>
-      <c r="V25" s="179">
+      <c r="T25" s="171"/>
+      <c r="U25" s="85" t="s">
+        <v>460</v>
+      </c>
+      <c r="V25" s="172">
         <v>1</v>
       </c>
-      <c r="W25" s="178"/>
+      <c r="W25" s="171"/>
       <c r="X25" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y25" s="180"/>
-      <c r="Z25" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y25" s="173"/>
+      <c r="Z25" s="166" t="s">
         <v>132</v>
       </c>
-      <c r="AA25" s="181">
+      <c r="AA25" s="174">
         <v>55</v>
       </c>
-      <c r="AB25" s="182"/>
-      <c r="AC25" s="185"/>
-      <c r="AD25" s="185"/>
-      <c r="AE25" s="186"/>
-      <c r="AF25" s="175"/>
-      <c r="AG25" s="176"/>
-      <c r="AH25" s="176" t="s">
-        <v>465</v>
+      <c r="AB25" s="175"/>
+      <c r="AC25" s="178"/>
+      <c r="AD25" s="178"/>
+      <c r="AE25" s="179"/>
+      <c r="AF25" s="168"/>
+      <c r="AG25" s="169"/>
+      <c r="AH25" s="169" t="s">
+        <v>448</v>
       </c>
       <c r="AI25"/>
       <c r="AJ25"/>
@@ -23538,19 +23451,19 @@
     </row>
     <row r="26" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="85" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="172" t="s">
+      <c r="C26" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="87" t="s">
-        <v>467</v>
+      <c r="D26" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E26" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F26" s="88" t="s">
         <v>120</v>
@@ -23558,23 +23471,23 @@
       <c r="G26" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="190" t="s">
+      <c r="H26" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="173" t="s">
+      <c r="I26" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J26" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="174" t="s">
+      <c r="K26" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L26" s="175"/>
-      <c r="M26" s="176"/>
-      <c r="N26" s="177"/>
-      <c r="O26" s="175"/>
-      <c r="P26" s="173" t="s">
+      <c r="L26" s="168"/>
+      <c r="M26" s="169"/>
+      <c r="N26" s="170"/>
+      <c r="O26" s="168"/>
+      <c r="P26" s="166" t="s">
         <v>176</v>
       </c>
       <c r="Q26" s="89" t="s">
@@ -23582,32 +23495,31 @@
       </c>
       <c r="R26" s="99"/>
       <c r="S26" s="100"/>
-      <c r="T26" s="178"/>
-      <c r="U26" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-5</v>
-      </c>
-      <c r="V26" s="179">
+      <c r="T26" s="171"/>
+      <c r="U26" s="85" t="s">
+        <v>461</v>
+      </c>
+      <c r="V26" s="172">
         <v>1</v>
       </c>
-      <c r="W26" s="178"/>
+      <c r="W26" s="171"/>
       <c r="X26" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y26" s="180"/>
-      <c r="Z26" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y26" s="173"/>
+      <c r="Z26" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA26" s="181">
+      <c r="AA26" s="174">
         <v>60</v>
       </c>
-      <c r="AB26" s="182"/>
-      <c r="AC26" s="185"/>
-      <c r="AD26" s="185"/>
-      <c r="AE26" s="186"/>
-      <c r="AF26" s="175"/>
-      <c r="AG26" s="176"/>
-      <c r="AH26" s="176"/>
+      <c r="AB26" s="175"/>
+      <c r="AC26" s="178"/>
+      <c r="AD26" s="178"/>
+      <c r="AE26" s="179"/>
+      <c r="AF26" s="168"/>
+      <c r="AG26" s="169"/>
+      <c r="AH26" s="169"/>
       <c r="AI26"/>
       <c r="AJ26"/>
       <c r="AK26"/>
@@ -24601,19 +24513,19 @@
     </row>
     <row r="27" spans="1:1024" s="104" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="85" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="172" t="s">
+      <c r="C27" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="87" t="s">
-        <v>469</v>
+      <c r="D27" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E27" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F27" s="88" t="s">
         <v>120</v>
@@ -24621,23 +24533,23 @@
       <c r="G27" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H27" s="173" t="s">
+      <c r="H27" s="166" t="s">
         <v>184</v>
       </c>
-      <c r="I27" s="173" t="s">
+      <c r="I27" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J27" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="174" t="s">
+      <c r="K27" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L27" s="175"/>
-      <c r="M27" s="176"/>
-      <c r="N27" s="177"/>
-      <c r="O27" s="175"/>
-      <c r="P27" s="173" t="s">
+      <c r="L27" s="168"/>
+      <c r="M27" s="169"/>
+      <c r="N27" s="170"/>
+      <c r="O27" s="168"/>
+      <c r="P27" s="166" t="s">
         <v>181</v>
       </c>
       <c r="Q27" s="89" t="s">
@@ -24645,48 +24557,47 @@
       </c>
       <c r="R27" s="99"/>
       <c r="S27" s="100"/>
-      <c r="T27" s="178"/>
-      <c r="U27" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-6</v>
-      </c>
-      <c r="V27" s="179">
+      <c r="T27" s="171"/>
+      <c r="U27" s="85" t="s">
+        <v>462</v>
+      </c>
+      <c r="V27" s="172">
         <v>1</v>
       </c>
-      <c r="W27" s="178"/>
+      <c r="W27" s="171"/>
       <c r="X27" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y27" s="180"/>
-      <c r="Z27" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y27" s="173"/>
+      <c r="Z27" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA27" s="181">
+      <c r="AA27" s="174">
         <v>65</v>
       </c>
-      <c r="AB27" s="182"/>
-      <c r="AC27" s="185"/>
-      <c r="AD27" s="185"/>
-      <c r="AE27" s="186"/>
-      <c r="AF27" s="175"/>
-      <c r="AG27" s="176"/>
-      <c r="AH27" s="176"/>
+      <c r="AB27" s="175"/>
+      <c r="AC27" s="178"/>
+      <c r="AD27" s="178"/>
+      <c r="AE27" s="179"/>
+      <c r="AF27" s="168"/>
+      <c r="AG27" s="169"/>
+      <c r="AH27" s="169"/>
     </row>
     <row r="28" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="85" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="172" t="s">
+      <c r="C28" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="87" t="s">
-        <v>471</v>
+      <c r="D28" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E28" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F28" s="88" t="s">
         <v>120</v>
@@ -24694,23 +24605,23 @@
       <c r="G28" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="190" t="s">
+      <c r="H28" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="173" t="s">
+      <c r="I28" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J28" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K28" s="174" t="s">
+      <c r="K28" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L28" s="175"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="177"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="173" t="s">
+      <c r="L28" s="168"/>
+      <c r="M28" s="169"/>
+      <c r="N28" s="170"/>
+      <c r="O28" s="168"/>
+      <c r="P28" s="166" t="s">
         <v>186</v>
       </c>
       <c r="Q28" s="89" t="s">
@@ -24718,32 +24629,31 @@
       </c>
       <c r="R28" s="99"/>
       <c r="S28" s="100"/>
-      <c r="T28" s="178"/>
-      <c r="U28" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-7</v>
-      </c>
-      <c r="V28" s="179">
+      <c r="T28" s="171"/>
+      <c r="U28" s="85" t="s">
+        <v>463</v>
+      </c>
+      <c r="V28" s="172">
         <v>1</v>
       </c>
-      <c r="W28" s="178"/>
+      <c r="W28" s="171"/>
       <c r="X28" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y28" s="180"/>
-      <c r="Z28" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y28" s="173"/>
+      <c r="Z28" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA28" s="181">
+      <c r="AA28" s="174">
         <v>70</v>
       </c>
-      <c r="AB28" s="182"/>
-      <c r="AC28" s="185"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="186"/>
-      <c r="AF28" s="175"/>
-      <c r="AG28" s="176"/>
-      <c r="AH28" s="176"/>
+      <c r="AB28" s="175"/>
+      <c r="AC28" s="178"/>
+      <c r="AD28" s="178"/>
+      <c r="AE28" s="179"/>
+      <c r="AF28" s="168"/>
+      <c r="AG28" s="169"/>
+      <c r="AH28" s="169"/>
       <c r="AI28"/>
       <c r="AJ28"/>
       <c r="AK28"/>
@@ -25737,19 +25647,19 @@
     </row>
     <row r="29" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="85" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="172" t="s">
+      <c r="C29" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="87" t="s">
-        <v>473</v>
+      <c r="D29" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E29" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F29" s="88" t="s">
         <v>120</v>
@@ -25757,23 +25667,23 @@
       <c r="G29" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H29" s="190" t="s">
+      <c r="H29" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I29" s="173" t="s">
+      <c r="I29" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J29" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K29" s="174" t="s">
+      <c r="K29" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L29" s="175"/>
-      <c r="M29" s="176"/>
-      <c r="N29" s="177"/>
-      <c r="O29" s="175"/>
-      <c r="P29" s="173" t="s">
+      <c r="L29" s="168"/>
+      <c r="M29" s="169"/>
+      <c r="N29" s="170"/>
+      <c r="O29" s="168"/>
+      <c r="P29" s="166" t="s">
         <v>190</v>
       </c>
       <c r="Q29" s="89" t="s">
@@ -25781,32 +25691,31 @@
       </c>
       <c r="R29" s="99"/>
       <c r="S29" s="100"/>
-      <c r="T29" s="178"/>
-      <c r="U29" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-8</v>
-      </c>
-      <c r="V29" s="179">
+      <c r="T29" s="171"/>
+      <c r="U29" s="85" t="s">
+        <v>464</v>
+      </c>
+      <c r="V29" s="172">
         <v>1</v>
       </c>
-      <c r="W29" s="178"/>
+      <c r="W29" s="171"/>
       <c r="X29" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y29" s="180"/>
-      <c r="Z29" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y29" s="173"/>
+      <c r="Z29" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA29" s="181">
+      <c r="AA29" s="174">
         <v>75</v>
       </c>
-      <c r="AB29" s="182"/>
-      <c r="AC29" s="185"/>
-      <c r="AD29" s="185"/>
-      <c r="AE29" s="186"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="176"/>
-      <c r="AH29" s="176"/>
+      <c r="AB29" s="175"/>
+      <c r="AC29" s="178"/>
+      <c r="AD29" s="178"/>
+      <c r="AE29" s="179"/>
+      <c r="AF29" s="168"/>
+      <c r="AG29" s="169"/>
+      <c r="AH29" s="169"/>
       <c r="AI29"/>
       <c r="AJ29"/>
       <c r="AK29"/>
@@ -26800,19 +26709,19 @@
     </row>
     <row r="30" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="85" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="172" t="s">
+      <c r="C30" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="87" t="s">
-        <v>475</v>
+      <c r="D30" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F30" s="88" t="s">
         <v>120</v>
@@ -26820,23 +26729,23 @@
       <c r="G30" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="190" t="s">
+      <c r="H30" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I30" s="173" t="s">
+      <c r="I30" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J30" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K30" s="174" t="s">
+      <c r="K30" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L30" s="175"/>
-      <c r="M30" s="176"/>
-      <c r="N30" s="177"/>
-      <c r="O30" s="175"/>
-      <c r="P30" s="173" t="s">
+      <c r="L30" s="168"/>
+      <c r="M30" s="169"/>
+      <c r="N30" s="170"/>
+      <c r="O30" s="168"/>
+      <c r="P30" s="166" t="s">
         <v>194</v>
       </c>
       <c r="Q30" s="89" t="s">
@@ -26844,32 +26753,31 @@
       </c>
       <c r="R30" s="99"/>
       <c r="S30" s="100"/>
-      <c r="T30" s="178"/>
-      <c r="U30" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-9</v>
-      </c>
-      <c r="V30" s="179">
+      <c r="T30" s="171"/>
+      <c r="U30" s="85" t="s">
+        <v>465</v>
+      </c>
+      <c r="V30" s="172">
         <v>1</v>
       </c>
-      <c r="W30" s="178"/>
+      <c r="W30" s="171"/>
       <c r="X30" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y30" s="180"/>
-      <c r="Z30" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y30" s="173"/>
+      <c r="Z30" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA30" s="181">
+      <c r="AA30" s="174">
         <v>80</v>
       </c>
-      <c r="AB30" s="182"/>
-      <c r="AC30" s="185"/>
-      <c r="AD30" s="185"/>
-      <c r="AE30" s="186"/>
-      <c r="AF30" s="175"/>
-      <c r="AG30" s="176"/>
-      <c r="AH30" s="176"/>
+      <c r="AB30" s="175"/>
+      <c r="AC30" s="178"/>
+      <c r="AD30" s="178"/>
+      <c r="AE30" s="179"/>
+      <c r="AF30" s="168"/>
+      <c r="AG30" s="169"/>
+      <c r="AH30" s="169"/>
       <c r="AI30"/>
       <c r="AJ30"/>
       <c r="AK30"/>
@@ -27863,19 +27771,19 @@
     </row>
     <row r="31" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="85" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="87" t="s">
-        <v>477</v>
+      <c r="D31" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E31" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F31" s="88" t="s">
         <v>120</v>
@@ -27883,23 +27791,23 @@
       <c r="G31" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H31" s="190" t="s">
+      <c r="H31" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I31" s="173" t="s">
+      <c r="I31" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J31" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K31" s="174" t="s">
+      <c r="K31" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L31" s="175"/>
-      <c r="M31" s="176"/>
-      <c r="N31" s="177"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="173" t="s">
+      <c r="L31" s="168"/>
+      <c r="M31" s="169"/>
+      <c r="N31" s="170"/>
+      <c r="O31" s="168"/>
+      <c r="P31" s="166" t="s">
         <v>198</v>
       </c>
       <c r="Q31" s="89" t="s">
@@ -27907,32 +27815,31 @@
       </c>
       <c r="R31" s="99"/>
       <c r="S31" s="100"/>
-      <c r="T31" s="178"/>
-      <c r="U31" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-10</v>
-      </c>
-      <c r="V31" s="179">
+      <c r="T31" s="171"/>
+      <c r="U31" s="85" t="s">
+        <v>466</v>
+      </c>
+      <c r="V31" s="172">
         <v>1</v>
       </c>
-      <c r="W31" s="178"/>
+      <c r="W31" s="171"/>
       <c r="X31" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y31" s="180"/>
-      <c r="Z31" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y31" s="173"/>
+      <c r="Z31" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA31" s="181">
+      <c r="AA31" s="174">
         <v>85</v>
       </c>
-      <c r="AB31" s="182"/>
-      <c r="AC31" s="185"/>
-      <c r="AD31" s="185"/>
-      <c r="AE31" s="186"/>
-      <c r="AF31" s="175"/>
-      <c r="AG31" s="176"/>
-      <c r="AH31" s="176"/>
+      <c r="AB31" s="175"/>
+      <c r="AC31" s="178"/>
+      <c r="AD31" s="178"/>
+      <c r="AE31" s="179"/>
+      <c r="AF31" s="168"/>
+      <c r="AG31" s="169"/>
+      <c r="AH31" s="169"/>
       <c r="AI31"/>
       <c r="AJ31"/>
       <c r="AK31"/>
@@ -28926,19 +28833,19 @@
     </row>
     <row r="32" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="85" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="172" t="s">
+      <c r="C32" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="87" t="s">
-        <v>479</v>
+      <c r="D32" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F32" s="88" t="s">
         <v>120</v>
@@ -28946,23 +28853,23 @@
       <c r="G32" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H32" s="190" t="s">
+      <c r="H32" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I32" s="173" t="s">
+      <c r="I32" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J32" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K32" s="174" t="s">
+      <c r="K32" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L32" s="175"/>
-      <c r="M32" s="176"/>
-      <c r="N32" s="177"/>
-      <c r="O32" s="175"/>
-      <c r="P32" s="173" t="s">
+      <c r="L32" s="168"/>
+      <c r="M32" s="169"/>
+      <c r="N32" s="170"/>
+      <c r="O32" s="168"/>
+      <c r="P32" s="166" t="s">
         <v>202</v>
       </c>
       <c r="Q32" s="89" t="s">
@@ -28970,32 +28877,31 @@
       </c>
       <c r="R32" s="99"/>
       <c r="S32" s="100"/>
-      <c r="T32" s="178"/>
-      <c r="U32" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-11</v>
-      </c>
-      <c r="V32" s="179">
+      <c r="T32" s="171"/>
+      <c r="U32" s="85" t="s">
+        <v>467</v>
+      </c>
+      <c r="V32" s="172">
         <v>1</v>
       </c>
-      <c r="W32" s="178"/>
+      <c r="W32" s="171"/>
       <c r="X32" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y32" s="180"/>
-      <c r="Z32" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y32" s="173"/>
+      <c r="Z32" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA32" s="181">
+      <c r="AA32" s="174">
         <v>90</v>
       </c>
-      <c r="AB32" s="182"/>
-      <c r="AC32" s="185"/>
-      <c r="AD32" s="185"/>
-      <c r="AE32" s="186"/>
-      <c r="AF32" s="175"/>
-      <c r="AG32" s="176"/>
-      <c r="AH32" s="176"/>
+      <c r="AB32" s="175"/>
+      <c r="AC32" s="178"/>
+      <c r="AD32" s="178"/>
+      <c r="AE32" s="179"/>
+      <c r="AF32" s="168"/>
+      <c r="AG32" s="169"/>
+      <c r="AH32" s="169"/>
       <c r="AI32"/>
       <c r="AJ32"/>
       <c r="AK32"/>
@@ -29989,19 +29895,19 @@
     </row>
     <row r="33" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="85" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="172" t="s">
+      <c r="C33" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="87" t="s">
-        <v>481</v>
+      <c r="D33" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E33" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F33" s="88" t="s">
         <v>120</v>
@@ -30009,23 +29915,23 @@
       <c r="G33" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H33" s="190" t="s">
+      <c r="H33" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I33" s="173" t="s">
+      <c r="I33" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J33" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K33" s="174" t="s">
+      <c r="K33" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L33" s="175"/>
-      <c r="M33" s="176"/>
-      <c r="N33" s="177"/>
-      <c r="O33" s="175"/>
-      <c r="P33" s="173" t="s">
+      <c r="L33" s="168"/>
+      <c r="M33" s="169"/>
+      <c r="N33" s="170"/>
+      <c r="O33" s="168"/>
+      <c r="P33" s="166" t="s">
         <v>206</v>
       </c>
       <c r="Q33" s="89" t="s">
@@ -30033,32 +29939,31 @@
       </c>
       <c r="R33" s="99"/>
       <c r="S33" s="100"/>
-      <c r="T33" s="178"/>
-      <c r="U33" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-12</v>
-      </c>
-      <c r="V33" s="179">
+      <c r="T33" s="171"/>
+      <c r="U33" s="85" t="s">
+        <v>468</v>
+      </c>
+      <c r="V33" s="172">
         <v>1</v>
       </c>
-      <c r="W33" s="178"/>
+      <c r="W33" s="171"/>
       <c r="X33" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y33" s="180"/>
-      <c r="Z33" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y33" s="173"/>
+      <c r="Z33" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA33" s="181">
+      <c r="AA33" s="174">
         <v>95</v>
       </c>
-      <c r="AB33" s="182"/>
-      <c r="AC33" s="185"/>
-      <c r="AD33" s="185"/>
-      <c r="AE33" s="186"/>
-      <c r="AF33" s="175"/>
-      <c r="AG33" s="176"/>
-      <c r="AH33" s="176"/>
+      <c r="AB33" s="175"/>
+      <c r="AC33" s="178"/>
+      <c r="AD33" s="178"/>
+      <c r="AE33" s="179"/>
+      <c r="AF33" s="168"/>
+      <c r="AG33" s="169"/>
+      <c r="AH33" s="169"/>
       <c r="AI33"/>
       <c r="AJ33"/>
       <c r="AK33"/>
@@ -31052,19 +30957,19 @@
     </row>
     <row r="34" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="85" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="172" t="s">
+      <c r="C34" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="87" t="s">
-        <v>483</v>
+      <c r="D34" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E34" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F34" s="88" t="s">
         <v>120</v>
@@ -31072,23 +30977,23 @@
       <c r="G34" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H34" s="190" t="s">
+      <c r="H34" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="173" t="s">
+      <c r="I34" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J34" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K34" s="174" t="s">
+      <c r="K34" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L34" s="175"/>
-      <c r="M34" s="176"/>
-      <c r="N34" s="177"/>
-      <c r="O34" s="175"/>
-      <c r="P34" s="173" t="s">
+      <c r="L34" s="168"/>
+      <c r="M34" s="169"/>
+      <c r="N34" s="170"/>
+      <c r="O34" s="168"/>
+      <c r="P34" s="166" t="s">
         <v>210</v>
       </c>
       <c r="Q34" s="89" t="s">
@@ -31096,32 +31001,31 @@
       </c>
       <c r="R34" s="99"/>
       <c r="S34" s="100"/>
-      <c r="T34" s="178"/>
-      <c r="U34" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-1</v>
-      </c>
-      <c r="V34" s="179">
+      <c r="T34" s="171"/>
+      <c r="U34" s="85" t="s">
+        <v>469</v>
+      </c>
+      <c r="V34" s="172">
         <v>1</v>
       </c>
-      <c r="W34" s="178"/>
+      <c r="W34" s="171"/>
       <c r="X34" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y34" s="180"/>
-      <c r="Z34" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y34" s="173"/>
+      <c r="Z34" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA34" s="181">
+      <c r="AA34" s="174">
         <v>100</v>
       </c>
-      <c r="AB34" s="182"/>
-      <c r="AC34" s="185"/>
-      <c r="AD34" s="185"/>
-      <c r="AE34" s="186"/>
-      <c r="AF34" s="175"/>
-      <c r="AG34" s="176"/>
-      <c r="AH34" s="176"/>
+      <c r="AB34" s="175"/>
+      <c r="AC34" s="178"/>
+      <c r="AD34" s="178"/>
+      <c r="AE34" s="179"/>
+      <c r="AF34" s="168"/>
+      <c r="AG34" s="169"/>
+      <c r="AH34" s="169"/>
       <c r="AI34"/>
       <c r="AJ34"/>
       <c r="AK34"/>
@@ -32115,19 +32019,19 @@
     </row>
     <row r="35" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="85" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B35" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="172" t="s">
+      <c r="C35" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="87" t="s">
-        <v>486</v>
+      <c r="D35" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E35" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F35" s="88" t="s">
         <v>120</v>
@@ -32135,23 +32039,23 @@
       <c r="G35" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="190" t="s">
+      <c r="H35" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I35" s="173" t="s">
+      <c r="I35" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J35" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K35" s="174" t="s">
+      <c r="K35" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L35" s="175"/>
-      <c r="M35" s="176"/>
-      <c r="N35" s="177"/>
-      <c r="O35" s="175"/>
-      <c r="P35" s="173" t="s">
+      <c r="L35" s="168"/>
+      <c r="M35" s="169"/>
+      <c r="N35" s="170"/>
+      <c r="O35" s="168"/>
+      <c r="P35" s="166" t="s">
         <v>214</v>
       </c>
       <c r="Q35" s="89" t="s">
@@ -32159,32 +32063,31 @@
       </c>
       <c r="R35" s="99"/>
       <c r="S35" s="100"/>
-      <c r="T35" s="178"/>
-      <c r="U35" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-2</v>
-      </c>
-      <c r="V35" s="179">
+      <c r="T35" s="171"/>
+      <c r="U35" s="85" t="s">
+        <v>470</v>
+      </c>
+      <c r="V35" s="172">
         <v>1</v>
       </c>
-      <c r="W35" s="178"/>
+      <c r="W35" s="171"/>
       <c r="X35" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y35" s="180"/>
-      <c r="Z35" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y35" s="173"/>
+      <c r="Z35" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA35" s="181">
+      <c r="AA35" s="174">
         <v>100</v>
       </c>
-      <c r="AB35" s="182"/>
-      <c r="AC35" s="185"/>
-      <c r="AD35" s="185"/>
-      <c r="AE35" s="186"/>
-      <c r="AF35" s="175"/>
-      <c r="AG35" s="176"/>
-      <c r="AH35" s="176"/>
+      <c r="AB35" s="175"/>
+      <c r="AC35" s="178"/>
+      <c r="AD35" s="178"/>
+      <c r="AE35" s="179"/>
+      <c r="AF35" s="168"/>
+      <c r="AG35" s="169"/>
+      <c r="AH35" s="169"/>
       <c r="AI35"/>
       <c r="AJ35"/>
       <c r="AK35"/>
@@ -33178,19 +33081,19 @@
     </row>
     <row r="36" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="85" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="B36" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="172" t="s">
+      <c r="C36" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="87" t="s">
-        <v>488</v>
+      <c r="D36" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E36" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F36" s="88" t="s">
         <v>120</v>
@@ -33198,23 +33101,23 @@
       <c r="G36" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H36" s="190" t="s">
+      <c r="H36" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I36" s="173" t="s">
+      <c r="I36" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J36" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K36" s="174" t="s">
+      <c r="K36" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L36" s="175"/>
-      <c r="M36" s="176"/>
-      <c r="N36" s="177"/>
-      <c r="O36" s="175"/>
-      <c r="P36" s="173" t="s">
+      <c r="L36" s="168"/>
+      <c r="M36" s="169"/>
+      <c r="N36" s="170"/>
+      <c r="O36" s="168"/>
+      <c r="P36" s="166" t="s">
         <v>218</v>
       </c>
       <c r="Q36" s="89" t="s">
@@ -33222,48 +33125,47 @@
       </c>
       <c r="R36" s="99"/>
       <c r="S36" s="100"/>
-      <c r="T36" s="178"/>
-      <c r="U36" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-3</v>
-      </c>
-      <c r="V36" s="179">
+      <c r="T36" s="171"/>
+      <c r="U36" s="85" t="s">
+        <v>471</v>
+      </c>
+      <c r="V36" s="172">
         <v>1</v>
       </c>
-      <c r="W36" s="178"/>
+      <c r="W36" s="171"/>
       <c r="X36" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y36" s="180"/>
-      <c r="Z36" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y36" s="173"/>
+      <c r="Z36" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA36" s="181">
+      <c r="AA36" s="174">
         <v>100</v>
       </c>
-      <c r="AB36" s="182"/>
-      <c r="AC36" s="185"/>
-      <c r="AD36" s="185"/>
-      <c r="AE36" s="186"/>
-      <c r="AF36" s="175"/>
-      <c r="AG36" s="176"/>
-      <c r="AH36" s="176"/>
+      <c r="AB36" s="175"/>
+      <c r="AC36" s="178"/>
+      <c r="AD36" s="178"/>
+      <c r="AE36" s="179"/>
+      <c r="AF36" s="168"/>
+      <c r="AG36" s="169"/>
+      <c r="AH36" s="169"/>
     </row>
     <row r="37" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="85" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B37" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="172" t="s">
+      <c r="C37" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D37" s="87" t="s">
-        <v>490</v>
+      <c r="D37" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E37" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F37" s="88" t="s">
         <v>120</v>
@@ -33271,23 +33173,23 @@
       <c r="G37" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="190" t="s">
+      <c r="H37" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I37" s="173" t="s">
+      <c r="I37" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J37" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K37" s="174" t="s">
+      <c r="K37" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L37" s="175"/>
-      <c r="M37" s="176"/>
-      <c r="N37" s="177"/>
-      <c r="O37" s="175"/>
-      <c r="P37" s="173" t="s">
+      <c r="L37" s="168"/>
+      <c r="M37" s="169"/>
+      <c r="N37" s="170"/>
+      <c r="O37" s="168"/>
+      <c r="P37" s="166" t="s">
         <v>222</v>
       </c>
       <c r="Q37" s="89" t="s">
@@ -33295,48 +33197,47 @@
       </c>
       <c r="R37" s="99"/>
       <c r="S37" s="100"/>
-      <c r="T37" s="178"/>
-      <c r="U37" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-4</v>
-      </c>
-      <c r="V37" s="179">
+      <c r="T37" s="171"/>
+      <c r="U37" s="85" t="s">
+        <v>472</v>
+      </c>
+      <c r="V37" s="172">
         <v>1</v>
       </c>
-      <c r="W37" s="178"/>
+      <c r="W37" s="171"/>
       <c r="X37" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y37" s="180"/>
-      <c r="Z37" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y37" s="173"/>
+      <c r="Z37" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA37" s="181">
+      <c r="AA37" s="174">
         <v>100</v>
       </c>
-      <c r="AB37" s="182"/>
-      <c r="AC37" s="185"/>
-      <c r="AD37" s="185"/>
-      <c r="AE37" s="186"/>
-      <c r="AF37" s="175"/>
-      <c r="AG37" s="176"/>
-      <c r="AH37" s="176"/>
+      <c r="AB37" s="175"/>
+      <c r="AC37" s="178"/>
+      <c r="AD37" s="178"/>
+      <c r="AE37" s="179"/>
+      <c r="AF37" s="168"/>
+      <c r="AG37" s="169"/>
+      <c r="AH37" s="169"/>
     </row>
     <row r="38" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="85" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B38" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="172" t="s">
+      <c r="C38" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="87" t="s">
-        <v>492</v>
+      <c r="D38" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E38" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F38" s="88" t="s">
         <v>120</v>
@@ -33344,23 +33245,23 @@
       <c r="G38" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H38" s="190" t="s">
+      <c r="H38" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I38" s="173" t="s">
+      <c r="I38" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J38" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K38" s="174" t="s">
+      <c r="K38" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L38" s="175"/>
-      <c r="M38" s="176"/>
-      <c r="N38" s="177"/>
-      <c r="O38" s="175"/>
-      <c r="P38" s="173" t="s">
+      <c r="L38" s="168"/>
+      <c r="M38" s="169"/>
+      <c r="N38" s="170"/>
+      <c r="O38" s="168"/>
+      <c r="P38" s="166" t="s">
         <v>226</v>
       </c>
       <c r="Q38" s="89" t="s">
@@ -33368,48 +33269,47 @@
       </c>
       <c r="R38" s="99"/>
       <c r="S38" s="100"/>
-      <c r="T38" s="178"/>
-      <c r="U38" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-5</v>
-      </c>
-      <c r="V38" s="179">
+      <c r="T38" s="171"/>
+      <c r="U38" s="85" t="s">
+        <v>473</v>
+      </c>
+      <c r="V38" s="172">
         <v>1</v>
       </c>
-      <c r="W38" s="178"/>
+      <c r="W38" s="171"/>
       <c r="X38" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y38" s="180"/>
-      <c r="Z38" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y38" s="173"/>
+      <c r="Z38" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA38" s="181">
+      <c r="AA38" s="174">
         <v>100</v>
       </c>
-      <c r="AB38" s="182"/>
-      <c r="AC38" s="185"/>
-      <c r="AD38" s="185"/>
-      <c r="AE38" s="186"/>
-      <c r="AF38" s="175"/>
-      <c r="AG38" s="176"/>
-      <c r="AH38" s="176"/>
+      <c r="AB38" s="175"/>
+      <c r="AC38" s="178"/>
+      <c r="AD38" s="178"/>
+      <c r="AE38" s="179"/>
+      <c r="AF38" s="168"/>
+      <c r="AG38" s="169"/>
+      <c r="AH38" s="169"/>
     </row>
     <row r="39" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="85" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="B39" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="172" t="s">
+      <c r="C39" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D39" s="87" t="s">
-        <v>494</v>
+      <c r="D39" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E39" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F39" s="88" t="s">
         <v>120</v>
@@ -33417,23 +33317,23 @@
       <c r="G39" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H39" s="190" t="s">
+      <c r="H39" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I39" s="173" t="s">
+      <c r="I39" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J39" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K39" s="174" t="s">
+      <c r="K39" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L39" s="175"/>
-      <c r="M39" s="176"/>
-      <c r="N39" s="177"/>
-      <c r="O39" s="175"/>
-      <c r="P39" s="173" t="s">
+      <c r="L39" s="168"/>
+      <c r="M39" s="169"/>
+      <c r="N39" s="170"/>
+      <c r="O39" s="168"/>
+      <c r="P39" s="166" t="s">
         <v>230</v>
       </c>
       <c r="Q39" s="89" t="s">
@@ -33441,32 +33341,31 @@
       </c>
       <c r="R39" s="99"/>
       <c r="S39" s="100"/>
-      <c r="T39" s="178"/>
-      <c r="U39" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-6</v>
-      </c>
-      <c r="V39" s="179">
+      <c r="T39" s="171"/>
+      <c r="U39" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="V39" s="172">
         <v>1</v>
       </c>
-      <c r="W39" s="178"/>
+      <c r="W39" s="171"/>
       <c r="X39" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y39" s="180"/>
-      <c r="Z39" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y39" s="173"/>
+      <c r="Z39" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA39" s="181">
+      <c r="AA39" s="174">
         <v>100</v>
       </c>
-      <c r="AB39" s="182"/>
-      <c r="AC39" s="185"/>
-      <c r="AD39" s="185"/>
-      <c r="AE39" s="186"/>
-      <c r="AF39" s="175"/>
-      <c r="AG39" s="176"/>
-      <c r="AH39" s="176"/>
+      <c r="AB39" s="175"/>
+      <c r="AC39" s="178"/>
+      <c r="AD39" s="178"/>
+      <c r="AE39" s="179"/>
+      <c r="AF39" s="168"/>
+      <c r="AG39" s="169"/>
+      <c r="AH39" s="169"/>
       <c r="AI39"/>
       <c r="AJ39"/>
       <c r="AK39"/>
@@ -34460,19 +34359,19 @@
     </row>
     <row r="40" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="85" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="B40" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="172" t="s">
+      <c r="C40" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="87" t="s">
-        <v>496</v>
+      <c r="D40" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E40" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F40" s="88" t="s">
         <v>120</v>
@@ -34480,23 +34379,23 @@
       <c r="G40" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H40" s="190" t="s">
+      <c r="H40" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I40" s="173" t="s">
+      <c r="I40" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J40" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K40" s="174" t="s">
+      <c r="K40" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L40" s="175"/>
-      <c r="M40" s="176"/>
-      <c r="N40" s="177"/>
-      <c r="O40" s="175"/>
-      <c r="P40" s="173" t="s">
+      <c r="L40" s="168"/>
+      <c r="M40" s="169"/>
+      <c r="N40" s="170"/>
+      <c r="O40" s="168"/>
+      <c r="P40" s="166" t="s">
         <v>234</v>
       </c>
       <c r="Q40" s="89" t="s">
@@ -34504,32 +34403,31 @@
       </c>
       <c r="R40" s="99"/>
       <c r="S40" s="100"/>
-      <c r="T40" s="178"/>
-      <c r="U40" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-7</v>
-      </c>
-      <c r="V40" s="179">
+      <c r="T40" s="171"/>
+      <c r="U40" s="85" t="s">
+        <v>475</v>
+      </c>
+      <c r="V40" s="172">
         <v>1</v>
       </c>
-      <c r="W40" s="178"/>
+      <c r="W40" s="171"/>
       <c r="X40" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y40" s="180"/>
-      <c r="Z40" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y40" s="173"/>
+      <c r="Z40" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA40" s="181">
+      <c r="AA40" s="174">
         <v>100</v>
       </c>
-      <c r="AB40" s="182"/>
-      <c r="AC40" s="185"/>
-      <c r="AD40" s="185"/>
-      <c r="AE40" s="186"/>
-      <c r="AF40" s="175"/>
-      <c r="AG40" s="176"/>
-      <c r="AH40" s="176"/>
+      <c r="AB40" s="175"/>
+      <c r="AC40" s="178"/>
+      <c r="AD40" s="178"/>
+      <c r="AE40" s="179"/>
+      <c r="AF40" s="168"/>
+      <c r="AG40" s="169"/>
+      <c r="AH40" s="169"/>
       <c r="AI40"/>
       <c r="AJ40"/>
       <c r="AK40"/>
@@ -35523,19 +35421,19 @@
     </row>
     <row r="41" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="85" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B41" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="172" t="s">
+      <c r="C41" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D41" s="87" t="s">
-        <v>498</v>
+      <c r="D41" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F41" s="88" t="s">
         <v>120</v>
@@ -35543,23 +35441,23 @@
       <c r="G41" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H41" s="190" t="s">
+      <c r="H41" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I41" s="173" t="s">
+      <c r="I41" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J41" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K41" s="174" t="s">
+      <c r="K41" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L41" s="175"/>
-      <c r="M41" s="176"/>
-      <c r="N41" s="177"/>
-      <c r="O41" s="175"/>
-      <c r="P41" s="173" t="s">
+      <c r="L41" s="168"/>
+      <c r="M41" s="169"/>
+      <c r="N41" s="170"/>
+      <c r="O41" s="168"/>
+      <c r="P41" s="166" t="s">
         <v>238</v>
       </c>
       <c r="Q41" s="89" t="s">
@@ -35567,32 +35465,31 @@
       </c>
       <c r="R41" s="99"/>
       <c r="S41" s="100"/>
-      <c r="T41" s="178"/>
-      <c r="U41" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-8</v>
-      </c>
-      <c r="V41" s="179">
+      <c r="T41" s="171"/>
+      <c r="U41" s="85" t="s">
+        <v>476</v>
+      </c>
+      <c r="V41" s="172">
         <v>1</v>
       </c>
-      <c r="W41" s="178"/>
+      <c r="W41" s="171"/>
       <c r="X41" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y41" s="180"/>
-      <c r="Z41" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y41" s="173"/>
+      <c r="Z41" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA41" s="181">
+      <c r="AA41" s="174">
         <v>100</v>
       </c>
-      <c r="AB41" s="182"/>
-      <c r="AC41" s="185"/>
-      <c r="AD41" s="185"/>
-      <c r="AE41" s="186"/>
-      <c r="AF41" s="175"/>
-      <c r="AG41" s="176"/>
-      <c r="AH41" s="176"/>
+      <c r="AB41" s="175"/>
+      <c r="AC41" s="178"/>
+      <c r="AD41" s="178"/>
+      <c r="AE41" s="179"/>
+      <c r="AF41" s="168"/>
+      <c r="AG41" s="169"/>
+      <c r="AH41" s="169"/>
       <c r="AI41"/>
       <c r="AJ41"/>
       <c r="AK41"/>
@@ -36586,19 +36483,19 @@
     </row>
     <row r="42" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="85" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="B42" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="172" t="s">
+      <c r="C42" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="87" t="s">
-        <v>500</v>
+      <c r="D42" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F42" s="88" t="s">
         <v>120</v>
@@ -36606,23 +36503,23 @@
       <c r="G42" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H42" s="190" t="s">
+      <c r="H42" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I42" s="173" t="s">
+      <c r="I42" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J42" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K42" s="174" t="s">
+      <c r="K42" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L42" s="175"/>
-      <c r="M42" s="176"/>
-      <c r="N42" s="177"/>
-      <c r="O42" s="175"/>
-      <c r="P42" s="173" t="s">
+      <c r="L42" s="168"/>
+      <c r="M42" s="169"/>
+      <c r="N42" s="170"/>
+      <c r="O42" s="168"/>
+      <c r="P42" s="166" t="s">
         <v>242</v>
       </c>
       <c r="Q42" s="89" t="s">
@@ -36630,32 +36527,31 @@
       </c>
       <c r="R42" s="99"/>
       <c r="S42" s="100"/>
-      <c r="T42" s="178"/>
-      <c r="U42" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-9</v>
-      </c>
-      <c r="V42" s="179">
+      <c r="T42" s="171"/>
+      <c r="U42" s="85" t="s">
+        <v>477</v>
+      </c>
+      <c r="V42" s="172">
         <v>1</v>
       </c>
-      <c r="W42" s="178"/>
+      <c r="W42" s="171"/>
       <c r="X42" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y42" s="180"/>
-      <c r="Z42" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y42" s="173"/>
+      <c r="Z42" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA42" s="181">
+      <c r="AA42" s="174">
         <v>100</v>
       </c>
-      <c r="AB42" s="182"/>
-      <c r="AC42" s="185"/>
-      <c r="AD42" s="185"/>
-      <c r="AE42" s="186"/>
-      <c r="AF42" s="175"/>
-      <c r="AG42" s="176"/>
-      <c r="AH42" s="176"/>
+      <c r="AB42" s="175"/>
+      <c r="AC42" s="178"/>
+      <c r="AD42" s="178"/>
+      <c r="AE42" s="179"/>
+      <c r="AF42" s="168"/>
+      <c r="AG42" s="169"/>
+      <c r="AH42" s="169"/>
       <c r="AI42"/>
       <c r="AJ42"/>
       <c r="AK42"/>
@@ -37649,19 +37545,19 @@
     </row>
     <row r="43" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="85" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="B43" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="172" t="s">
+      <c r="C43" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="87" t="s">
-        <v>502</v>
+      <c r="D43" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E43" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F43" s="88" t="s">
         <v>120</v>
@@ -37669,23 +37565,23 @@
       <c r="G43" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H43" s="190" t="s">
+      <c r="H43" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I43" s="173" t="s">
+      <c r="I43" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J43" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K43" s="174" t="s">
+      <c r="K43" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L43" s="175"/>
-      <c r="M43" s="176"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="175"/>
-      <c r="P43" s="173" t="s">
+      <c r="L43" s="168"/>
+      <c r="M43" s="169"/>
+      <c r="N43" s="170"/>
+      <c r="O43" s="168"/>
+      <c r="P43" s="166" t="s">
         <v>246</v>
       </c>
       <c r="Q43" s="89" t="s">
@@ -37693,32 +37589,31 @@
       </c>
       <c r="R43" s="99"/>
       <c r="S43" s="100"/>
-      <c r="T43" s="178"/>
-      <c r="U43" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-10</v>
-      </c>
-      <c r="V43" s="179">
+      <c r="T43" s="171"/>
+      <c r="U43" s="85" t="s">
+        <v>478</v>
+      </c>
+      <c r="V43" s="172">
         <v>1</v>
       </c>
-      <c r="W43" s="178"/>
+      <c r="W43" s="171"/>
       <c r="X43" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y43" s="180"/>
-      <c r="Z43" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y43" s="173"/>
+      <c r="Z43" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA43" s="181">
+      <c r="AA43" s="174">
         <v>100</v>
       </c>
-      <c r="AB43" s="182"/>
-      <c r="AC43" s="185"/>
-      <c r="AD43" s="185"/>
-      <c r="AE43" s="186"/>
-      <c r="AF43" s="175"/>
-      <c r="AG43" s="176"/>
-      <c r="AH43" s="176"/>
+      <c r="AB43" s="175"/>
+      <c r="AC43" s="178"/>
+      <c r="AD43" s="178"/>
+      <c r="AE43" s="179"/>
+      <c r="AF43" s="168"/>
+      <c r="AG43" s="169"/>
+      <c r="AH43" s="169"/>
       <c r="AI43"/>
       <c r="AJ43"/>
       <c r="AK43"/>
@@ -38712,19 +38607,19 @@
     </row>
     <row r="44" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="85" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="B44" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="172" t="s">
+      <c r="C44" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="87" t="s">
-        <v>504</v>
+      <c r="D44" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E44" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F44" s="88" t="s">
         <v>120</v>
@@ -38732,23 +38627,23 @@
       <c r="G44" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H44" s="190" t="s">
+      <c r="H44" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I44" s="173" t="s">
+      <c r="I44" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J44" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K44" s="174" t="s">
+      <c r="K44" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L44" s="175"/>
-      <c r="M44" s="176"/>
-      <c r="N44" s="177"/>
-      <c r="O44" s="175"/>
-      <c r="P44" s="173" t="s">
+      <c r="L44" s="168"/>
+      <c r="M44" s="169"/>
+      <c r="N44" s="170"/>
+      <c r="O44" s="168"/>
+      <c r="P44" s="166" t="s">
         <v>250</v>
       </c>
       <c r="Q44" s="89" t="s">
@@ -38756,32 +38651,31 @@
       </c>
       <c r="R44" s="99"/>
       <c r="S44" s="100"/>
-      <c r="T44" s="178"/>
-      <c r="U44" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-11</v>
-      </c>
-      <c r="V44" s="179">
+      <c r="T44" s="171"/>
+      <c r="U44" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="V44" s="172">
         <v>1</v>
       </c>
-      <c r="W44" s="178"/>
+      <c r="W44" s="171"/>
       <c r="X44" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y44" s="180"/>
-      <c r="Z44" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y44" s="173"/>
+      <c r="Z44" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA44" s="181">
+      <c r="AA44" s="174">
         <v>100</v>
       </c>
-      <c r="AB44" s="182"/>
-      <c r="AC44" s="185"/>
-      <c r="AD44" s="185"/>
-      <c r="AE44" s="186"/>
-      <c r="AF44" s="175"/>
-      <c r="AG44" s="176"/>
-      <c r="AH44" s="176"/>
+      <c r="AB44" s="175"/>
+      <c r="AC44" s="178"/>
+      <c r="AD44" s="178"/>
+      <c r="AE44" s="179"/>
+      <c r="AF44" s="168"/>
+      <c r="AG44" s="169"/>
+      <c r="AH44" s="169"/>
       <c r="AI44"/>
       <c r="AJ44"/>
       <c r="AK44"/>
@@ -39775,19 +39669,19 @@
     </row>
     <row r="45" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="85" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="B45" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="172" t="s">
+      <c r="C45" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D45" s="87" t="s">
-        <v>267</v>
+      <c r="D45" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E45" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F45" s="88" t="s">
         <v>120</v>
@@ -39795,23 +39689,23 @@
       <c r="G45" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H45" s="190" t="s">
+      <c r="H45" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I45" s="173" t="s">
+      <c r="I45" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J45" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K45" s="174" t="s">
+      <c r="K45" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L45" s="175"/>
-      <c r="M45" s="176"/>
-      <c r="N45" s="177"/>
-      <c r="O45" s="175"/>
-      <c r="P45" s="173" t="s">
+      <c r="L45" s="168"/>
+      <c r="M45" s="169"/>
+      <c r="N45" s="170"/>
+      <c r="O45" s="168"/>
+      <c r="P45" s="166" t="s">
         <v>254</v>
       </c>
       <c r="Q45" s="89" t="s">
@@ -39819,30 +39713,29 @@
       </c>
       <c r="R45" s="99"/>
       <c r="S45" s="100"/>
-      <c r="T45" s="178"/>
-      <c r="U45" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-1</v>
-      </c>
-      <c r="V45" s="179">
+      <c r="T45" s="171"/>
+      <c r="U45" s="85" t="s">
+        <v>480</v>
+      </c>
+      <c r="V45" s="172">
         <v>1</v>
       </c>
-      <c r="W45" s="178"/>
+      <c r="W45" s="171"/>
       <c r="X45" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y45" s="180"/>
-      <c r="Z45" s="184"/>
-      <c r="AA45" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y45" s="173"/>
+      <c r="Z45" s="177"/>
+      <c r="AA45" s="174">
         <v>100</v>
       </c>
-      <c r="AB45" s="182"/>
-      <c r="AC45" s="185"/>
-      <c r="AD45" s="185"/>
-      <c r="AE45" s="186"/>
-      <c r="AF45" s="175"/>
-      <c r="AG45" s="176"/>
-      <c r="AH45" s="176"/>
+      <c r="AB45" s="175"/>
+      <c r="AC45" s="178"/>
+      <c r="AD45" s="178"/>
+      <c r="AE45" s="179"/>
+      <c r="AF45" s="168"/>
+      <c r="AG45" s="169"/>
+      <c r="AH45" s="169"/>
       <c r="AI45"/>
       <c r="AJ45"/>
       <c r="AK45"/>
@@ -40836,19 +40729,19 @@
     </row>
     <row r="46" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="85" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="B46" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="172" t="s">
+      <c r="C46" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D46" s="87" t="s">
-        <v>271</v>
+      <c r="D46" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E46" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F46" s="88" t="s">
         <v>120</v>
@@ -40856,23 +40749,23 @@
       <c r="G46" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H46" s="190" t="s">
+      <c r="H46" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I46" s="173" t="s">
+      <c r="I46" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J46" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K46" s="174" t="s">
+      <c r="K46" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L46" s="175"/>
-      <c r="M46" s="176"/>
-      <c r="N46" s="177"/>
-      <c r="O46" s="175"/>
-      <c r="P46" s="173" t="s">
+      <c r="L46" s="168"/>
+      <c r="M46" s="169"/>
+      <c r="N46" s="170"/>
+      <c r="O46" s="168"/>
+      <c r="P46" s="166" t="s">
         <v>258</v>
       </c>
       <c r="Q46" s="89" t="s">
@@ -40880,30 +40773,29 @@
       </c>
       <c r="R46" s="99"/>
       <c r="S46" s="100"/>
-      <c r="T46" s="178"/>
-      <c r="U46" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-2</v>
-      </c>
-      <c r="V46" s="179">
+      <c r="T46" s="171"/>
+      <c r="U46" s="85" t="s">
+        <v>481</v>
+      </c>
+      <c r="V46" s="172">
         <v>1</v>
       </c>
-      <c r="W46" s="178"/>
+      <c r="W46" s="171"/>
       <c r="X46" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y46" s="180"/>
-      <c r="Z46" s="184"/>
-      <c r="AA46" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y46" s="173"/>
+      <c r="Z46" s="177"/>
+      <c r="AA46" s="174">
         <v>100</v>
       </c>
-      <c r="AB46" s="182"/>
-      <c r="AC46" s="185"/>
-      <c r="AD46" s="185"/>
-      <c r="AE46" s="186"/>
-      <c r="AF46" s="175"/>
-      <c r="AG46" s="176"/>
-      <c r="AH46" s="176"/>
+      <c r="AB46" s="175"/>
+      <c r="AC46" s="178"/>
+      <c r="AD46" s="178"/>
+      <c r="AE46" s="179"/>
+      <c r="AF46" s="168"/>
+      <c r="AG46" s="169"/>
+      <c r="AH46" s="169"/>
       <c r="AI46"/>
       <c r="AJ46"/>
       <c r="AK46"/>
@@ -41897,19 +41789,19 @@
     </row>
     <row r="47" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="85" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
       <c r="B47" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="172" t="s">
+      <c r="C47" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="87" t="s">
-        <v>275</v>
+      <c r="D47" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F47" s="88" t="s">
         <v>120</v>
@@ -41917,23 +41809,23 @@
       <c r="G47" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H47" s="190" t="s">
+      <c r="H47" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I47" s="173" t="s">
+      <c r="I47" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J47" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K47" s="174" t="s">
+      <c r="K47" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L47" s="175"/>
-      <c r="M47" s="176"/>
-      <c r="N47" s="177"/>
-      <c r="O47" s="175"/>
-      <c r="P47" s="173" t="s">
+      <c r="L47" s="168"/>
+      <c r="M47" s="169"/>
+      <c r="N47" s="170"/>
+      <c r="O47" s="168"/>
+      <c r="P47" s="166" t="s">
         <v>262</v>
       </c>
       <c r="Q47" s="89" t="s">
@@ -41941,30 +41833,29 @@
       </c>
       <c r="R47" s="99"/>
       <c r="S47" s="100"/>
-      <c r="T47" s="178"/>
-      <c r="U47" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-3</v>
-      </c>
-      <c r="V47" s="179">
+      <c r="T47" s="171"/>
+      <c r="U47" s="85" t="s">
+        <v>482</v>
+      </c>
+      <c r="V47" s="172">
         <v>1</v>
       </c>
-      <c r="W47" s="178"/>
+      <c r="W47" s="171"/>
       <c r="X47" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y47" s="180"/>
-      <c r="Z47" s="184"/>
-      <c r="AA47" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y47" s="173"/>
+      <c r="Z47" s="177"/>
+      <c r="AA47" s="174">
         <v>100</v>
       </c>
-      <c r="AB47" s="182"/>
-      <c r="AC47" s="185"/>
-      <c r="AD47" s="185"/>
-      <c r="AE47" s="186"/>
-      <c r="AF47" s="175"/>
-      <c r="AG47" s="176"/>
-      <c r="AH47" s="176"/>
+      <c r="AB47" s="175"/>
+      <c r="AC47" s="178"/>
+      <c r="AD47" s="178"/>
+      <c r="AE47" s="179"/>
+      <c r="AF47" s="168"/>
+      <c r="AG47" s="169"/>
+      <c r="AH47" s="169"/>
       <c r="AI47"/>
       <c r="AJ47"/>
       <c r="AK47"/>
@@ -42958,19 +42849,19 @@
     </row>
     <row r="48" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="85" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="B48" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="172" t="s">
+      <c r="C48" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="87" t="s">
-        <v>279</v>
+      <c r="D48" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E48" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F48" s="88" t="s">
         <v>120</v>
@@ -42978,23 +42869,23 @@
       <c r="G48" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H48" s="190" t="s">
+      <c r="H48" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I48" s="173" t="s">
+      <c r="I48" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J48" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K48" s="174" t="s">
+      <c r="K48" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L48" s="175"/>
-      <c r="M48" s="176"/>
-      <c r="N48" s="177"/>
-      <c r="O48" s="175"/>
-      <c r="P48" s="173" t="s">
+      <c r="L48" s="168"/>
+      <c r="M48" s="169"/>
+      <c r="N48" s="170"/>
+      <c r="O48" s="168"/>
+      <c r="P48" s="166" t="s">
         <v>266</v>
       </c>
       <c r="Q48" s="89" t="s">
@@ -43002,30 +42893,29 @@
       </c>
       <c r="R48" s="99"/>
       <c r="S48" s="100"/>
-      <c r="T48" s="178"/>
-      <c r="U48" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-4</v>
-      </c>
-      <c r="V48" s="179">
+      <c r="T48" s="171"/>
+      <c r="U48" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="V48" s="172">
         <v>1</v>
       </c>
-      <c r="W48" s="178"/>
+      <c r="W48" s="171"/>
       <c r="X48" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y48" s="180"/>
-      <c r="Z48" s="184"/>
-      <c r="AA48" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y48" s="173"/>
+      <c r="Z48" s="177"/>
+      <c r="AA48" s="174">
         <v>100</v>
       </c>
-      <c r="AB48" s="182"/>
-      <c r="AC48" s="185"/>
-      <c r="AD48" s="185"/>
-      <c r="AE48" s="186"/>
-      <c r="AF48" s="175"/>
-      <c r="AG48" s="176"/>
-      <c r="AH48" s="176"/>
+      <c r="AB48" s="175"/>
+      <c r="AC48" s="178"/>
+      <c r="AD48" s="178"/>
+      <c r="AE48" s="179"/>
+      <c r="AF48" s="168"/>
+      <c r="AG48" s="169"/>
+      <c r="AH48" s="169"/>
       <c r="AI48"/>
       <c r="AJ48"/>
       <c r="AK48"/>
@@ -44019,19 +43909,19 @@
     </row>
     <row r="49" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="85" t="s">
-        <v>510</v>
+        <v>484</v>
       </c>
       <c r="B49" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="172" t="s">
+      <c r="C49" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D49" s="87" t="s">
-        <v>283</v>
+      <c r="D49" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E49" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F49" s="88" t="s">
         <v>120</v>
@@ -44039,23 +43929,23 @@
       <c r="G49" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H49" s="190" t="s">
+      <c r="H49" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I49" s="173" t="s">
+      <c r="I49" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J49" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K49" s="174" t="s">
+      <c r="K49" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L49" s="175"/>
-      <c r="M49" s="176"/>
-      <c r="N49" s="177"/>
-      <c r="O49" s="175"/>
-      <c r="P49" s="173" t="s">
+      <c r="L49" s="168"/>
+      <c r="M49" s="169"/>
+      <c r="N49" s="170"/>
+      <c r="O49" s="168"/>
+      <c r="P49" s="166" t="s">
         <v>270</v>
       </c>
       <c r="Q49" s="89" t="s">
@@ -44063,30 +43953,29 @@
       </c>
       <c r="R49" s="99"/>
       <c r="S49" s="100"/>
-      <c r="T49" s="178"/>
-      <c r="U49" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-5</v>
-      </c>
-      <c r="V49" s="179">
+      <c r="T49" s="171"/>
+      <c r="U49" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="V49" s="172">
         <v>1</v>
       </c>
-      <c r="W49" s="178"/>
+      <c r="W49" s="171"/>
       <c r="X49" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y49" s="180"/>
-      <c r="Z49" s="184"/>
-      <c r="AA49" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y49" s="173"/>
+      <c r="Z49" s="177"/>
+      <c r="AA49" s="174">
         <v>100</v>
       </c>
-      <c r="AB49" s="182"/>
-      <c r="AC49" s="185"/>
-      <c r="AD49" s="185"/>
-      <c r="AE49" s="186"/>
-      <c r="AF49" s="175"/>
-      <c r="AG49" s="176"/>
-      <c r="AH49" s="176"/>
+      <c r="AB49" s="175"/>
+      <c r="AC49" s="178"/>
+      <c r="AD49" s="178"/>
+      <c r="AE49" s="179"/>
+      <c r="AF49" s="168"/>
+      <c r="AG49" s="169"/>
+      <c r="AH49" s="169"/>
       <c r="AI49"/>
       <c r="AJ49"/>
       <c r="AK49"/>
@@ -45079,20 +44968,20 @@
       <c r="AMJ49"/>
     </row>
     <row r="50" spans="1:1024" s="107" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="106" t="s">
-        <v>511</v>
+      <c r="A50" s="85" t="s">
+        <v>485</v>
       </c>
       <c r="B50" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="172" t="s">
+      <c r="C50" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="87" t="s">
-        <v>107</v>
+      <c r="D50" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E50" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F50" s="88" t="s">
         <v>120</v>
@@ -45100,23 +44989,23 @@
       <c r="G50" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H50" s="190" t="s">
+      <c r="H50" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I50" s="173" t="s">
+      <c r="I50" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J50" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K50" s="174" t="s">
+      <c r="K50" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L50" s="175"/>
-      <c r="M50" s="176"/>
-      <c r="N50" s="177"/>
-      <c r="O50" s="175"/>
-      <c r="P50" s="173" t="s">
+      <c r="L50" s="168"/>
+      <c r="M50" s="169"/>
+      <c r="N50" s="170"/>
+      <c r="O50" s="168"/>
+      <c r="P50" s="166" t="s">
         <v>274</v>
       </c>
       <c r="Q50" s="89" t="s">
@@ -45124,46 +45013,45 @@
       </c>
       <c r="R50" s="99"/>
       <c r="S50" s="100"/>
-      <c r="T50" s="178"/>
-      <c r="U50" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-1</v>
-      </c>
-      <c r="V50" s="179">
+      <c r="T50" s="171"/>
+      <c r="U50" s="85" t="s">
+        <v>485</v>
+      </c>
+      <c r="V50" s="172">
         <v>1</v>
       </c>
-      <c r="W50" s="178"/>
+      <c r="W50" s="171"/>
       <c r="X50" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y50" s="180"/>
-      <c r="Z50" s="184"/>
-      <c r="AA50" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y50" s="173"/>
+      <c r="Z50" s="177"/>
+      <c r="AA50" s="174">
         <v>100</v>
       </c>
-      <c r="AB50" s="182"/>
-      <c r="AC50" s="185"/>
-      <c r="AD50" s="185"/>
-      <c r="AE50" s="186"/>
-      <c r="AF50" s="175"/>
-      <c r="AG50" s="176"/>
-      <c r="AH50" s="176"/>
+      <c r="AB50" s="175"/>
+      <c r="AC50" s="178"/>
+      <c r="AD50" s="178"/>
+      <c r="AE50" s="179"/>
+      <c r="AF50" s="168"/>
+      <c r="AG50" s="169"/>
+      <c r="AH50" s="169"/>
     </row>
     <row r="51" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="106" t="s">
-        <v>513</v>
+      <c r="A51" s="85" t="s">
+        <v>486</v>
       </c>
       <c r="B51" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="172" t="s">
+      <c r="C51" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D51" s="87" t="s">
-        <v>107</v>
+      <c r="D51" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E51" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F51" s="88" t="s">
         <v>120</v>
@@ -45171,23 +45059,23 @@
       <c r="G51" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H51" s="190" t="s">
+      <c r="H51" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I51" s="173" t="s">
+      <c r="I51" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J51" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K51" s="174" t="s">
+      <c r="K51" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L51" s="175"/>
-      <c r="M51" s="176"/>
-      <c r="N51" s="177"/>
-      <c r="O51" s="175"/>
-      <c r="P51" s="188" t="s">
+      <c r="L51" s="168"/>
+      <c r="M51" s="169"/>
+      <c r="N51" s="170"/>
+      <c r="O51" s="168"/>
+      <c r="P51" s="180" t="s">
         <v>278</v>
       </c>
       <c r="Q51" s="89" t="s">
@@ -45195,30 +45083,29 @@
       </c>
       <c r="R51" s="99"/>
       <c r="S51" s="100"/>
-      <c r="T51" s="178"/>
-      <c r="U51" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-2</v>
-      </c>
-      <c r="V51" s="179">
+      <c r="T51" s="171"/>
+      <c r="U51" s="85" t="s">
+        <v>486</v>
+      </c>
+      <c r="V51" s="172">
         <v>1</v>
       </c>
-      <c r="W51" s="178"/>
+      <c r="W51" s="171"/>
       <c r="X51" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y51" s="180"/>
-      <c r="Z51" s="184"/>
-      <c r="AA51" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y51" s="173"/>
+      <c r="Z51" s="177"/>
+      <c r="AA51" s="174">
         <v>100</v>
       </c>
-      <c r="AB51" s="182"/>
-      <c r="AC51" s="185"/>
-      <c r="AD51" s="185"/>
-      <c r="AE51" s="186"/>
-      <c r="AF51" s="175"/>
-      <c r="AG51" s="176"/>
-      <c r="AH51" s="176"/>
+      <c r="AB51" s="175"/>
+      <c r="AC51" s="178"/>
+      <c r="AD51" s="178"/>
+      <c r="AE51" s="179"/>
+      <c r="AF51" s="168"/>
+      <c r="AG51" s="169"/>
+      <c r="AH51" s="169"/>
       <c r="AI51"/>
       <c r="AJ51"/>
       <c r="AK51"/>
@@ -46211,20 +46098,20 @@
       <c r="AMJ51"/>
     </row>
     <row r="52" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="106" t="s">
-        <v>514</v>
+      <c r="A52" s="85" t="s">
+        <v>487</v>
       </c>
       <c r="B52" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="172" t="s">
+      <c r="C52" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="87" t="s">
-        <v>107</v>
+      <c r="D52" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E52" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F52" s="88" t="s">
         <v>120</v>
@@ -46232,23 +46119,23 @@
       <c r="G52" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H52" s="190" t="s">
+      <c r="H52" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I52" s="173" t="s">
+      <c r="I52" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J52" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K52" s="174" t="s">
+      <c r="K52" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L52" s="175"/>
-      <c r="M52" s="176"/>
-      <c r="N52" s="177"/>
-      <c r="O52" s="175"/>
-      <c r="P52" s="191" t="s">
+      <c r="L52" s="168"/>
+      <c r="M52" s="169"/>
+      <c r="N52" s="170"/>
+      <c r="O52" s="168"/>
+      <c r="P52" s="183" t="s">
         <v>282</v>
       </c>
       <c r="Q52" s="89" t="s">
@@ -46256,30 +46143,29 @@
       </c>
       <c r="R52" s="99"/>
       <c r="S52" s="100"/>
-      <c r="T52" s="178"/>
-      <c r="U52" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-3</v>
-      </c>
-      <c r="V52" s="179">
+      <c r="T52" s="171"/>
+      <c r="U52" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="V52" s="172">
         <v>1</v>
       </c>
-      <c r="W52" s="178"/>
+      <c r="W52" s="171"/>
       <c r="X52" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y52" s="180"/>
-      <c r="Z52" s="184"/>
-      <c r="AA52" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y52" s="173"/>
+      <c r="Z52" s="177"/>
+      <c r="AA52" s="174">
         <v>100</v>
       </c>
-      <c r="AB52" s="182"/>
-      <c r="AC52" s="185"/>
-      <c r="AD52" s="185"/>
-      <c r="AE52" s="186"/>
-      <c r="AF52" s="175"/>
-      <c r="AG52" s="176"/>
-      <c r="AH52" s="176"/>
+      <c r="AB52" s="175"/>
+      <c r="AC52" s="178"/>
+      <c r="AD52" s="178"/>
+      <c r="AE52" s="179"/>
+      <c r="AF52" s="168"/>
+      <c r="AG52" s="169"/>
+      <c r="AH52" s="169"/>
       <c r="AI52"/>
       <c r="AJ52"/>
       <c r="AK52"/>
@@ -69502,6 +69388,7 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="Z9:AA9"/>
   </mergeCells>
+  <phoneticPr fontId="48" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L53:L394" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
@@ -69523,7 +69410,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="20">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -69624,25 +69511,7 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C15:C52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{428E6055-04A8-6C4C-89A7-EF7F7D8D6474}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>V15:V52 N15:N17 AE17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF8CDC01-B85F-E14A-8E02-465A52BD9AAC}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AE18:AE52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22E74F9B-E324-7B45-A9DA-64F55B2673AF}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>N18:N52</xm:sqref>
+          <xm:sqref>C15:C52 V15:V52 N15:N52 AE17:AE52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -69658,7 +69527,7 @@
   <dimension ref="A1:AL103"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C37" sqref="C37:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Simplify (OP/OF): Show only wts applications for rna orders (#444)
* Create change_prep_category_on_rna_applications.sql

* use only wts applications in rna test

* Update 1508.19.mip_rna.xlsx
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
+++ b/tests/fixtures/orderforms/1508.19.mip_rna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AA3D19-29D8-D249-A98C-0B0B8D983E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5ABF3D-3D10-D142-93C8-32D533CD07C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="23860" windowHeight="25900" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13000" yWindow="460" windowWidth="35700" windowHeight="25000" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="488">
   <si>
     <t>Document name</t>
   </si>
@@ -1920,19 +1920,7 @@
     <t>Emilia Ottosson Laakso</t>
   </si>
   <si>
-    <t>whole-genome-1</t>
-  </si>
-  <si>
-    <t>whole-genome</t>
-  </si>
-  <si>
     <t>plate</t>
-  </si>
-  <si>
-    <t>whole-genome-2</t>
-  </si>
-  <si>
-    <t>whole-genome-3</t>
   </si>
   <si>
     <t>LymphoMATIC</t>
@@ -1953,13 +1941,7 @@
     <t>GMCKsolid</t>
   </si>
   <si>
-    <t>whole-genome-4</t>
-  </si>
-  <si>
     <t>GMSmyeloid</t>
-  </si>
-  <si>
-    <t>whole-genome-5</t>
   </si>
   <si>
     <t>other (specify in comment field)</t>
@@ -1968,157 +1950,7 @@
     <t>Other bait set</t>
   </si>
   <si>
-    <t>whole-genome-6</t>
-  </si>
-  <si>
-    <t>whole-genome-7</t>
-  </si>
-  <si>
-    <t>whole-exome-1</t>
-  </si>
-  <si>
-    <t>EXOTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome</t>
-  </si>
-  <si>
-    <t>whole-exome-2</t>
-  </si>
-  <si>
-    <t>EXOTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-3</t>
-  </si>
-  <si>
-    <t>EXOTTTR060</t>
-  </si>
-  <si>
-    <t>whole-exome-4</t>
-  </si>
-  <si>
-    <t>EXOTTTR080</t>
-  </si>
-  <si>
     <t>Other Elution buffer</t>
-  </si>
-  <si>
-    <t>whole-exome-5</t>
-  </si>
-  <si>
-    <t>EXOTTTR100</t>
-  </si>
-  <si>
-    <t>whole-exome-6</t>
-  </si>
-  <si>
-    <t>EXOTTTR120</t>
-  </si>
-  <si>
-    <t>whole-exome-7</t>
-  </si>
-  <si>
-    <t>EXOTTTR140</t>
-  </si>
-  <si>
-    <t>whole-exome-8</t>
-  </si>
-  <si>
-    <t>EXTTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome-9</t>
-  </si>
-  <si>
-    <t>EXTTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-10</t>
-  </si>
-  <si>
-    <t>EXLTTTR020</t>
-  </si>
-  <si>
-    <t>whole-exome-11</t>
-  </si>
-  <si>
-    <t>EXLTTTR040</t>
-  </si>
-  <si>
-    <t>whole-exome-12</t>
-  </si>
-  <si>
-    <t>EXLTTTR060</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-1</t>
-  </si>
-  <si>
-    <t>EXLTTTR080</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-2</t>
-  </si>
-  <si>
-    <t>PANTTTR010</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-3</t>
-  </si>
-  <si>
-    <t>PANTTTR020</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-4</t>
-  </si>
-  <si>
-    <t>PANTTTR030</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-5</t>
-  </si>
-  <si>
-    <t>PANTTTR040</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-6</t>
-  </si>
-  <si>
-    <t>PANTTTR050</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-7</t>
-  </si>
-  <si>
-    <t>PALTTTR010</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-8</t>
-  </si>
-  <si>
-    <t>PALTTTR020</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-9</t>
-  </si>
-  <si>
-    <t>PALTTTR030</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-10</t>
-  </si>
-  <si>
-    <t>PALTTTR040</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-11</t>
-  </si>
-  <si>
-    <t>PALTTTR050</t>
   </si>
   <si>
     <t>rna-1</t>
@@ -2139,16 +1971,103 @@
     <t>rna-5</t>
   </si>
   <si>
-    <t>gene-list-test-1</t>
+    <t>rna-6</t>
   </si>
   <si>
-    <t>gene-list-test</t>
+    <t>rna-7</t>
   </si>
   <si>
-    <t>gene-list-test-2</t>
+    <t>rna-8</t>
   </si>
   <si>
-    <t>gene-list-test-3</t>
+    <t>rna-9</t>
+  </si>
+  <si>
+    <t>rna-10</t>
+  </si>
+  <si>
+    <t>rna-11</t>
+  </si>
+  <si>
+    <t>rna-12</t>
+  </si>
+  <si>
+    <t>rna-13</t>
+  </si>
+  <si>
+    <t>rna-14</t>
+  </si>
+  <si>
+    <t>rna-15</t>
+  </si>
+  <si>
+    <t>rna-16</t>
+  </si>
+  <si>
+    <t>rna-17</t>
+  </si>
+  <si>
+    <t>rna-18</t>
+  </si>
+  <si>
+    <t>rna-19</t>
+  </si>
+  <si>
+    <t>rna-20</t>
+  </si>
+  <si>
+    <t>rna-21</t>
+  </si>
+  <si>
+    <t>rna-22</t>
+  </si>
+  <si>
+    <t>rna-23</t>
+  </si>
+  <si>
+    <t>rna-24</t>
+  </si>
+  <si>
+    <t>rna-25</t>
+  </si>
+  <si>
+    <t>rna-26</t>
+  </si>
+  <si>
+    <t>rna-27</t>
+  </si>
+  <si>
+    <t>rna-28</t>
+  </si>
+  <si>
+    <t>rna-29</t>
+  </si>
+  <si>
+    <t>rna-30</t>
+  </si>
+  <si>
+    <t>rna-31</t>
+  </si>
+  <si>
+    <t>rna-32</t>
+  </si>
+  <si>
+    <t>rna-33</t>
+  </si>
+  <si>
+    <t>rna-34</t>
+  </si>
+  <si>
+    <t>rna-35</t>
+  </si>
+  <si>
+    <t>rna-36</t>
+  </si>
+  <si>
+    <t>rna-37</t>
+  </si>
+  <si>
+    <t>rna-38</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2078,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="48" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2478,6 +2397,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -2794,7 +2719,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3252,27 +3177,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3326,10 +3230,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="36" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -3341,6 +3241,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -4226,8 +4147,8 @@
   </sheetPr>
   <dimension ref="A1:AMK395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:AH52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -10499,56 +10420,56 @@
       <c r="AH8" s="42"/>
     </row>
     <row r="9" spans="1:1024" s="48" customFormat="1" ht="22" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="167" t="s">
+      <c r="A9" s="186" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="167"/>
-      <c r="C9" s="167"/>
-      <c r="D9" s="167"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="167"/>
-      <c r="G9" s="167"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="167"/>
-      <c r="K9" s="167"/>
+      <c r="B9" s="186"/>
+      <c r="C9" s="186"/>
+      <c r="D9" s="186"/>
+      <c r="E9" s="186"/>
+      <c r="F9" s="186"/>
+      <c r="G9" s="186"/>
+      <c r="H9" s="186"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="186"/>
       <c r="L9" s="44"/>
-      <c r="M9" s="168" t="s">
+      <c r="M9" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="168"/>
+      <c r="N9" s="187"/>
       <c r="O9" s="159"/>
-      <c r="P9" s="169" t="s">
+      <c r="P9" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="Q9" s="169"/>
-      <c r="R9" s="169"/>
-      <c r="S9" s="169"/>
+      <c r="Q9" s="188"/>
+      <c r="R9" s="188"/>
+      <c r="S9" s="188"/>
       <c r="T9" s="45"/>
-      <c r="U9" s="170" t="s">
+      <c r="U9" s="189" t="s">
         <v>27</v>
       </c>
-      <c r="V9" s="170"/>
+      <c r="V9" s="189"/>
       <c r="W9" s="45"/>
       <c r="X9" s="46" t="s">
         <v>28</v>
       </c>
       <c r="Y9" s="47"/>
-      <c r="Z9" s="171" t="s">
+      <c r="Z9" s="190" t="s">
         <v>29</v>
       </c>
-      <c r="AA9" s="171"/>
+      <c r="AA9" s="190"/>
       <c r="AB9" s="47"/>
-      <c r="AC9" s="165" t="s">
+      <c r="AC9" s="184" t="s">
         <v>30</v>
       </c>
-      <c r="AD9" s="165"/>
-      <c r="AE9" s="165"/>
+      <c r="AD9" s="184"/>
+      <c r="AE9" s="184"/>
       <c r="AF9" s="45"/>
-      <c r="AG9" s="166" t="s">
+      <c r="AG9" s="185" t="s">
         <v>18</v>
       </c>
-      <c r="AH9" s="166"/>
+      <c r="AH9" s="185"/>
     </row>
     <row r="10" spans="1:1024" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="49" t="s">
@@ -11836,19 +11757,19 @@
     </row>
     <row r="15" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="85" t="s">
-        <v>438</v>
+        <v>449</v>
       </c>
       <c r="B15" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="172" t="s">
+      <c r="C15" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D15" s="87" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="E15" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F15" s="88" t="s">
         <v>95</v>
@@ -11856,72 +11777,72 @@
       <c r="G15" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="173" t="s">
+      <c r="H15" s="166" t="s">
         <v>98</v>
       </c>
-      <c r="I15" s="173" t="s">
+      <c r="I15" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J15" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="K15" s="174" t="s">
+      <c r="K15" s="167" t="s">
         <v>92</v>
       </c>
-      <c r="L15" s="175"/>
-      <c r="M15" s="176" t="s">
-        <v>440</v>
-      </c>
-      <c r="N15" s="177" t="s">
+      <c r="L15" s="168"/>
+      <c r="M15" s="169" t="s">
+        <v>438</v>
+      </c>
+      <c r="N15" s="170" t="s">
         <v>102</v>
       </c>
-      <c r="O15" s="175"/>
-      <c r="P15" s="173" t="s">
+      <c r="O15" s="168"/>
+      <c r="P15" s="166" t="s">
         <v>103</v>
       </c>
       <c r="Q15" s="89" t="s">
         <v>100</v>
       </c>
       <c r="R15" s="85" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="S15" s="94" t="s">
-        <v>442</v>
-      </c>
-      <c r="T15" s="178"/>
+        <v>452</v>
+      </c>
+      <c r="T15" s="171"/>
       <c r="U15" s="85" t="s">
-        <v>438</v>
-      </c>
-      <c r="V15" s="179">
+        <v>449</v>
+      </c>
+      <c r="V15" s="172">
         <v>1</v>
       </c>
-      <c r="W15" s="178"/>
+      <c r="W15" s="171"/>
       <c r="X15" s="112" t="s">
-        <v>443</v>
-      </c>
-      <c r="Y15" s="180"/>
+        <v>439</v>
+      </c>
+      <c r="Y15" s="173"/>
       <c r="Z15" s="96" t="s">
-        <v>444</v>
-      </c>
-      <c r="AA15" s="181">
+        <v>440</v>
+      </c>
+      <c r="AA15" s="174">
         <v>5</v>
       </c>
-      <c r="AB15" s="182"/>
-      <c r="AC15" s="183">
+      <c r="AB15" s="175"/>
+      <c r="AC15" s="176">
         <v>1</v>
       </c>
-      <c r="AD15" s="183">
+      <c r="AD15" s="176">
         <v>2</v>
       </c>
       <c r="AE15" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="AF15" s="175"/>
-      <c r="AG15" s="176" t="s">
-        <v>445</v>
-      </c>
-      <c r="AH15" s="176" t="s">
-        <v>446</v>
+      <c r="AF15" s="168"/>
+      <c r="AG15" s="169" t="s">
+        <v>441</v>
+      </c>
+      <c r="AH15" s="169" t="s">
+        <v>442</v>
       </c>
       <c r="AI15"/>
       <c r="AJ15"/>
@@ -12916,19 +12837,19 @@
     </row>
     <row r="16" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="85" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="B16" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="172" t="s">
+      <c r="C16" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D16" s="87" t="s">
-        <v>119</v>
+        <v>406</v>
       </c>
       <c r="E16" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F16" s="88" t="s">
         <v>108</v>
@@ -12936,23 +12857,23 @@
       <c r="G16" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="173" t="s">
+      <c r="H16" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="I16" s="173" t="s">
+      <c r="I16" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J16" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K16" s="174" t="s">
+      <c r="K16" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L16" s="175"/>
-      <c r="M16" s="176"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="175"/>
-      <c r="P16" s="173" t="s">
+      <c r="L16" s="168"/>
+      <c r="M16" s="169"/>
+      <c r="N16" s="170"/>
+      <c r="O16" s="168"/>
+      <c r="P16" s="166" t="s">
         <v>116</v>
       </c>
       <c r="Q16" s="89" t="s">
@@ -12960,31 +12881,31 @@
       </c>
       <c r="R16" s="99"/>
       <c r="S16" s="100"/>
-      <c r="T16" s="178"/>
+      <c r="T16" s="171"/>
       <c r="U16" s="85" t="s">
-        <v>441</v>
-      </c>
-      <c r="V16" s="179">
+        <v>451</v>
+      </c>
+      <c r="V16" s="172">
         <v>1</v>
       </c>
-      <c r="W16" s="178"/>
+      <c r="W16" s="171"/>
       <c r="X16" s="101" t="s">
-        <v>447</v>
-      </c>
-      <c r="Y16" s="180"/>
-      <c r="Z16" s="184"/>
-      <c r="AA16" s="181">
+        <v>443</v>
+      </c>
+      <c r="Y16" s="173"/>
+      <c r="Z16" s="177"/>
+      <c r="AA16" s="174">
         <v>10</v>
       </c>
-      <c r="AB16" s="182"/>
-      <c r="AC16" s="183"/>
-      <c r="AD16" s="183"/>
+      <c r="AB16" s="175"/>
+      <c r="AC16" s="176"/>
+      <c r="AD16" s="176"/>
       <c r="AE16" s="96" t="s">
         <v>117</v>
       </c>
-      <c r="AF16" s="175"/>
-      <c r="AG16" s="176"/>
-      <c r="AH16" s="176"/>
+      <c r="AF16" s="168"/>
+      <c r="AG16" s="169"/>
+      <c r="AH16" s="169"/>
       <c r="AI16"/>
       <c r="AJ16"/>
       <c r="AK16"/>
@@ -13978,19 +13899,19 @@
     </row>
     <row r="17" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="85" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="B17" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="172" t="s">
+      <c r="C17" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D17" s="87" t="s">
-        <v>128</v>
+        <v>271</v>
       </c>
       <c r="E17" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F17" s="88" t="s">
         <v>95</v>
@@ -13998,23 +13919,23 @@
       <c r="G17" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="173" t="s">
+      <c r="H17" s="166" t="s">
         <v>179</v>
       </c>
-      <c r="I17" s="173" t="s">
+      <c r="I17" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J17" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K17" s="174" t="s">
+      <c r="K17" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L17" s="175"/>
-      <c r="M17" s="176"/>
-      <c r="N17" s="177"/>
-      <c r="O17" s="175"/>
-      <c r="P17" s="173" t="s">
+      <c r="L17" s="168"/>
+      <c r="M17" s="169"/>
+      <c r="N17" s="170"/>
+      <c r="O17" s="168"/>
+      <c r="P17" s="166" t="s">
         <v>126</v>
       </c>
       <c r="Q17" s="89" t="s">
@@ -14022,29 +13943,29 @@
       </c>
       <c r="R17" s="99"/>
       <c r="S17" s="100"/>
-      <c r="T17" s="178"/>
-      <c r="U17" s="94" t="s">
-        <v>442</v>
-      </c>
-      <c r="V17" s="179">
+      <c r="T17" s="171"/>
+      <c r="U17" s="85" t="s">
+        <v>452</v>
+      </c>
+      <c r="V17" s="172">
         <v>1</v>
       </c>
-      <c r="W17" s="178"/>
+      <c r="W17" s="171"/>
       <c r="X17" s="112" t="s">
-        <v>448</v>
-      </c>
-      <c r="Y17" s="180"/>
-      <c r="Z17" s="184"/>
-      <c r="AA17" s="181">
+        <v>444</v>
+      </c>
+      <c r="Y17" s="173"/>
+      <c r="Z17" s="177"/>
+      <c r="AA17" s="174">
         <v>15</v>
       </c>
-      <c r="AB17" s="182"/>
-      <c r="AC17" s="185"/>
-      <c r="AD17" s="185"/>
-      <c r="AE17" s="186"/>
-      <c r="AF17" s="175"/>
-      <c r="AG17" s="176"/>
-      <c r="AH17" s="176"/>
+      <c r="AB17" s="175"/>
+      <c r="AC17" s="178"/>
+      <c r="AD17" s="178"/>
+      <c r="AE17" s="179"/>
+      <c r="AF17" s="168"/>
+      <c r="AG17" s="169"/>
+      <c r="AH17" s="169"/>
       <c r="AI17"/>
       <c r="AJ17"/>
       <c r="AK17"/>
@@ -15038,19 +14959,19 @@
     </row>
     <row r="18" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="85" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B18" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="172" t="s">
+      <c r="C18" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D18" s="87" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="E18" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F18" s="88" t="s">
         <v>120</v>
@@ -15058,23 +14979,23 @@
       <c r="G18" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="173" t="s">
+      <c r="H18" s="166" t="s">
         <v>174</v>
       </c>
-      <c r="I18" s="173" t="s">
+      <c r="I18" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J18" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K18" s="174" t="s">
+      <c r="K18" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L18" s="175"/>
-      <c r="M18" s="176"/>
-      <c r="N18" s="177"/>
-      <c r="O18" s="175"/>
-      <c r="P18" s="173" t="s">
+      <c r="L18" s="168"/>
+      <c r="M18" s="169"/>
+      <c r="N18" s="170"/>
+      <c r="O18" s="168"/>
+      <c r="P18" s="166" t="s">
         <v>134</v>
       </c>
       <c r="Q18" s="89" t="s">
@@ -15082,30 +15003,29 @@
       </c>
       <c r="R18" s="99"/>
       <c r="S18" s="100"/>
-      <c r="T18" s="178"/>
-      <c r="U18" s="187" t="str">
-        <f>A18</f>
-        <v>whole-genome-4</v>
-      </c>
-      <c r="V18" s="179">
+      <c r="T18" s="171"/>
+      <c r="U18" s="85" t="s">
+        <v>453</v>
+      </c>
+      <c r="V18" s="172">
         <v>1</v>
       </c>
-      <c r="W18" s="178"/>
+      <c r="W18" s="171"/>
       <c r="X18" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y18" s="180"/>
-      <c r="Z18" s="184"/>
-      <c r="AA18" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y18" s="173"/>
+      <c r="Z18" s="177"/>
+      <c r="AA18" s="174">
         <v>20</v>
       </c>
-      <c r="AB18" s="182"/>
-      <c r="AC18" s="185"/>
-      <c r="AD18" s="185"/>
-      <c r="AE18" s="186"/>
-      <c r="AF18" s="175"/>
-      <c r="AG18" s="176"/>
-      <c r="AH18" s="176"/>
+      <c r="AB18" s="175"/>
+      <c r="AC18" s="178"/>
+      <c r="AD18" s="178"/>
+      <c r="AE18" s="179"/>
+      <c r="AF18" s="168"/>
+      <c r="AG18" s="169"/>
+      <c r="AH18" s="169"/>
       <c r="AI18"/>
       <c r="AJ18"/>
       <c r="AK18"/>
@@ -16099,19 +16019,19 @@
     </row>
     <row r="19" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="85" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="B19" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="172" t="s">
+      <c r="C19" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D19" s="87" t="s">
-        <v>142</v>
+        <v>279</v>
       </c>
       <c r="E19" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F19" s="88" t="s">
         <v>120</v>
@@ -16119,23 +16039,23 @@
       <c r="G19" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H19" s="188" t="s">
+      <c r="H19" s="180" t="s">
         <v>138</v>
       </c>
-      <c r="I19" s="173" t="s">
+      <c r="I19" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J19" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K19" s="174" t="s">
+      <c r="K19" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L19" s="175"/>
-      <c r="M19" s="176"/>
-      <c r="N19" s="177"/>
-      <c r="O19" s="175"/>
-      <c r="P19" s="173" t="s">
+      <c r="L19" s="168"/>
+      <c r="M19" s="169"/>
+      <c r="N19" s="170"/>
+      <c r="O19" s="168"/>
+      <c r="P19" s="166" t="s">
         <v>141</v>
       </c>
       <c r="Q19" s="89" t="s">
@@ -16143,31 +16063,30 @@
       </c>
       <c r="R19" s="99"/>
       <c r="S19" s="100"/>
-      <c r="T19" s="178"/>
-      <c r="U19" s="187" t="str">
-        <f t="shared" ref="U19:U52" si="0">A19</f>
-        <v>whole-genome-5</v>
-      </c>
-      <c r="V19" s="179">
+      <c r="T19" s="171"/>
+      <c r="U19" s="85" t="s">
+        <v>454</v>
+      </c>
+      <c r="V19" s="172">
         <v>1</v>
       </c>
-      <c r="W19" s="178"/>
+      <c r="W19" s="171"/>
       <c r="X19" s="112" t="s">
-        <v>452</v>
-      </c>
-      <c r="Y19" s="180"/>
-      <c r="Z19" s="184"/>
-      <c r="AA19" s="181">
+        <v>446</v>
+      </c>
+      <c r="Y19" s="173"/>
+      <c r="Z19" s="177"/>
+      <c r="AA19" s="174">
         <v>25</v>
       </c>
-      <c r="AB19" s="182"/>
-      <c r="AC19" s="185"/>
-      <c r="AD19" s="185"/>
-      <c r="AE19" s="186"/>
-      <c r="AF19" s="175"/>
-      <c r="AG19" s="176"/>
-      <c r="AH19" s="176" t="s">
-        <v>453</v>
+      <c r="AB19" s="175"/>
+      <c r="AC19" s="178"/>
+      <c r="AD19" s="178"/>
+      <c r="AE19" s="179"/>
+      <c r="AF19" s="168"/>
+      <c r="AG19" s="169"/>
+      <c r="AH19" s="169" t="s">
+        <v>447</v>
       </c>
       <c r="AI19"/>
       <c r="AJ19"/>
@@ -17162,19 +17081,19 @@
     </row>
     <row r="20" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="85" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B20" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D20" s="87" t="s">
-        <v>147</v>
+        <v>405</v>
       </c>
       <c r="E20" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F20" s="88" t="s">
         <v>120</v>
@@ -17182,23 +17101,23 @@
       <c r="G20" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="173" t="s">
+      <c r="H20" s="166" t="s">
         <v>154</v>
       </c>
-      <c r="I20" s="173" t="s">
+      <c r="I20" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J20" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K20" s="174" t="s">
+      <c r="K20" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L20" s="175"/>
-      <c r="M20" s="176"/>
-      <c r="N20" s="177"/>
-      <c r="O20" s="175"/>
-      <c r="P20" s="173" t="s">
+      <c r="L20" s="168"/>
+      <c r="M20" s="169"/>
+      <c r="N20" s="170"/>
+      <c r="O20" s="168"/>
+      <c r="P20" s="166" t="s">
         <v>146</v>
       </c>
       <c r="Q20" s="89" t="s">
@@ -17206,30 +17125,29 @@
       </c>
       <c r="R20" s="99"/>
       <c r="S20" s="100"/>
-      <c r="T20" s="178"/>
-      <c r="U20" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-genome-6</v>
-      </c>
-      <c r="V20" s="179">
+      <c r="T20" s="171"/>
+      <c r="U20" s="85" t="s">
+        <v>455</v>
+      </c>
+      <c r="V20" s="172">
         <v>1</v>
       </c>
-      <c r="W20" s="178"/>
+      <c r="W20" s="171"/>
       <c r="X20" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y20" s="180"/>
-      <c r="Z20" s="184"/>
-      <c r="AA20" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y20" s="173"/>
+      <c r="Z20" s="177"/>
+      <c r="AA20" s="174">
         <v>30</v>
       </c>
-      <c r="AB20" s="182"/>
-      <c r="AC20" s="185"/>
-      <c r="AD20" s="185"/>
-      <c r="AE20" s="186"/>
-      <c r="AF20" s="175"/>
-      <c r="AG20" s="176"/>
-      <c r="AH20" s="176"/>
+      <c r="AB20" s="175"/>
+      <c r="AC20" s="178"/>
+      <c r="AD20" s="178"/>
+      <c r="AE20" s="179"/>
+      <c r="AF20" s="168"/>
+      <c r="AG20" s="169"/>
+      <c r="AH20" s="169"/>
       <c r="AI20"/>
       <c r="AJ20"/>
       <c r="AK20"/>
@@ -18223,19 +18141,19 @@
     </row>
     <row r="21" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="85" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B21" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="172" t="s">
+      <c r="C21" s="165" t="s">
         <v>135</v>
       </c>
       <c r="D21" s="87" t="s">
-        <v>152</v>
+        <v>283</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>439</v>
+        <v>450</v>
       </c>
       <c r="F21" s="88" t="s">
         <v>120</v>
@@ -18243,23 +18161,23 @@
       <c r="G21" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H21" s="173" t="s">
+      <c r="H21" s="166" t="s">
         <v>169</v>
       </c>
-      <c r="I21" s="173" t="s">
+      <c r="I21" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J21" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K21" s="174" t="s">
+      <c r="K21" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L21" s="175"/>
-      <c r="M21" s="176"/>
-      <c r="N21" s="177"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="173" t="s">
+      <c r="L21" s="168"/>
+      <c r="M21" s="169"/>
+      <c r="N21" s="170"/>
+      <c r="O21" s="168"/>
+      <c r="P21" s="166" t="s">
         <v>151</v>
       </c>
       <c r="Q21" s="89" t="s">
@@ -18267,30 +18185,29 @@
       </c>
       <c r="R21" s="99"/>
       <c r="S21" s="100"/>
-      <c r="T21" s="178"/>
-      <c r="U21" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-genome-7</v>
-      </c>
-      <c r="V21" s="179">
+      <c r="T21" s="171"/>
+      <c r="U21" s="85" t="s">
+        <v>456</v>
+      </c>
+      <c r="V21" s="172">
         <v>1</v>
       </c>
-      <c r="W21" s="178"/>
+      <c r="W21" s="171"/>
       <c r="X21" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y21" s="180"/>
-      <c r="Z21" s="184"/>
-      <c r="AA21" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y21" s="173"/>
+      <c r="Z21" s="177"/>
+      <c r="AA21" s="174">
         <v>35</v>
       </c>
-      <c r="AB21" s="182"/>
-      <c r="AC21" s="185"/>
-      <c r="AD21" s="185"/>
-      <c r="AE21" s="186"/>
-      <c r="AF21" s="175"/>
-      <c r="AG21" s="176"/>
-      <c r="AH21" s="176"/>
+      <c r="AB21" s="175"/>
+      <c r="AC21" s="178"/>
+      <c r="AD21" s="178"/>
+      <c r="AE21" s="179"/>
+      <c r="AF21" s="168"/>
+      <c r="AG21" s="169"/>
+      <c r="AH21" s="169"/>
       <c r="AI21"/>
       <c r="AJ21"/>
       <c r="AK21"/>
@@ -19284,19 +19201,19 @@
     </row>
     <row r="22" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="85" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B22" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="87" t="s">
-        <v>457</v>
+      <c r="D22" s="112" t="s">
+        <v>407</v>
       </c>
       <c r="E22" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F22" s="88" t="s">
         <v>120</v>
@@ -19304,23 +19221,23 @@
       <c r="G22" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H22" s="173" t="s">
+      <c r="H22" s="166" t="s">
         <v>130</v>
       </c>
-      <c r="I22" s="173" t="s">
+      <c r="I22" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J22" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K22" s="174" t="s">
+      <c r="K22" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L22" s="175"/>
-      <c r="M22" s="176"/>
-      <c r="N22" s="177"/>
-      <c r="O22" s="175"/>
-      <c r="P22" s="173" t="s">
+      <c r="L22" s="168"/>
+      <c r="M22" s="169"/>
+      <c r="N22" s="170"/>
+      <c r="O22" s="168"/>
+      <c r="P22" s="166" t="s">
         <v>156</v>
       </c>
       <c r="Q22" s="89" t="s">
@@ -19328,32 +19245,31 @@
       </c>
       <c r="R22" s="99"/>
       <c r="S22" s="100"/>
-      <c r="T22" s="178"/>
-      <c r="U22" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-1</v>
-      </c>
-      <c r="V22" s="179">
+      <c r="T22" s="171"/>
+      <c r="U22" s="85" t="s">
+        <v>457</v>
+      </c>
+      <c r="V22" s="172">
         <v>1</v>
       </c>
-      <c r="W22" s="178"/>
+      <c r="W22" s="171"/>
       <c r="X22" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y22" s="180"/>
-      <c r="Z22" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y22" s="173"/>
+      <c r="Z22" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA22" s="181">
+      <c r="AA22" s="174">
         <v>40</v>
       </c>
-      <c r="AB22" s="182"/>
-      <c r="AC22" s="185"/>
-      <c r="AD22" s="185"/>
-      <c r="AE22" s="186"/>
-      <c r="AF22" s="175"/>
-      <c r="AG22" s="176"/>
-      <c r="AH22" s="189"/>
+      <c r="AB22" s="175"/>
+      <c r="AC22" s="178"/>
+      <c r="AD22" s="178"/>
+      <c r="AE22" s="179"/>
+      <c r="AF22" s="168"/>
+      <c r="AG22" s="169"/>
+      <c r="AH22" s="181"/>
       <c r="AI22"/>
       <c r="AJ22"/>
       <c r="AK22"/>
@@ -20347,19 +20263,19 @@
     </row>
     <row r="23" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="85" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B23" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="172" t="s">
+      <c r="C23" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="87" t="s">
-        <v>460</v>
+      <c r="D23" s="112" t="s">
+        <v>409</v>
       </c>
       <c r="E23" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F23" s="88" t="s">
         <v>120</v>
@@ -20367,23 +20283,23 @@
       <c r="G23" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="173" t="s">
+      <c r="H23" s="166" t="s">
         <v>159</v>
       </c>
-      <c r="I23" s="173" t="s">
+      <c r="I23" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J23" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K23" s="174" t="s">
+      <c r="K23" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L23" s="175"/>
-      <c r="M23" s="176"/>
-      <c r="N23" s="177"/>
-      <c r="O23" s="175"/>
-      <c r="P23" s="173" t="s">
+      <c r="L23" s="168"/>
+      <c r="M23" s="169"/>
+      <c r="N23" s="170"/>
+      <c r="O23" s="168"/>
+      <c r="P23" s="166" t="s">
         <v>161</v>
       </c>
       <c r="Q23" s="89" t="s">
@@ -20391,32 +20307,31 @@
       </c>
       <c r="R23" s="99"/>
       <c r="S23" s="100"/>
-      <c r="T23" s="178"/>
-      <c r="U23" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-2</v>
-      </c>
-      <c r="V23" s="179">
+      <c r="T23" s="171"/>
+      <c r="U23" s="85" t="s">
+        <v>458</v>
+      </c>
+      <c r="V23" s="172">
         <v>1</v>
       </c>
-      <c r="W23" s="178"/>
+      <c r="W23" s="171"/>
       <c r="X23" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y23" s="180"/>
-      <c r="Z23" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y23" s="173"/>
+      <c r="Z23" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="AA23" s="181">
+      <c r="AA23" s="174">
         <v>45</v>
       </c>
-      <c r="AB23" s="182"/>
-      <c r="AC23" s="185"/>
-      <c r="AD23" s="185"/>
-      <c r="AE23" s="186"/>
-      <c r="AF23" s="175"/>
-      <c r="AG23" s="176"/>
-      <c r="AH23" s="176"/>
+      <c r="AB23" s="175"/>
+      <c r="AC23" s="178"/>
+      <c r="AD23" s="178"/>
+      <c r="AE23" s="179"/>
+      <c r="AF23" s="168"/>
+      <c r="AG23" s="169"/>
+      <c r="AH23" s="169"/>
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
@@ -21410,19 +21325,19 @@
     </row>
     <row r="24" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="85" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B24" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="172" t="s">
+      <c r="C24" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="87" t="s">
-        <v>462</v>
+      <c r="D24" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E24" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F24" s="88" t="s">
         <v>120</v>
@@ -21430,23 +21345,23 @@
       <c r="G24" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H24" s="173" t="s">
+      <c r="H24" s="166" t="s">
         <v>122</v>
       </c>
-      <c r="I24" s="173" t="s">
+      <c r="I24" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J24" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K24" s="174" t="s">
+      <c r="K24" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L24" s="175"/>
-      <c r="M24" s="176"/>
-      <c r="N24" s="177"/>
-      <c r="O24" s="175"/>
-      <c r="P24" s="173" t="s">
+      <c r="L24" s="168"/>
+      <c r="M24" s="169"/>
+      <c r="N24" s="170"/>
+      <c r="O24" s="168"/>
+      <c r="P24" s="166" t="s">
         <v>166</v>
       </c>
       <c r="Q24" s="89" t="s">
@@ -21454,32 +21369,31 @@
       </c>
       <c r="R24" s="99"/>
       <c r="S24" s="100"/>
-      <c r="T24" s="178"/>
-      <c r="U24" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-3</v>
-      </c>
-      <c r="V24" s="179">
+      <c r="T24" s="171"/>
+      <c r="U24" s="85" t="s">
+        <v>459</v>
+      </c>
+      <c r="V24" s="172">
         <v>1</v>
       </c>
-      <c r="W24" s="178"/>
+      <c r="W24" s="171"/>
       <c r="X24" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y24" s="180"/>
+        <v>445</v>
+      </c>
+      <c r="Y24" s="173"/>
       <c r="Z24" s="112" t="s">
         <v>124</v>
       </c>
-      <c r="AA24" s="181">
+      <c r="AA24" s="174">
         <v>50</v>
       </c>
-      <c r="AB24" s="182"/>
-      <c r="AC24" s="185"/>
-      <c r="AD24" s="185"/>
-      <c r="AE24" s="186"/>
-      <c r="AF24" s="175"/>
-      <c r="AG24" s="176"/>
-      <c r="AH24" s="176"/>
+      <c r="AB24" s="175"/>
+      <c r="AC24" s="178"/>
+      <c r="AD24" s="178"/>
+      <c r="AE24" s="179"/>
+      <c r="AF24" s="168"/>
+      <c r="AG24" s="169"/>
+      <c r="AH24" s="169"/>
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -22473,19 +22387,19 @@
     </row>
     <row r="25" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="85" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B25" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="172" t="s">
+      <c r="C25" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D25" s="87" t="s">
-        <v>464</v>
+      <c r="D25" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E25" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F25" s="88" t="s">
         <v>120</v>
@@ -22493,23 +22407,23 @@
       <c r="G25" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H25" s="190" t="s">
+      <c r="H25" s="182" t="s">
         <v>149</v>
       </c>
-      <c r="I25" s="173" t="s">
+      <c r="I25" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J25" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K25" s="174" t="s">
+      <c r="K25" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L25" s="175"/>
-      <c r="M25" s="176"/>
-      <c r="N25" s="177"/>
-      <c r="O25" s="175"/>
-      <c r="P25" s="173" t="s">
+      <c r="L25" s="168"/>
+      <c r="M25" s="169"/>
+      <c r="N25" s="170"/>
+      <c r="O25" s="168"/>
+      <c r="P25" s="166" t="s">
         <v>171</v>
       </c>
       <c r="Q25" s="89" t="s">
@@ -22517,33 +22431,32 @@
       </c>
       <c r="R25" s="99"/>
       <c r="S25" s="100"/>
-      <c r="T25" s="178"/>
-      <c r="U25" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-4</v>
-      </c>
-      <c r="V25" s="179">
+      <c r="T25" s="171"/>
+      <c r="U25" s="85" t="s">
+        <v>460</v>
+      </c>
+      <c r="V25" s="172">
         <v>1</v>
       </c>
-      <c r="W25" s="178"/>
+      <c r="W25" s="171"/>
       <c r="X25" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y25" s="180"/>
-      <c r="Z25" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y25" s="173"/>
+      <c r="Z25" s="166" t="s">
         <v>132</v>
       </c>
-      <c r="AA25" s="181">
+      <c r="AA25" s="174">
         <v>55</v>
       </c>
-      <c r="AB25" s="182"/>
-      <c r="AC25" s="185"/>
-      <c r="AD25" s="185"/>
-      <c r="AE25" s="186"/>
-      <c r="AF25" s="175"/>
-      <c r="AG25" s="176"/>
-      <c r="AH25" s="176" t="s">
-        <v>465</v>
+      <c r="AB25" s="175"/>
+      <c r="AC25" s="178"/>
+      <c r="AD25" s="178"/>
+      <c r="AE25" s="179"/>
+      <c r="AF25" s="168"/>
+      <c r="AG25" s="169"/>
+      <c r="AH25" s="169" t="s">
+        <v>448</v>
       </c>
       <c r="AI25"/>
       <c r="AJ25"/>
@@ -23538,19 +23451,19 @@
     </row>
     <row r="26" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="85" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B26" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C26" s="172" t="s">
+      <c r="C26" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="87" t="s">
-        <v>467</v>
+      <c r="D26" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E26" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F26" s="88" t="s">
         <v>120</v>
@@ -23558,23 +23471,23 @@
       <c r="G26" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="190" t="s">
+      <c r="H26" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I26" s="173" t="s">
+      <c r="I26" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J26" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K26" s="174" t="s">
+      <c r="K26" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L26" s="175"/>
-      <c r="M26" s="176"/>
-      <c r="N26" s="177"/>
-      <c r="O26" s="175"/>
-      <c r="P26" s="173" t="s">
+      <c r="L26" s="168"/>
+      <c r="M26" s="169"/>
+      <c r="N26" s="170"/>
+      <c r="O26" s="168"/>
+      <c r="P26" s="166" t="s">
         <v>176</v>
       </c>
       <c r="Q26" s="89" t="s">
@@ -23582,32 +23495,31 @@
       </c>
       <c r="R26" s="99"/>
       <c r="S26" s="100"/>
-      <c r="T26" s="178"/>
-      <c r="U26" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-5</v>
-      </c>
-      <c r="V26" s="179">
+      <c r="T26" s="171"/>
+      <c r="U26" s="85" t="s">
+        <v>461</v>
+      </c>
+      <c r="V26" s="172">
         <v>1</v>
       </c>
-      <c r="W26" s="178"/>
+      <c r="W26" s="171"/>
       <c r="X26" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y26" s="180"/>
-      <c r="Z26" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y26" s="173"/>
+      <c r="Z26" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA26" s="181">
+      <c r="AA26" s="174">
         <v>60</v>
       </c>
-      <c r="AB26" s="182"/>
-      <c r="AC26" s="185"/>
-      <c r="AD26" s="185"/>
-      <c r="AE26" s="186"/>
-      <c r="AF26" s="175"/>
-      <c r="AG26" s="176"/>
-      <c r="AH26" s="176"/>
+      <c r="AB26" s="175"/>
+      <c r="AC26" s="178"/>
+      <c r="AD26" s="178"/>
+      <c r="AE26" s="179"/>
+      <c r="AF26" s="168"/>
+      <c r="AG26" s="169"/>
+      <c r="AH26" s="169"/>
       <c r="AI26"/>
       <c r="AJ26"/>
       <c r="AK26"/>
@@ -24601,19 +24513,19 @@
     </row>
     <row r="27" spans="1:1024" s="104" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="85" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B27" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C27" s="172" t="s">
+      <c r="C27" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D27" s="87" t="s">
-        <v>469</v>
+      <c r="D27" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E27" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F27" s="88" t="s">
         <v>120</v>
@@ -24621,23 +24533,23 @@
       <c r="G27" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H27" s="173" t="s">
+      <c r="H27" s="166" t="s">
         <v>184</v>
       </c>
-      <c r="I27" s="173" t="s">
+      <c r="I27" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J27" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="174" t="s">
+      <c r="K27" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L27" s="175"/>
-      <c r="M27" s="176"/>
-      <c r="N27" s="177"/>
-      <c r="O27" s="175"/>
-      <c r="P27" s="173" t="s">
+      <c r="L27" s="168"/>
+      <c r="M27" s="169"/>
+      <c r="N27" s="170"/>
+      <c r="O27" s="168"/>
+      <c r="P27" s="166" t="s">
         <v>181</v>
       </c>
       <c r="Q27" s="89" t="s">
@@ -24645,48 +24557,47 @@
       </c>
       <c r="R27" s="99"/>
       <c r="S27" s="100"/>
-      <c r="T27" s="178"/>
-      <c r="U27" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-6</v>
-      </c>
-      <c r="V27" s="179">
+      <c r="T27" s="171"/>
+      <c r="U27" s="85" t="s">
+        <v>462</v>
+      </c>
+      <c r="V27" s="172">
         <v>1</v>
       </c>
-      <c r="W27" s="178"/>
+      <c r="W27" s="171"/>
       <c r="X27" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y27" s="180"/>
-      <c r="Z27" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y27" s="173"/>
+      <c r="Z27" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA27" s="181">
+      <c r="AA27" s="174">
         <v>65</v>
       </c>
-      <c r="AB27" s="182"/>
-      <c r="AC27" s="185"/>
-      <c r="AD27" s="185"/>
-      <c r="AE27" s="186"/>
-      <c r="AF27" s="175"/>
-      <c r="AG27" s="176"/>
-      <c r="AH27" s="176"/>
+      <c r="AB27" s="175"/>
+      <c r="AC27" s="178"/>
+      <c r="AD27" s="178"/>
+      <c r="AE27" s="179"/>
+      <c r="AF27" s="168"/>
+      <c r="AG27" s="169"/>
+      <c r="AH27" s="169"/>
     </row>
     <row r="28" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="85" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="B28" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="172" t="s">
+      <c r="C28" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D28" s="87" t="s">
-        <v>471</v>
+      <c r="D28" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E28" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F28" s="88" t="s">
         <v>120</v>
@@ -24694,23 +24605,23 @@
       <c r="G28" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H28" s="190" t="s">
+      <c r="H28" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I28" s="173" t="s">
+      <c r="I28" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J28" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K28" s="174" t="s">
+      <c r="K28" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L28" s="175"/>
-      <c r="M28" s="176"/>
-      <c r="N28" s="177"/>
-      <c r="O28" s="175"/>
-      <c r="P28" s="173" t="s">
+      <c r="L28" s="168"/>
+      <c r="M28" s="169"/>
+      <c r="N28" s="170"/>
+      <c r="O28" s="168"/>
+      <c r="P28" s="166" t="s">
         <v>186</v>
       </c>
       <c r="Q28" s="89" t="s">
@@ -24718,32 +24629,31 @@
       </c>
       <c r="R28" s="99"/>
       <c r="S28" s="100"/>
-      <c r="T28" s="178"/>
-      <c r="U28" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-7</v>
-      </c>
-      <c r="V28" s="179">
+      <c r="T28" s="171"/>
+      <c r="U28" s="85" t="s">
+        <v>463</v>
+      </c>
+      <c r="V28" s="172">
         <v>1</v>
       </c>
-      <c r="W28" s="178"/>
+      <c r="W28" s="171"/>
       <c r="X28" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y28" s="180"/>
-      <c r="Z28" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y28" s="173"/>
+      <c r="Z28" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA28" s="181">
+      <c r="AA28" s="174">
         <v>70</v>
       </c>
-      <c r="AB28" s="182"/>
-      <c r="AC28" s="185"/>
-      <c r="AD28" s="185"/>
-      <c r="AE28" s="186"/>
-      <c r="AF28" s="175"/>
-      <c r="AG28" s="176"/>
-      <c r="AH28" s="176"/>
+      <c r="AB28" s="175"/>
+      <c r="AC28" s="178"/>
+      <c r="AD28" s="178"/>
+      <c r="AE28" s="179"/>
+      <c r="AF28" s="168"/>
+      <c r="AG28" s="169"/>
+      <c r="AH28" s="169"/>
       <c r="AI28"/>
       <c r="AJ28"/>
       <c r="AK28"/>
@@ -25737,19 +25647,19 @@
     </row>
     <row r="29" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="85" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B29" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="172" t="s">
+      <c r="C29" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="87" t="s">
-        <v>473</v>
+      <c r="D29" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E29" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F29" s="88" t="s">
         <v>120</v>
@@ -25757,23 +25667,23 @@
       <c r="G29" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H29" s="190" t="s">
+      <c r="H29" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I29" s="173" t="s">
+      <c r="I29" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J29" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K29" s="174" t="s">
+      <c r="K29" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L29" s="175"/>
-      <c r="M29" s="176"/>
-      <c r="N29" s="177"/>
-      <c r="O29" s="175"/>
-      <c r="P29" s="173" t="s">
+      <c r="L29" s="168"/>
+      <c r="M29" s="169"/>
+      <c r="N29" s="170"/>
+      <c r="O29" s="168"/>
+      <c r="P29" s="166" t="s">
         <v>190</v>
       </c>
       <c r="Q29" s="89" t="s">
@@ -25781,32 +25691,31 @@
       </c>
       <c r="R29" s="99"/>
       <c r="S29" s="100"/>
-      <c r="T29" s="178"/>
-      <c r="U29" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-8</v>
-      </c>
-      <c r="V29" s="179">
+      <c r="T29" s="171"/>
+      <c r="U29" s="85" t="s">
+        <v>464</v>
+      </c>
+      <c r="V29" s="172">
         <v>1</v>
       </c>
-      <c r="W29" s="178"/>
+      <c r="W29" s="171"/>
       <c r="X29" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y29" s="180"/>
-      <c r="Z29" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y29" s="173"/>
+      <c r="Z29" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA29" s="181">
+      <c r="AA29" s="174">
         <v>75</v>
       </c>
-      <c r="AB29" s="182"/>
-      <c r="AC29" s="185"/>
-      <c r="AD29" s="185"/>
-      <c r="AE29" s="186"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="176"/>
-      <c r="AH29" s="176"/>
+      <c r="AB29" s="175"/>
+      <c r="AC29" s="178"/>
+      <c r="AD29" s="178"/>
+      <c r="AE29" s="179"/>
+      <c r="AF29" s="168"/>
+      <c r="AG29" s="169"/>
+      <c r="AH29" s="169"/>
       <c r="AI29"/>
       <c r="AJ29"/>
       <c r="AK29"/>
@@ -26800,19 +26709,19 @@
     </row>
     <row r="30" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="85" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="B30" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="172" t="s">
+      <c r="C30" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D30" s="87" t="s">
-        <v>475</v>
+      <c r="D30" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E30" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F30" s="88" t="s">
         <v>120</v>
@@ -26820,23 +26729,23 @@
       <c r="G30" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="190" t="s">
+      <c r="H30" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I30" s="173" t="s">
+      <c r="I30" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J30" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K30" s="174" t="s">
+      <c r="K30" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L30" s="175"/>
-      <c r="M30" s="176"/>
-      <c r="N30" s="177"/>
-      <c r="O30" s="175"/>
-      <c r="P30" s="173" t="s">
+      <c r="L30" s="168"/>
+      <c r="M30" s="169"/>
+      <c r="N30" s="170"/>
+      <c r="O30" s="168"/>
+      <c r="P30" s="166" t="s">
         <v>194</v>
       </c>
       <c r="Q30" s="89" t="s">
@@ -26844,32 +26753,31 @@
       </c>
       <c r="R30" s="99"/>
       <c r="S30" s="100"/>
-      <c r="T30" s="178"/>
-      <c r="U30" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-9</v>
-      </c>
-      <c r="V30" s="179">
+      <c r="T30" s="171"/>
+      <c r="U30" s="85" t="s">
+        <v>465</v>
+      </c>
+      <c r="V30" s="172">
         <v>1</v>
       </c>
-      <c r="W30" s="178"/>
+      <c r="W30" s="171"/>
       <c r="X30" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y30" s="180"/>
-      <c r="Z30" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y30" s="173"/>
+      <c r="Z30" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA30" s="181">
+      <c r="AA30" s="174">
         <v>80</v>
       </c>
-      <c r="AB30" s="182"/>
-      <c r="AC30" s="185"/>
-      <c r="AD30" s="185"/>
-      <c r="AE30" s="186"/>
-      <c r="AF30" s="175"/>
-      <c r="AG30" s="176"/>
-      <c r="AH30" s="176"/>
+      <c r="AB30" s="175"/>
+      <c r="AC30" s="178"/>
+      <c r="AD30" s="178"/>
+      <c r="AE30" s="179"/>
+      <c r="AF30" s="168"/>
+      <c r="AG30" s="169"/>
+      <c r="AH30" s="169"/>
       <c r="AI30"/>
       <c r="AJ30"/>
       <c r="AK30"/>
@@ -27863,19 +27771,19 @@
     </row>
     <row r="31" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="85" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="B31" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D31" s="87" t="s">
-        <v>477</v>
+      <c r="D31" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E31" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F31" s="88" t="s">
         <v>120</v>
@@ -27883,23 +27791,23 @@
       <c r="G31" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H31" s="190" t="s">
+      <c r="H31" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I31" s="173" t="s">
+      <c r="I31" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J31" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K31" s="174" t="s">
+      <c r="K31" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L31" s="175"/>
-      <c r="M31" s="176"/>
-      <c r="N31" s="177"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="173" t="s">
+      <c r="L31" s="168"/>
+      <c r="M31" s="169"/>
+      <c r="N31" s="170"/>
+      <c r="O31" s="168"/>
+      <c r="P31" s="166" t="s">
         <v>198</v>
       </c>
       <c r="Q31" s="89" t="s">
@@ -27907,32 +27815,31 @@
       </c>
       <c r="R31" s="99"/>
       <c r="S31" s="100"/>
-      <c r="T31" s="178"/>
-      <c r="U31" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-10</v>
-      </c>
-      <c r="V31" s="179">
+      <c r="T31" s="171"/>
+      <c r="U31" s="85" t="s">
+        <v>466</v>
+      </c>
+      <c r="V31" s="172">
         <v>1</v>
       </c>
-      <c r="W31" s="178"/>
+      <c r="W31" s="171"/>
       <c r="X31" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y31" s="180"/>
-      <c r="Z31" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y31" s="173"/>
+      <c r="Z31" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA31" s="181">
+      <c r="AA31" s="174">
         <v>85</v>
       </c>
-      <c r="AB31" s="182"/>
-      <c r="AC31" s="185"/>
-      <c r="AD31" s="185"/>
-      <c r="AE31" s="186"/>
-      <c r="AF31" s="175"/>
-      <c r="AG31" s="176"/>
-      <c r="AH31" s="176"/>
+      <c r="AB31" s="175"/>
+      <c r="AC31" s="178"/>
+      <c r="AD31" s="178"/>
+      <c r="AE31" s="179"/>
+      <c r="AF31" s="168"/>
+      <c r="AG31" s="169"/>
+      <c r="AH31" s="169"/>
       <c r="AI31"/>
       <c r="AJ31"/>
       <c r="AK31"/>
@@ -28926,19 +28833,19 @@
     </row>
     <row r="32" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="85" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="B32" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="172" t="s">
+      <c r="C32" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="87" t="s">
-        <v>479</v>
+      <c r="D32" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F32" s="88" t="s">
         <v>120</v>
@@ -28946,23 +28853,23 @@
       <c r="G32" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H32" s="190" t="s">
+      <c r="H32" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I32" s="173" t="s">
+      <c r="I32" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J32" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K32" s="174" t="s">
+      <c r="K32" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L32" s="175"/>
-      <c r="M32" s="176"/>
-      <c r="N32" s="177"/>
-      <c r="O32" s="175"/>
-      <c r="P32" s="173" t="s">
+      <c r="L32" s="168"/>
+      <c r="M32" s="169"/>
+      <c r="N32" s="170"/>
+      <c r="O32" s="168"/>
+      <c r="P32" s="166" t="s">
         <v>202</v>
       </c>
       <c r="Q32" s="89" t="s">
@@ -28970,32 +28877,31 @@
       </c>
       <c r="R32" s="99"/>
       <c r="S32" s="100"/>
-      <c r="T32" s="178"/>
-      <c r="U32" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-11</v>
-      </c>
-      <c r="V32" s="179">
+      <c r="T32" s="171"/>
+      <c r="U32" s="85" t="s">
+        <v>467</v>
+      </c>
+      <c r="V32" s="172">
         <v>1</v>
       </c>
-      <c r="W32" s="178"/>
+      <c r="W32" s="171"/>
       <c r="X32" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y32" s="180"/>
-      <c r="Z32" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y32" s="173"/>
+      <c r="Z32" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA32" s="181">
+      <c r="AA32" s="174">
         <v>90</v>
       </c>
-      <c r="AB32" s="182"/>
-      <c r="AC32" s="185"/>
-      <c r="AD32" s="185"/>
-      <c r="AE32" s="186"/>
-      <c r="AF32" s="175"/>
-      <c r="AG32" s="176"/>
-      <c r="AH32" s="176"/>
+      <c r="AB32" s="175"/>
+      <c r="AC32" s="178"/>
+      <c r="AD32" s="178"/>
+      <c r="AE32" s="179"/>
+      <c r="AF32" s="168"/>
+      <c r="AG32" s="169"/>
+      <c r="AH32" s="169"/>
       <c r="AI32"/>
       <c r="AJ32"/>
       <c r="AK32"/>
@@ -29989,19 +29895,19 @@
     </row>
     <row r="33" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="85" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
       <c r="B33" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="172" t="s">
+      <c r="C33" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="87" t="s">
-        <v>481</v>
+      <c r="D33" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E33" s="85" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="F33" s="88" t="s">
         <v>120</v>
@@ -30009,23 +29915,23 @@
       <c r="G33" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H33" s="190" t="s">
+      <c r="H33" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I33" s="173" t="s">
+      <c r="I33" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J33" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K33" s="174" t="s">
+      <c r="K33" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L33" s="175"/>
-      <c r="M33" s="176"/>
-      <c r="N33" s="177"/>
-      <c r="O33" s="175"/>
-      <c r="P33" s="173" t="s">
+      <c r="L33" s="168"/>
+      <c r="M33" s="169"/>
+      <c r="N33" s="170"/>
+      <c r="O33" s="168"/>
+      <c r="P33" s="166" t="s">
         <v>206</v>
       </c>
       <c r="Q33" s="89" t="s">
@@ -30033,32 +29939,31 @@
       </c>
       <c r="R33" s="99"/>
       <c r="S33" s="100"/>
-      <c r="T33" s="178"/>
-      <c r="U33" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>whole-exome-12</v>
-      </c>
-      <c r="V33" s="179">
+      <c r="T33" s="171"/>
+      <c r="U33" s="85" t="s">
+        <v>468</v>
+      </c>
+      <c r="V33" s="172">
         <v>1</v>
       </c>
-      <c r="W33" s="178"/>
+      <c r="W33" s="171"/>
       <c r="X33" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y33" s="180"/>
-      <c r="Z33" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y33" s="173"/>
+      <c r="Z33" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA33" s="181">
+      <c r="AA33" s="174">
         <v>95</v>
       </c>
-      <c r="AB33" s="182"/>
-      <c r="AC33" s="185"/>
-      <c r="AD33" s="185"/>
-      <c r="AE33" s="186"/>
-      <c r="AF33" s="175"/>
-      <c r="AG33" s="176"/>
-      <c r="AH33" s="176"/>
+      <c r="AB33" s="175"/>
+      <c r="AC33" s="178"/>
+      <c r="AD33" s="178"/>
+      <c r="AE33" s="179"/>
+      <c r="AF33" s="168"/>
+      <c r="AG33" s="169"/>
+      <c r="AH33" s="169"/>
       <c r="AI33"/>
       <c r="AJ33"/>
       <c r="AK33"/>
@@ -31052,19 +30957,19 @@
     </row>
     <row r="34" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="85" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="B34" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="172" t="s">
+      <c r="C34" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D34" s="87" t="s">
-        <v>483</v>
+      <c r="D34" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E34" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F34" s="88" t="s">
         <v>120</v>
@@ -31072,23 +30977,23 @@
       <c r="G34" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H34" s="190" t="s">
+      <c r="H34" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I34" s="173" t="s">
+      <c r="I34" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J34" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K34" s="174" t="s">
+      <c r="K34" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L34" s="175"/>
-      <c r="M34" s="176"/>
-      <c r="N34" s="177"/>
-      <c r="O34" s="175"/>
-      <c r="P34" s="173" t="s">
+      <c r="L34" s="168"/>
+      <c r="M34" s="169"/>
+      <c r="N34" s="170"/>
+      <c r="O34" s="168"/>
+      <c r="P34" s="166" t="s">
         <v>210</v>
       </c>
       <c r="Q34" s="89" t="s">
@@ -31096,32 +31001,31 @@
       </c>
       <c r="R34" s="99"/>
       <c r="S34" s="100"/>
-      <c r="T34" s="178"/>
-      <c r="U34" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-1</v>
-      </c>
-      <c r="V34" s="179">
+      <c r="T34" s="171"/>
+      <c r="U34" s="85" t="s">
+        <v>469</v>
+      </c>
+      <c r="V34" s="172">
         <v>1</v>
       </c>
-      <c r="W34" s="178"/>
+      <c r="W34" s="171"/>
       <c r="X34" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y34" s="180"/>
-      <c r="Z34" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y34" s="173"/>
+      <c r="Z34" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA34" s="181">
+      <c r="AA34" s="174">
         <v>100</v>
       </c>
-      <c r="AB34" s="182"/>
-      <c r="AC34" s="185"/>
-      <c r="AD34" s="185"/>
-      <c r="AE34" s="186"/>
-      <c r="AF34" s="175"/>
-      <c r="AG34" s="176"/>
-      <c r="AH34" s="176"/>
+      <c r="AB34" s="175"/>
+      <c r="AC34" s="178"/>
+      <c r="AD34" s="178"/>
+      <c r="AE34" s="179"/>
+      <c r="AF34" s="168"/>
+      <c r="AG34" s="169"/>
+      <c r="AH34" s="169"/>
       <c r="AI34"/>
       <c r="AJ34"/>
       <c r="AK34"/>
@@ -32115,19 +32019,19 @@
     </row>
     <row r="35" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="85" t="s">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="B35" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="172" t="s">
+      <c r="C35" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D35" s="87" t="s">
-        <v>486</v>
+      <c r="D35" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E35" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F35" s="88" t="s">
         <v>120</v>
@@ -32135,23 +32039,23 @@
       <c r="G35" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H35" s="190" t="s">
+      <c r="H35" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I35" s="173" t="s">
+      <c r="I35" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J35" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K35" s="174" t="s">
+      <c r="K35" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L35" s="175"/>
-      <c r="M35" s="176"/>
-      <c r="N35" s="177"/>
-      <c r="O35" s="175"/>
-      <c r="P35" s="173" t="s">
+      <c r="L35" s="168"/>
+      <c r="M35" s="169"/>
+      <c r="N35" s="170"/>
+      <c r="O35" s="168"/>
+      <c r="P35" s="166" t="s">
         <v>214</v>
       </c>
       <c r="Q35" s="89" t="s">
@@ -32159,32 +32063,31 @@
       </c>
       <c r="R35" s="99"/>
       <c r="S35" s="100"/>
-      <c r="T35" s="178"/>
-      <c r="U35" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-2</v>
-      </c>
-      <c r="V35" s="179">
+      <c r="T35" s="171"/>
+      <c r="U35" s="85" t="s">
+        <v>470</v>
+      </c>
+      <c r="V35" s="172">
         <v>1</v>
       </c>
-      <c r="W35" s="178"/>
+      <c r="W35" s="171"/>
       <c r="X35" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y35" s="180"/>
-      <c r="Z35" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y35" s="173"/>
+      <c r="Z35" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA35" s="181">
+      <c r="AA35" s="174">
         <v>100</v>
       </c>
-      <c r="AB35" s="182"/>
-      <c r="AC35" s="185"/>
-      <c r="AD35" s="185"/>
-      <c r="AE35" s="186"/>
-      <c r="AF35" s="175"/>
-      <c r="AG35" s="176"/>
-      <c r="AH35" s="176"/>
+      <c r="AB35" s="175"/>
+      <c r="AC35" s="178"/>
+      <c r="AD35" s="178"/>
+      <c r="AE35" s="179"/>
+      <c r="AF35" s="168"/>
+      <c r="AG35" s="169"/>
+      <c r="AH35" s="169"/>
       <c r="AI35"/>
       <c r="AJ35"/>
       <c r="AK35"/>
@@ -33178,19 +33081,19 @@
     </row>
     <row r="36" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="85" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="B36" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="172" t="s">
+      <c r="C36" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D36" s="87" t="s">
-        <v>488</v>
+      <c r="D36" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E36" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F36" s="88" t="s">
         <v>120</v>
@@ -33198,23 +33101,23 @@
       <c r="G36" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H36" s="190" t="s">
+      <c r="H36" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I36" s="173" t="s">
+      <c r="I36" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J36" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K36" s="174" t="s">
+      <c r="K36" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L36" s="175"/>
-      <c r="M36" s="176"/>
-      <c r="N36" s="177"/>
-      <c r="O36" s="175"/>
-      <c r="P36" s="173" t="s">
+      <c r="L36" s="168"/>
+      <c r="M36" s="169"/>
+      <c r="N36" s="170"/>
+      <c r="O36" s="168"/>
+      <c r="P36" s="166" t="s">
         <v>218</v>
       </c>
       <c r="Q36" s="89" t="s">
@@ -33222,48 +33125,47 @@
       </c>
       <c r="R36" s="99"/>
       <c r="S36" s="100"/>
-      <c r="T36" s="178"/>
-      <c r="U36" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-3</v>
-      </c>
-      <c r="V36" s="179">
+      <c r="T36" s="171"/>
+      <c r="U36" s="85" t="s">
+        <v>471</v>
+      </c>
+      <c r="V36" s="172">
         <v>1</v>
       </c>
-      <c r="W36" s="178"/>
+      <c r="W36" s="171"/>
       <c r="X36" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y36" s="180"/>
-      <c r="Z36" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y36" s="173"/>
+      <c r="Z36" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA36" s="181">
+      <c r="AA36" s="174">
         <v>100</v>
       </c>
-      <c r="AB36" s="182"/>
-      <c r="AC36" s="185"/>
-      <c r="AD36" s="185"/>
-      <c r="AE36" s="186"/>
-      <c r="AF36" s="175"/>
-      <c r="AG36" s="176"/>
-      <c r="AH36" s="176"/>
+      <c r="AB36" s="175"/>
+      <c r="AC36" s="178"/>
+      <c r="AD36" s="178"/>
+      <c r="AE36" s="179"/>
+      <c r="AF36" s="168"/>
+      <c r="AG36" s="169"/>
+      <c r="AH36" s="169"/>
     </row>
     <row r="37" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="85" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B37" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C37" s="172" t="s">
+      <c r="C37" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D37" s="87" t="s">
-        <v>490</v>
+      <c r="D37" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E37" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F37" s="88" t="s">
         <v>120</v>
@@ -33271,23 +33173,23 @@
       <c r="G37" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H37" s="190" t="s">
+      <c r="H37" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I37" s="173" t="s">
+      <c r="I37" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J37" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K37" s="174" t="s">
+      <c r="K37" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L37" s="175"/>
-      <c r="M37" s="176"/>
-      <c r="N37" s="177"/>
-      <c r="O37" s="175"/>
-      <c r="P37" s="173" t="s">
+      <c r="L37" s="168"/>
+      <c r="M37" s="169"/>
+      <c r="N37" s="170"/>
+      <c r="O37" s="168"/>
+      <c r="P37" s="166" t="s">
         <v>222</v>
       </c>
       <c r="Q37" s="89" t="s">
@@ -33295,48 +33197,47 @@
       </c>
       <c r="R37" s="99"/>
       <c r="S37" s="100"/>
-      <c r="T37" s="178"/>
-      <c r="U37" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-4</v>
-      </c>
-      <c r="V37" s="179">
+      <c r="T37" s="171"/>
+      <c r="U37" s="85" t="s">
+        <v>472</v>
+      </c>
+      <c r="V37" s="172">
         <v>1</v>
       </c>
-      <c r="W37" s="178"/>
+      <c r="W37" s="171"/>
       <c r="X37" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y37" s="180"/>
-      <c r="Z37" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y37" s="173"/>
+      <c r="Z37" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA37" s="181">
+      <c r="AA37" s="174">
         <v>100</v>
       </c>
-      <c r="AB37" s="182"/>
-      <c r="AC37" s="185"/>
-      <c r="AD37" s="185"/>
-      <c r="AE37" s="186"/>
-      <c r="AF37" s="175"/>
-      <c r="AG37" s="176"/>
-      <c r="AH37" s="176"/>
+      <c r="AB37" s="175"/>
+      <c r="AC37" s="178"/>
+      <c r="AD37" s="178"/>
+      <c r="AE37" s="179"/>
+      <c r="AF37" s="168"/>
+      <c r="AG37" s="169"/>
+      <c r="AH37" s="169"/>
     </row>
     <row r="38" spans="1:1024" s="105" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="85" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="B38" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="172" t="s">
+      <c r="C38" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D38" s="87" t="s">
-        <v>492</v>
+      <c r="D38" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E38" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F38" s="88" t="s">
         <v>120</v>
@@ -33344,23 +33245,23 @@
       <c r="G38" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H38" s="190" t="s">
+      <c r="H38" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I38" s="173" t="s">
+      <c r="I38" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J38" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K38" s="174" t="s">
+      <c r="K38" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L38" s="175"/>
-      <c r="M38" s="176"/>
-      <c r="N38" s="177"/>
-      <c r="O38" s="175"/>
-      <c r="P38" s="173" t="s">
+      <c r="L38" s="168"/>
+      <c r="M38" s="169"/>
+      <c r="N38" s="170"/>
+      <c r="O38" s="168"/>
+      <c r="P38" s="166" t="s">
         <v>226</v>
       </c>
       <c r="Q38" s="89" t="s">
@@ -33368,48 +33269,47 @@
       </c>
       <c r="R38" s="99"/>
       <c r="S38" s="100"/>
-      <c r="T38" s="178"/>
-      <c r="U38" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-5</v>
-      </c>
-      <c r="V38" s="179">
+      <c r="T38" s="171"/>
+      <c r="U38" s="85" t="s">
+        <v>473</v>
+      </c>
+      <c r="V38" s="172">
         <v>1</v>
       </c>
-      <c r="W38" s="178"/>
+      <c r="W38" s="171"/>
       <c r="X38" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y38" s="180"/>
-      <c r="Z38" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y38" s="173"/>
+      <c r="Z38" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA38" s="181">
+      <c r="AA38" s="174">
         <v>100</v>
       </c>
-      <c r="AB38" s="182"/>
-      <c r="AC38" s="185"/>
-      <c r="AD38" s="185"/>
-      <c r="AE38" s="186"/>
-      <c r="AF38" s="175"/>
-      <c r="AG38" s="176"/>
-      <c r="AH38" s="176"/>
+      <c r="AB38" s="175"/>
+      <c r="AC38" s="178"/>
+      <c r="AD38" s="178"/>
+      <c r="AE38" s="179"/>
+      <c r="AF38" s="168"/>
+      <c r="AG38" s="169"/>
+      <c r="AH38" s="169"/>
     </row>
     <row r="39" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="85" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
       <c r="B39" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="172" t="s">
+      <c r="C39" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D39" s="87" t="s">
-        <v>494</v>
+      <c r="D39" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E39" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F39" s="88" t="s">
         <v>120</v>
@@ -33417,23 +33317,23 @@
       <c r="G39" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H39" s="190" t="s">
+      <c r="H39" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I39" s="173" t="s">
+      <c r="I39" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J39" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K39" s="174" t="s">
+      <c r="K39" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L39" s="175"/>
-      <c r="M39" s="176"/>
-      <c r="N39" s="177"/>
-      <c r="O39" s="175"/>
-      <c r="P39" s="173" t="s">
+      <c r="L39" s="168"/>
+      <c r="M39" s="169"/>
+      <c r="N39" s="170"/>
+      <c r="O39" s="168"/>
+      <c r="P39" s="166" t="s">
         <v>230</v>
       </c>
       <c r="Q39" s="89" t="s">
@@ -33441,32 +33341,31 @@
       </c>
       <c r="R39" s="99"/>
       <c r="S39" s="100"/>
-      <c r="T39" s="178"/>
-      <c r="U39" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-6</v>
-      </c>
-      <c r="V39" s="179">
+      <c r="T39" s="171"/>
+      <c r="U39" s="85" t="s">
+        <v>474</v>
+      </c>
+      <c r="V39" s="172">
         <v>1</v>
       </c>
-      <c r="W39" s="178"/>
+      <c r="W39" s="171"/>
       <c r="X39" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y39" s="180"/>
-      <c r="Z39" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y39" s="173"/>
+      <c r="Z39" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA39" s="181">
+      <c r="AA39" s="174">
         <v>100</v>
       </c>
-      <c r="AB39" s="182"/>
-      <c r="AC39" s="185"/>
-      <c r="AD39" s="185"/>
-      <c r="AE39" s="186"/>
-      <c r="AF39" s="175"/>
-      <c r="AG39" s="176"/>
-      <c r="AH39" s="176"/>
+      <c r="AB39" s="175"/>
+      <c r="AC39" s="178"/>
+      <c r="AD39" s="178"/>
+      <c r="AE39" s="179"/>
+      <c r="AF39" s="168"/>
+      <c r="AG39" s="169"/>
+      <c r="AH39" s="169"/>
       <c r="AI39"/>
       <c r="AJ39"/>
       <c r="AK39"/>
@@ -34460,19 +34359,19 @@
     </row>
     <row r="40" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="85" t="s">
-        <v>495</v>
+        <v>475</v>
       </c>
       <c r="B40" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="172" t="s">
+      <c r="C40" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D40" s="87" t="s">
-        <v>496</v>
+      <c r="D40" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E40" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F40" s="88" t="s">
         <v>120</v>
@@ -34480,23 +34379,23 @@
       <c r="G40" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H40" s="190" t="s">
+      <c r="H40" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I40" s="173" t="s">
+      <c r="I40" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J40" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K40" s="174" t="s">
+      <c r="K40" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L40" s="175"/>
-      <c r="M40" s="176"/>
-      <c r="N40" s="177"/>
-      <c r="O40" s="175"/>
-      <c r="P40" s="173" t="s">
+      <c r="L40" s="168"/>
+      <c r="M40" s="169"/>
+      <c r="N40" s="170"/>
+      <c r="O40" s="168"/>
+      <c r="P40" s="166" t="s">
         <v>234</v>
       </c>
       <c r="Q40" s="89" t="s">
@@ -34504,32 +34403,31 @@
       </c>
       <c r="R40" s="99"/>
       <c r="S40" s="100"/>
-      <c r="T40" s="178"/>
-      <c r="U40" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-7</v>
-      </c>
-      <c r="V40" s="179">
+      <c r="T40" s="171"/>
+      <c r="U40" s="85" t="s">
+        <v>475</v>
+      </c>
+      <c r="V40" s="172">
         <v>1</v>
       </c>
-      <c r="W40" s="178"/>
+      <c r="W40" s="171"/>
       <c r="X40" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y40" s="180"/>
-      <c r="Z40" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y40" s="173"/>
+      <c r="Z40" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA40" s="181">
+      <c r="AA40" s="174">
         <v>100</v>
       </c>
-      <c r="AB40" s="182"/>
-      <c r="AC40" s="185"/>
-      <c r="AD40" s="185"/>
-      <c r="AE40" s="186"/>
-      <c r="AF40" s="175"/>
-      <c r="AG40" s="176"/>
-      <c r="AH40" s="176"/>
+      <c r="AB40" s="175"/>
+      <c r="AC40" s="178"/>
+      <c r="AD40" s="178"/>
+      <c r="AE40" s="179"/>
+      <c r="AF40" s="168"/>
+      <c r="AG40" s="169"/>
+      <c r="AH40" s="169"/>
       <c r="AI40"/>
       <c r="AJ40"/>
       <c r="AK40"/>
@@ -35523,19 +35421,19 @@
     </row>
     <row r="41" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="85" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B41" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="172" t="s">
+      <c r="C41" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D41" s="87" t="s">
-        <v>498</v>
+      <c r="D41" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F41" s="88" t="s">
         <v>120</v>
@@ -35543,23 +35441,23 @@
       <c r="G41" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H41" s="190" t="s">
+      <c r="H41" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I41" s="173" t="s">
+      <c r="I41" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J41" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K41" s="174" t="s">
+      <c r="K41" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L41" s="175"/>
-      <c r="M41" s="176"/>
-      <c r="N41" s="177"/>
-      <c r="O41" s="175"/>
-      <c r="P41" s="173" t="s">
+      <c r="L41" s="168"/>
+      <c r="M41" s="169"/>
+      <c r="N41" s="170"/>
+      <c r="O41" s="168"/>
+      <c r="P41" s="166" t="s">
         <v>238</v>
       </c>
       <c r="Q41" s="89" t="s">
@@ -35567,32 +35465,31 @@
       </c>
       <c r="R41" s="99"/>
       <c r="S41" s="100"/>
-      <c r="T41" s="178"/>
-      <c r="U41" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-8</v>
-      </c>
-      <c r="V41" s="179">
+      <c r="T41" s="171"/>
+      <c r="U41" s="85" t="s">
+        <v>476</v>
+      </c>
+      <c r="V41" s="172">
         <v>1</v>
       </c>
-      <c r="W41" s="178"/>
+      <c r="W41" s="171"/>
       <c r="X41" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y41" s="180"/>
-      <c r="Z41" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y41" s="173"/>
+      <c r="Z41" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA41" s="181">
+      <c r="AA41" s="174">
         <v>100</v>
       </c>
-      <c r="AB41" s="182"/>
-      <c r="AC41" s="185"/>
-      <c r="AD41" s="185"/>
-      <c r="AE41" s="186"/>
-      <c r="AF41" s="175"/>
-      <c r="AG41" s="176"/>
-      <c r="AH41" s="176"/>
+      <c r="AB41" s="175"/>
+      <c r="AC41" s="178"/>
+      <c r="AD41" s="178"/>
+      <c r="AE41" s="179"/>
+      <c r="AF41" s="168"/>
+      <c r="AG41" s="169"/>
+      <c r="AH41" s="169"/>
       <c r="AI41"/>
       <c r="AJ41"/>
       <c r="AK41"/>
@@ -36586,19 +36483,19 @@
     </row>
     <row r="42" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="85" t="s">
-        <v>499</v>
+        <v>477</v>
       </c>
       <c r="B42" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="172" t="s">
+      <c r="C42" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="87" t="s">
-        <v>500</v>
+      <c r="D42" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F42" s="88" t="s">
         <v>120</v>
@@ -36606,23 +36503,23 @@
       <c r="G42" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H42" s="190" t="s">
+      <c r="H42" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I42" s="173" t="s">
+      <c r="I42" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J42" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K42" s="174" t="s">
+      <c r="K42" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L42" s="175"/>
-      <c r="M42" s="176"/>
-      <c r="N42" s="177"/>
-      <c r="O42" s="175"/>
-      <c r="P42" s="173" t="s">
+      <c r="L42" s="168"/>
+      <c r="M42" s="169"/>
+      <c r="N42" s="170"/>
+      <c r="O42" s="168"/>
+      <c r="P42" s="166" t="s">
         <v>242</v>
       </c>
       <c r="Q42" s="89" t="s">
@@ -36630,32 +36527,31 @@
       </c>
       <c r="R42" s="99"/>
       <c r="S42" s="100"/>
-      <c r="T42" s="178"/>
-      <c r="U42" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-9</v>
-      </c>
-      <c r="V42" s="179">
+      <c r="T42" s="171"/>
+      <c r="U42" s="85" t="s">
+        <v>477</v>
+      </c>
+      <c r="V42" s="172">
         <v>1</v>
       </c>
-      <c r="W42" s="178"/>
+      <c r="W42" s="171"/>
       <c r="X42" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y42" s="180"/>
-      <c r="Z42" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y42" s="173"/>
+      <c r="Z42" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA42" s="181">
+      <c r="AA42" s="174">
         <v>100</v>
       </c>
-      <c r="AB42" s="182"/>
-      <c r="AC42" s="185"/>
-      <c r="AD42" s="185"/>
-      <c r="AE42" s="186"/>
-      <c r="AF42" s="175"/>
-      <c r="AG42" s="176"/>
-      <c r="AH42" s="176"/>
+      <c r="AB42" s="175"/>
+      <c r="AC42" s="178"/>
+      <c r="AD42" s="178"/>
+      <c r="AE42" s="179"/>
+      <c r="AF42" s="168"/>
+      <c r="AG42" s="169"/>
+      <c r="AH42" s="169"/>
       <c r="AI42"/>
       <c r="AJ42"/>
       <c r="AK42"/>
@@ -37649,19 +37545,19 @@
     </row>
     <row r="43" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="85" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="B43" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C43" s="172" t="s">
+      <c r="C43" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="87" t="s">
-        <v>502</v>
+      <c r="D43" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E43" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F43" s="88" t="s">
         <v>120</v>
@@ -37669,23 +37565,23 @@
       <c r="G43" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H43" s="190" t="s">
+      <c r="H43" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I43" s="173" t="s">
+      <c r="I43" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J43" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K43" s="174" t="s">
+      <c r="K43" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L43" s="175"/>
-      <c r="M43" s="176"/>
-      <c r="N43" s="177"/>
-      <c r="O43" s="175"/>
-      <c r="P43" s="173" t="s">
+      <c r="L43" s="168"/>
+      <c r="M43" s="169"/>
+      <c r="N43" s="170"/>
+      <c r="O43" s="168"/>
+      <c r="P43" s="166" t="s">
         <v>246</v>
       </c>
       <c r="Q43" s="89" t="s">
@@ -37693,32 +37589,31 @@
       </c>
       <c r="R43" s="99"/>
       <c r="S43" s="100"/>
-      <c r="T43" s="178"/>
-      <c r="U43" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-10</v>
-      </c>
-      <c r="V43" s="179">
+      <c r="T43" s="171"/>
+      <c r="U43" s="85" t="s">
+        <v>478</v>
+      </c>
+      <c r="V43" s="172">
         <v>1</v>
       </c>
-      <c r="W43" s="178"/>
+      <c r="W43" s="171"/>
       <c r="X43" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y43" s="180"/>
-      <c r="Z43" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y43" s="173"/>
+      <c r="Z43" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA43" s="181">
+      <c r="AA43" s="174">
         <v>100</v>
       </c>
-      <c r="AB43" s="182"/>
-      <c r="AC43" s="185"/>
-      <c r="AD43" s="185"/>
-      <c r="AE43" s="186"/>
-      <c r="AF43" s="175"/>
-      <c r="AG43" s="176"/>
-      <c r="AH43" s="176"/>
+      <c r="AB43" s="175"/>
+      <c r="AC43" s="178"/>
+      <c r="AD43" s="178"/>
+      <c r="AE43" s="179"/>
+      <c r="AF43" s="168"/>
+      <c r="AG43" s="169"/>
+      <c r="AH43" s="169"/>
       <c r="AI43"/>
       <c r="AJ43"/>
       <c r="AK43"/>
@@ -38712,19 +38607,19 @@
     </row>
     <row r="44" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="85" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
       <c r="B44" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="172" t="s">
+      <c r="C44" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="87" t="s">
-        <v>504</v>
+      <c r="D44" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E44" s="85" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
       <c r="F44" s="88" t="s">
         <v>120</v>
@@ -38732,23 +38627,23 @@
       <c r="G44" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H44" s="190" t="s">
+      <c r="H44" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I44" s="173" t="s">
+      <c r="I44" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J44" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K44" s="174" t="s">
+      <c r="K44" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L44" s="175"/>
-      <c r="M44" s="176"/>
-      <c r="N44" s="177"/>
-      <c r="O44" s="175"/>
-      <c r="P44" s="173" t="s">
+      <c r="L44" s="168"/>
+      <c r="M44" s="169"/>
+      <c r="N44" s="170"/>
+      <c r="O44" s="168"/>
+      <c r="P44" s="166" t="s">
         <v>250</v>
       </c>
       <c r="Q44" s="89" t="s">
@@ -38756,32 +38651,31 @@
       </c>
       <c r="R44" s="99"/>
       <c r="S44" s="100"/>
-      <c r="T44" s="178"/>
-      <c r="U44" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>cancer-capture-panels-11</v>
-      </c>
-      <c r="V44" s="179">
+      <c r="T44" s="171"/>
+      <c r="U44" s="85" t="s">
+        <v>479</v>
+      </c>
+      <c r="V44" s="172">
         <v>1</v>
       </c>
-      <c r="W44" s="178"/>
+      <c r="W44" s="171"/>
       <c r="X44" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y44" s="180"/>
-      <c r="Z44" s="173" t="s">
+        <v>445</v>
+      </c>
+      <c r="Y44" s="173"/>
+      <c r="Z44" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="AA44" s="181">
+      <c r="AA44" s="174">
         <v>100</v>
       </c>
-      <c r="AB44" s="182"/>
-      <c r="AC44" s="185"/>
-      <c r="AD44" s="185"/>
-      <c r="AE44" s="186"/>
-      <c r="AF44" s="175"/>
-      <c r="AG44" s="176"/>
-      <c r="AH44" s="176"/>
+      <c r="AB44" s="175"/>
+      <c r="AC44" s="178"/>
+      <c r="AD44" s="178"/>
+      <c r="AE44" s="179"/>
+      <c r="AF44" s="168"/>
+      <c r="AG44" s="169"/>
+      <c r="AH44" s="169"/>
       <c r="AI44"/>
       <c r="AJ44"/>
       <c r="AK44"/>
@@ -39775,19 +39669,19 @@
     </row>
     <row r="45" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="85" t="s">
-        <v>505</v>
+        <v>480</v>
       </c>
       <c r="B45" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="172" t="s">
+      <c r="C45" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D45" s="87" t="s">
-        <v>267</v>
+      <c r="D45" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E45" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F45" s="88" t="s">
         <v>120</v>
@@ -39795,23 +39689,23 @@
       <c r="G45" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H45" s="190" t="s">
+      <c r="H45" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I45" s="173" t="s">
+      <c r="I45" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J45" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K45" s="174" t="s">
+      <c r="K45" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L45" s="175"/>
-      <c r="M45" s="176"/>
-      <c r="N45" s="177"/>
-      <c r="O45" s="175"/>
-      <c r="P45" s="173" t="s">
+      <c r="L45" s="168"/>
+      <c r="M45" s="169"/>
+      <c r="N45" s="170"/>
+      <c r="O45" s="168"/>
+      <c r="P45" s="166" t="s">
         <v>254</v>
       </c>
       <c r="Q45" s="89" t="s">
@@ -39819,30 +39713,29 @@
       </c>
       <c r="R45" s="99"/>
       <c r="S45" s="100"/>
-      <c r="T45" s="178"/>
-      <c r="U45" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-1</v>
-      </c>
-      <c r="V45" s="179">
+      <c r="T45" s="171"/>
+      <c r="U45" s="85" t="s">
+        <v>480</v>
+      </c>
+      <c r="V45" s="172">
         <v>1</v>
       </c>
-      <c r="W45" s="178"/>
+      <c r="W45" s="171"/>
       <c r="X45" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y45" s="180"/>
-      <c r="Z45" s="184"/>
-      <c r="AA45" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y45" s="173"/>
+      <c r="Z45" s="177"/>
+      <c r="AA45" s="174">
         <v>100</v>
       </c>
-      <c r="AB45" s="182"/>
-      <c r="AC45" s="185"/>
-      <c r="AD45" s="185"/>
-      <c r="AE45" s="186"/>
-      <c r="AF45" s="175"/>
-      <c r="AG45" s="176"/>
-      <c r="AH45" s="176"/>
+      <c r="AB45" s="175"/>
+      <c r="AC45" s="178"/>
+      <c r="AD45" s="178"/>
+      <c r="AE45" s="179"/>
+      <c r="AF45" s="168"/>
+      <c r="AG45" s="169"/>
+      <c r="AH45" s="169"/>
       <c r="AI45"/>
       <c r="AJ45"/>
       <c r="AK45"/>
@@ -40836,19 +40729,19 @@
     </row>
     <row r="46" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="85" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="B46" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="172" t="s">
+      <c r="C46" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D46" s="87" t="s">
-        <v>271</v>
+      <c r="D46" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E46" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F46" s="88" t="s">
         <v>120</v>
@@ -40856,23 +40749,23 @@
       <c r="G46" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H46" s="190" t="s">
+      <c r="H46" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I46" s="173" t="s">
+      <c r="I46" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J46" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K46" s="174" t="s">
+      <c r="K46" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L46" s="175"/>
-      <c r="M46" s="176"/>
-      <c r="N46" s="177"/>
-      <c r="O46" s="175"/>
-      <c r="P46" s="173" t="s">
+      <c r="L46" s="168"/>
+      <c r="M46" s="169"/>
+      <c r="N46" s="170"/>
+      <c r="O46" s="168"/>
+      <c r="P46" s="166" t="s">
         <v>258</v>
       </c>
       <c r="Q46" s="89" t="s">
@@ -40880,30 +40773,29 @@
       </c>
       <c r="R46" s="99"/>
       <c r="S46" s="100"/>
-      <c r="T46" s="178"/>
-      <c r="U46" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-2</v>
-      </c>
-      <c r="V46" s="179">
+      <c r="T46" s="171"/>
+      <c r="U46" s="85" t="s">
+        <v>481</v>
+      </c>
+      <c r="V46" s="172">
         <v>1</v>
       </c>
-      <c r="W46" s="178"/>
+      <c r="W46" s="171"/>
       <c r="X46" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y46" s="180"/>
-      <c r="Z46" s="184"/>
-      <c r="AA46" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y46" s="173"/>
+      <c r="Z46" s="177"/>
+      <c r="AA46" s="174">
         <v>100</v>
       </c>
-      <c r="AB46" s="182"/>
-      <c r="AC46" s="185"/>
-      <c r="AD46" s="185"/>
-      <c r="AE46" s="186"/>
-      <c r="AF46" s="175"/>
-      <c r="AG46" s="176"/>
-      <c r="AH46" s="176"/>
+      <c r="AB46" s="175"/>
+      <c r="AC46" s="178"/>
+      <c r="AD46" s="178"/>
+      <c r="AE46" s="179"/>
+      <c r="AF46" s="168"/>
+      <c r="AG46" s="169"/>
+      <c r="AH46" s="169"/>
       <c r="AI46"/>
       <c r="AJ46"/>
       <c r="AK46"/>
@@ -41897,19 +41789,19 @@
     </row>
     <row r="47" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="85" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
       <c r="B47" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="172" t="s">
+      <c r="C47" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="87" t="s">
-        <v>275</v>
+      <c r="D47" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F47" s="88" t="s">
         <v>120</v>
@@ -41917,23 +41809,23 @@
       <c r="G47" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H47" s="190" t="s">
+      <c r="H47" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I47" s="173" t="s">
+      <c r="I47" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J47" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K47" s="174" t="s">
+      <c r="K47" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L47" s="175"/>
-      <c r="M47" s="176"/>
-      <c r="N47" s="177"/>
-      <c r="O47" s="175"/>
-      <c r="P47" s="173" t="s">
+      <c r="L47" s="168"/>
+      <c r="M47" s="169"/>
+      <c r="N47" s="170"/>
+      <c r="O47" s="168"/>
+      <c r="P47" s="166" t="s">
         <v>262</v>
       </c>
       <c r="Q47" s="89" t="s">
@@ -41941,30 +41833,29 @@
       </c>
       <c r="R47" s="99"/>
       <c r="S47" s="100"/>
-      <c r="T47" s="178"/>
-      <c r="U47" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-3</v>
-      </c>
-      <c r="V47" s="179">
+      <c r="T47" s="171"/>
+      <c r="U47" s="85" t="s">
+        <v>482</v>
+      </c>
+      <c r="V47" s="172">
         <v>1</v>
       </c>
-      <c r="W47" s="178"/>
+      <c r="W47" s="171"/>
       <c r="X47" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y47" s="180"/>
-      <c r="Z47" s="184"/>
-      <c r="AA47" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y47" s="173"/>
+      <c r="Z47" s="177"/>
+      <c r="AA47" s="174">
         <v>100</v>
       </c>
-      <c r="AB47" s="182"/>
-      <c r="AC47" s="185"/>
-      <c r="AD47" s="185"/>
-      <c r="AE47" s="186"/>
-      <c r="AF47" s="175"/>
-      <c r="AG47" s="176"/>
-      <c r="AH47" s="176"/>
+      <c r="AB47" s="175"/>
+      <c r="AC47" s="178"/>
+      <c r="AD47" s="178"/>
+      <c r="AE47" s="179"/>
+      <c r="AF47" s="168"/>
+      <c r="AG47" s="169"/>
+      <c r="AH47" s="169"/>
       <c r="AI47"/>
       <c r="AJ47"/>
       <c r="AK47"/>
@@ -42958,19 +42849,19 @@
     </row>
     <row r="48" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="85" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="B48" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="172" t="s">
+      <c r="C48" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="87" t="s">
-        <v>279</v>
+      <c r="D48" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E48" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F48" s="88" t="s">
         <v>120</v>
@@ -42978,23 +42869,23 @@
       <c r="G48" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H48" s="190" t="s">
+      <c r="H48" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I48" s="173" t="s">
+      <c r="I48" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J48" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K48" s="174" t="s">
+      <c r="K48" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L48" s="175"/>
-      <c r="M48" s="176"/>
-      <c r="N48" s="177"/>
-      <c r="O48" s="175"/>
-      <c r="P48" s="173" t="s">
+      <c r="L48" s="168"/>
+      <c r="M48" s="169"/>
+      <c r="N48" s="170"/>
+      <c r="O48" s="168"/>
+      <c r="P48" s="166" t="s">
         <v>266</v>
       </c>
       <c r="Q48" s="89" t="s">
@@ -43002,30 +42893,29 @@
       </c>
       <c r="R48" s="99"/>
       <c r="S48" s="100"/>
-      <c r="T48" s="178"/>
-      <c r="U48" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-4</v>
-      </c>
-      <c r="V48" s="179">
+      <c r="T48" s="171"/>
+      <c r="U48" s="85" t="s">
+        <v>483</v>
+      </c>
+      <c r="V48" s="172">
         <v>1</v>
       </c>
-      <c r="W48" s="178"/>
+      <c r="W48" s="171"/>
       <c r="X48" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y48" s="180"/>
-      <c r="Z48" s="184"/>
-      <c r="AA48" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y48" s="173"/>
+      <c r="Z48" s="177"/>
+      <c r="AA48" s="174">
         <v>100</v>
       </c>
-      <c r="AB48" s="182"/>
-      <c r="AC48" s="185"/>
-      <c r="AD48" s="185"/>
-      <c r="AE48" s="186"/>
-      <c r="AF48" s="175"/>
-      <c r="AG48" s="176"/>
-      <c r="AH48" s="176"/>
+      <c r="AB48" s="175"/>
+      <c r="AC48" s="178"/>
+      <c r="AD48" s="178"/>
+      <c r="AE48" s="179"/>
+      <c r="AF48" s="168"/>
+      <c r="AG48" s="169"/>
+      <c r="AH48" s="169"/>
       <c r="AI48"/>
       <c r="AJ48"/>
       <c r="AK48"/>
@@ -44019,19 +43909,19 @@
     </row>
     <row r="49" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="85" t="s">
-        <v>510</v>
+        <v>484</v>
       </c>
       <c r="B49" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="172" t="s">
+      <c r="C49" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D49" s="87" t="s">
-        <v>283</v>
+      <c r="D49" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E49" s="85" t="s">
-        <v>506</v>
+        <v>450</v>
       </c>
       <c r="F49" s="88" t="s">
         <v>120</v>
@@ -44039,23 +43929,23 @@
       <c r="G49" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H49" s="190" t="s">
+      <c r="H49" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I49" s="173" t="s">
+      <c r="I49" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J49" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K49" s="174" t="s">
+      <c r="K49" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L49" s="175"/>
-      <c r="M49" s="176"/>
-      <c r="N49" s="177"/>
-      <c r="O49" s="175"/>
-      <c r="P49" s="173" t="s">
+      <c r="L49" s="168"/>
+      <c r="M49" s="169"/>
+      <c r="N49" s="170"/>
+      <c r="O49" s="168"/>
+      <c r="P49" s="166" t="s">
         <v>270</v>
       </c>
       <c r="Q49" s="89" t="s">
@@ -44063,30 +43953,29 @@
       </c>
       <c r="R49" s="99"/>
       <c r="S49" s="100"/>
-      <c r="T49" s="178"/>
-      <c r="U49" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>rna-5</v>
-      </c>
-      <c r="V49" s="179">
+      <c r="T49" s="171"/>
+      <c r="U49" s="85" t="s">
+        <v>484</v>
+      </c>
+      <c r="V49" s="172">
         <v>1</v>
       </c>
-      <c r="W49" s="178"/>
+      <c r="W49" s="171"/>
       <c r="X49" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y49" s="180"/>
-      <c r="Z49" s="184"/>
-      <c r="AA49" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y49" s="173"/>
+      <c r="Z49" s="177"/>
+      <c r="AA49" s="174">
         <v>100</v>
       </c>
-      <c r="AB49" s="182"/>
-      <c r="AC49" s="185"/>
-      <c r="AD49" s="185"/>
-      <c r="AE49" s="186"/>
-      <c r="AF49" s="175"/>
-      <c r="AG49" s="176"/>
-      <c r="AH49" s="176"/>
+      <c r="AB49" s="175"/>
+      <c r="AC49" s="178"/>
+      <c r="AD49" s="178"/>
+      <c r="AE49" s="179"/>
+      <c r="AF49" s="168"/>
+      <c r="AG49" s="169"/>
+      <c r="AH49" s="169"/>
       <c r="AI49"/>
       <c r="AJ49"/>
       <c r="AK49"/>
@@ -45079,20 +44968,20 @@
       <c r="AMJ49"/>
     </row>
     <row r="50" spans="1:1024" s="107" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="106" t="s">
-        <v>511</v>
+      <c r="A50" s="85" t="s">
+        <v>485</v>
       </c>
       <c r="B50" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="172" t="s">
+      <c r="C50" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D50" s="87" t="s">
-        <v>107</v>
+      <c r="D50" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E50" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F50" s="88" t="s">
         <v>120</v>
@@ -45100,23 +44989,23 @@
       <c r="G50" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H50" s="190" t="s">
+      <c r="H50" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I50" s="173" t="s">
+      <c r="I50" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J50" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K50" s="174" t="s">
+      <c r="K50" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L50" s="175"/>
-      <c r="M50" s="176"/>
-      <c r="N50" s="177"/>
-      <c r="O50" s="175"/>
-      <c r="P50" s="173" t="s">
+      <c r="L50" s="168"/>
+      <c r="M50" s="169"/>
+      <c r="N50" s="170"/>
+      <c r="O50" s="168"/>
+      <c r="P50" s="166" t="s">
         <v>274</v>
       </c>
       <c r="Q50" s="89" t="s">
@@ -45124,46 +45013,45 @@
       </c>
       <c r="R50" s="99"/>
       <c r="S50" s="100"/>
-      <c r="T50" s="178"/>
-      <c r="U50" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-1</v>
-      </c>
-      <c r="V50" s="179">
+      <c r="T50" s="171"/>
+      <c r="U50" s="85" t="s">
+        <v>485</v>
+      </c>
+      <c r="V50" s="172">
         <v>1</v>
       </c>
-      <c r="W50" s="178"/>
+      <c r="W50" s="171"/>
       <c r="X50" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y50" s="180"/>
-      <c r="Z50" s="184"/>
-      <c r="AA50" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y50" s="173"/>
+      <c r="Z50" s="177"/>
+      <c r="AA50" s="174">
         <v>100</v>
       </c>
-      <c r="AB50" s="182"/>
-      <c r="AC50" s="185"/>
-      <c r="AD50" s="185"/>
-      <c r="AE50" s="186"/>
-      <c r="AF50" s="175"/>
-      <c r="AG50" s="176"/>
-      <c r="AH50" s="176"/>
+      <c r="AB50" s="175"/>
+      <c r="AC50" s="178"/>
+      <c r="AD50" s="178"/>
+      <c r="AE50" s="179"/>
+      <c r="AF50" s="168"/>
+      <c r="AG50" s="169"/>
+      <c r="AH50" s="169"/>
     </row>
     <row r="51" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="106" t="s">
-        <v>513</v>
+      <c r="A51" s="85" t="s">
+        <v>486</v>
       </c>
       <c r="B51" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C51" s="172" t="s">
+      <c r="C51" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D51" s="87" t="s">
-        <v>107</v>
+      <c r="D51" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E51" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F51" s="88" t="s">
         <v>120</v>
@@ -45171,23 +45059,23 @@
       <c r="G51" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H51" s="190" t="s">
+      <c r="H51" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I51" s="173" t="s">
+      <c r="I51" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J51" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K51" s="174" t="s">
+      <c r="K51" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L51" s="175"/>
-      <c r="M51" s="176"/>
-      <c r="N51" s="177"/>
-      <c r="O51" s="175"/>
-      <c r="P51" s="188" t="s">
+      <c r="L51" s="168"/>
+      <c r="M51" s="169"/>
+      <c r="N51" s="170"/>
+      <c r="O51" s="168"/>
+      <c r="P51" s="180" t="s">
         <v>278</v>
       </c>
       <c r="Q51" s="89" t="s">
@@ -45195,30 +45083,29 @@
       </c>
       <c r="R51" s="99"/>
       <c r="S51" s="100"/>
-      <c r="T51" s="178"/>
-      <c r="U51" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-2</v>
-      </c>
-      <c r="V51" s="179">
+      <c r="T51" s="171"/>
+      <c r="U51" s="85" t="s">
+        <v>486</v>
+      </c>
+      <c r="V51" s="172">
         <v>1</v>
       </c>
-      <c r="W51" s="178"/>
+      <c r="W51" s="171"/>
       <c r="X51" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y51" s="180"/>
-      <c r="Z51" s="184"/>
-      <c r="AA51" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y51" s="173"/>
+      <c r="Z51" s="177"/>
+      <c r="AA51" s="174">
         <v>100</v>
       </c>
-      <c r="AB51" s="182"/>
-      <c r="AC51" s="185"/>
-      <c r="AD51" s="185"/>
-      <c r="AE51" s="186"/>
-      <c r="AF51" s="175"/>
-      <c r="AG51" s="176"/>
-      <c r="AH51" s="176"/>
+      <c r="AB51" s="175"/>
+      <c r="AC51" s="178"/>
+      <c r="AD51" s="178"/>
+      <c r="AE51" s="179"/>
+      <c r="AF51" s="168"/>
+      <c r="AG51" s="169"/>
+      <c r="AH51" s="169"/>
       <c r="AI51"/>
       <c r="AJ51"/>
       <c r="AK51"/>
@@ -46211,20 +46098,20 @@
       <c r="AMJ51"/>
     </row>
     <row r="52" spans="1:1024" ht="25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="106" t="s">
-        <v>514</v>
+      <c r="A52" s="85" t="s">
+        <v>487</v>
       </c>
       <c r="B52" s="86" t="s">
         <v>96</v>
       </c>
-      <c r="C52" s="172" t="s">
+      <c r="C52" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="87" t="s">
-        <v>107</v>
+      <c r="D52" s="112" t="s">
+        <v>408</v>
       </c>
       <c r="E52" s="85" t="s">
-        <v>512</v>
+        <v>450</v>
       </c>
       <c r="F52" s="88" t="s">
         <v>120</v>
@@ -46232,23 +46119,23 @@
       <c r="G52" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="H52" s="190" t="s">
+      <c r="H52" s="182" t="s">
         <v>144</v>
       </c>
-      <c r="I52" s="173" t="s">
+      <c r="I52" s="166" t="s">
         <v>131</v>
       </c>
       <c r="J52" s="86" t="s">
         <v>110</v>
       </c>
-      <c r="K52" s="174" t="s">
+      <c r="K52" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="L52" s="175"/>
-      <c r="M52" s="176"/>
-      <c r="N52" s="177"/>
-      <c r="O52" s="175"/>
-      <c r="P52" s="191" t="s">
+      <c r="L52" s="168"/>
+      <c r="M52" s="169"/>
+      <c r="N52" s="170"/>
+      <c r="O52" s="168"/>
+      <c r="P52" s="183" t="s">
         <v>282</v>
       </c>
       <c r="Q52" s="89" t="s">
@@ -46256,30 +46143,29 @@
       </c>
       <c r="R52" s="99"/>
       <c r="S52" s="100"/>
-      <c r="T52" s="178"/>
-      <c r="U52" s="187" t="str">
-        <f t="shared" si="0"/>
-        <v>gene-list-test-3</v>
-      </c>
-      <c r="V52" s="179">
+      <c r="T52" s="171"/>
+      <c r="U52" s="85" t="s">
+        <v>487</v>
+      </c>
+      <c r="V52" s="172">
         <v>1</v>
       </c>
-      <c r="W52" s="178"/>
+      <c r="W52" s="171"/>
       <c r="X52" s="112" t="s">
-        <v>450</v>
-      </c>
-      <c r="Y52" s="180"/>
-      <c r="Z52" s="184"/>
-      <c r="AA52" s="181">
+        <v>445</v>
+      </c>
+      <c r="Y52" s="173"/>
+      <c r="Z52" s="177"/>
+      <c r="AA52" s="174">
         <v>100</v>
       </c>
-      <c r="AB52" s="182"/>
-      <c r="AC52" s="185"/>
-      <c r="AD52" s="185"/>
-      <c r="AE52" s="186"/>
-      <c r="AF52" s="175"/>
-      <c r="AG52" s="176"/>
-      <c r="AH52" s="176"/>
+      <c r="AB52" s="175"/>
+      <c r="AC52" s="178"/>
+      <c r="AD52" s="178"/>
+      <c r="AE52" s="179"/>
+      <c r="AF52" s="168"/>
+      <c r="AG52" s="169"/>
+      <c r="AH52" s="169"/>
       <c r="AI52"/>
       <c r="AJ52"/>
       <c r="AK52"/>
@@ -69502,6 +69388,7 @@
     <mergeCell ref="U9:V9"/>
     <mergeCell ref="Z9:AA9"/>
   </mergeCells>
+  <phoneticPr fontId="48" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L53:L394" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
@@ -69523,7 +69410,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="20">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -69624,25 +69511,7 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>C15:C52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{428E6055-04A8-6C4C-89A7-EF7F7D8D6474}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>V15:V52 N15:N17 AE17</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AF8CDC01-B85F-E14A-8E02-465A52BD9AAC}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>AE18:AE52</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22E74F9B-E324-7B45-A9DA-64F55B2673AF}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>N18:N52</xm:sqref>
+          <xm:sqref>C15:C52 V15:V52 N15:N52 AE17:AE52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -69658,7 +69527,7 @@
   <dimension ref="A1:AL103"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C37" sqref="C37:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>